<commit_message>
basically done -- will add some validation and comments
</commit_message>
<xml_diff>
--- a/pythonCW/230023476PortfolioProblem.xlsx
+++ b/pythonCW/230023476PortfolioProblem.xlsx
@@ -26427,8 +26427,8 @@
     <col width="14.4" customWidth="1" min="2" max="2"/>
     <col width="10.8" customWidth="1" min="3" max="3"/>
     <col width="16.8" customWidth="1" min="4" max="4"/>
-    <col width="4.8" customWidth="1" min="5" max="5"/>
-    <col width="4.8" customWidth="1" min="6" max="6"/>
+    <col width="8.4" customWidth="1" min="5" max="5"/>
+    <col width="7.199999999999999" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -26454,2013 +26454,2013 @@
       </c>
       <c r="E1" s="3" t="inlineStr">
         <is>
-          <t>w1</t>
+          <t>w_USA</t>
         </is>
       </c>
       <c r="F1" s="3" t="inlineStr">
         <is>
-          <t>w2</t>
+          <t>w_UK</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.1601</v>
+        <v>0.104</v>
       </c>
       <c r="B2" t="n">
-        <v>0.2118</v>
+        <v>0.1545</v>
       </c>
       <c r="C2" t="n">
-        <v>0.09279999999999999</v>
+        <v>0.0682</v>
       </c>
       <c r="D2" t="n">
-        <v>0.6613</v>
+        <v>0.3819</v>
       </c>
       <c r="E2" t="n">
-        <v>0.0721</v>
+        <v>0.9849</v>
       </c>
       <c r="F2" t="n">
-        <v>0.9278999999999999</v>
+        <v>0.0151</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0.1601</v>
+        <v>0.104</v>
       </c>
       <c r="B3" t="n">
-        <v>0.2118</v>
+        <v>0.1545</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0929</v>
+        <v>0.0682</v>
       </c>
       <c r="D3" t="n">
-        <v>0.6617</v>
+        <v>0.3821</v>
       </c>
       <c r="E3" t="n">
-        <v>0.073</v>
+        <v>0.9855</v>
       </c>
       <c r="F3" t="n">
-        <v>0.927</v>
+        <v>0.0145</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0.1603</v>
+        <v>0.1042</v>
       </c>
       <c r="B4" t="n">
-        <v>0.2114</v>
+        <v>0.1545</v>
       </c>
       <c r="C4" t="n">
-        <v>0.09320000000000001</v>
+        <v>0.0684</v>
       </c>
       <c r="D4" t="n">
-        <v>0.6634</v>
+        <v>0.383</v>
       </c>
       <c r="E4" t="n">
-        <v>0.0769</v>
+        <v>0.9882</v>
       </c>
       <c r="F4" t="n">
-        <v>0.9231</v>
+        <v>0.0118</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0.1603</v>
+        <v>0.1043</v>
       </c>
       <c r="B5" t="n">
-        <v>0.2112</v>
+        <v>0.1545</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0934</v>
+        <v>0.06850000000000001</v>
       </c>
       <c r="D5" t="n">
-        <v>0.6645</v>
+        <v>0.3836</v>
       </c>
       <c r="E5" t="n">
-        <v>0.0793</v>
+        <v>0.9901</v>
       </c>
       <c r="F5" t="n">
-        <v>0.9207</v>
+        <v>0.009900000000000001</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0.1606</v>
+        <v>0.1045</v>
       </c>
       <c r="B6" t="n">
-        <v>0.2106</v>
+        <v>0.1545</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0941</v>
+        <v>0.0687</v>
       </c>
       <c r="D6" t="n">
-        <v>0.6677999999999999</v>
+        <v>0.3854</v>
       </c>
       <c r="E6" t="n">
-        <v>0.0872</v>
+        <v>0.9954</v>
       </c>
       <c r="F6" t="n">
-        <v>0.9127999999999999</v>
+        <v>0.0046</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0.1608</v>
+        <v>0.1047</v>
       </c>
       <c r="B7" t="n">
-        <v>0.2103</v>
+        <v>0.1544</v>
       </c>
       <c r="C7" t="n">
-        <v>0.0945</v>
+        <v>0.0689</v>
       </c>
       <c r="D7" t="n">
-        <v>0.6695</v>
+        <v>0.3865</v>
       </c>
       <c r="E7" t="n">
-        <v>0.09130000000000001</v>
+        <v>0.9985000000000001</v>
       </c>
       <c r="F7" t="n">
-        <v>0.9087</v>
+        <v>0.0015</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>0.1612</v>
+        <v>0.1051</v>
       </c>
       <c r="B8" t="n">
-        <v>0.2094</v>
+        <v>0.1544</v>
       </c>
       <c r="C8" t="n">
-        <v>0.0954</v>
+        <v>0.0693</v>
       </c>
       <c r="D8" t="n">
-        <v>0.6744</v>
+        <v>0.3892</v>
       </c>
       <c r="E8" t="n">
-        <v>0.1031</v>
+        <v>1.0066</v>
       </c>
       <c r="F8" t="n">
-        <v>0.8969</v>
+        <v>-0.0066</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0.1614</v>
+        <v>0.1053</v>
       </c>
       <c r="B9" t="n">
-        <v>0.209</v>
+        <v>0.1544</v>
       </c>
       <c r="C9" t="n">
-        <v>0.0959</v>
+        <v>0.0696</v>
       </c>
       <c r="D9" t="n">
-        <v>0.6767</v>
+        <v>0.3907</v>
       </c>
       <c r="E9" t="n">
-        <v>0.1088</v>
+        <v>1.011</v>
       </c>
       <c r="F9" t="n">
-        <v>0.8912</v>
+        <v>-0.011</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>0.162</v>
+        <v>0.1059</v>
       </c>
       <c r="B10" t="n">
-        <v>0.2079</v>
+        <v>0.1544</v>
       </c>
       <c r="C10" t="n">
-        <v>0.09710000000000001</v>
+        <v>0.0701</v>
       </c>
       <c r="D10" t="n">
-        <v>0.6828</v>
+        <v>0.3942</v>
       </c>
       <c r="E10" t="n">
-        <v>0.1246</v>
+        <v>1.0217</v>
       </c>
       <c r="F10" t="n">
-        <v>0.8754</v>
+        <v>-0.0217</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>0.1622</v>
+        <v>0.1062</v>
       </c>
       <c r="B11" t="n">
-        <v>0.2075</v>
+        <v>0.1544</v>
       </c>
       <c r="C11" t="n">
-        <v>0.0977</v>
+        <v>0.0704</v>
       </c>
       <c r="D11" t="n">
-        <v>0.6856</v>
+        <v>0.3961</v>
       </c>
       <c r="E11" t="n">
-        <v>0.1319</v>
+        <v>1.0273</v>
       </c>
       <c r="F11" t="n">
-        <v>0.8681</v>
+        <v>-0.0273</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>0.1629</v>
+        <v>0.1068</v>
       </c>
       <c r="B12" t="n">
-        <v>0.2064</v>
+        <v>0.1544</v>
       </c>
       <c r="C12" t="n">
-        <v>0.09909999999999999</v>
+        <v>0.0711</v>
       </c>
       <c r="D12" t="n">
-        <v>0.6926</v>
+        <v>0.4006</v>
       </c>
       <c r="E12" t="n">
-        <v>0.1516</v>
+        <v>1.0407</v>
       </c>
       <c r="F12" t="n">
-        <v>0.8484</v>
+        <v>-0.0407</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>0.1633</v>
+        <v>0.1072</v>
       </c>
       <c r="B13" t="n">
-        <v>0.2059</v>
+        <v>0.1544</v>
       </c>
       <c r="C13" t="n">
-        <v>0.0997</v>
+        <v>0.07140000000000001</v>
       </c>
       <c r="D13" t="n">
-        <v>0.6957</v>
+        <v>0.4028</v>
       </c>
       <c r="E13" t="n">
-        <v>0.1606</v>
+        <v>1.0475</v>
       </c>
       <c r="F13" t="n">
-        <v>0.8394</v>
+        <v>-0.0475</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>0.1641</v>
+        <v>0.1084</v>
       </c>
       <c r="B14" t="n">
-        <v>0.2049</v>
+        <v>0.1544</v>
       </c>
       <c r="C14" t="n">
-        <v>0.1011</v>
+        <v>0.0727</v>
       </c>
       <c r="D14" t="n">
-        <v>0.7033</v>
+        <v>0.4107</v>
       </c>
       <c r="E14" t="n">
-        <v>0.1842</v>
+        <v>1.0717</v>
       </c>
       <c r="F14" t="n">
-        <v>0.8158</v>
+        <v>-0.0717</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>0.1645</v>
+        <v>0.1099</v>
       </c>
       <c r="B15" t="n">
-        <v>0.2045</v>
+        <v>0.1545</v>
       </c>
       <c r="C15" t="n">
-        <v>0.1017</v>
+        <v>0.074</v>
       </c>
       <c r="D15" t="n">
-        <v>0.7064</v>
+        <v>0.4197</v>
       </c>
       <c r="E15" t="n">
-        <v>0.1949</v>
+        <v>1.0999</v>
       </c>
       <c r="F15" t="n">
-        <v>0.8051</v>
+        <v>-0.0999</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>0.1655</v>
+        <v>0.1115</v>
       </c>
       <c r="B16" t="n">
-        <v>0.2038</v>
+        <v>0.1547</v>
       </c>
       <c r="C16" t="n">
-        <v>0.1032</v>
+        <v>0.0756</v>
       </c>
       <c r="D16" t="n">
-        <v>0.7138</v>
+        <v>0.4298</v>
       </c>
       <c r="E16" t="n">
-        <v>0.2224</v>
+        <v>1.1319</v>
       </c>
       <c r="F16" t="n">
-        <v>0.7776</v>
+        <v>-0.1319</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>0.1659</v>
+        <v>0.1133</v>
       </c>
       <c r="B17" t="n">
-        <v>0.2036</v>
+        <v>0.1549</v>
       </c>
       <c r="C17" t="n">
-        <v>0.1037</v>
+        <v>0.07729999999999999</v>
       </c>
       <c r="D17" t="n">
-        <v>0.7167</v>
+        <v>0.4409</v>
       </c>
       <c r="E17" t="n">
-        <v>0.2347</v>
+        <v>1.1679</v>
       </c>
       <c r="F17" t="n">
-        <v>0.7653</v>
+        <v>-0.1679</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>0.1671</v>
+        <v>0.1153</v>
       </c>
       <c r="B18" t="n">
-        <v>0.2034</v>
+        <v>0.1553</v>
       </c>
       <c r="C18" t="n">
-        <v>0.105</v>
+        <v>0.07920000000000001</v>
       </c>
       <c r="D18" t="n">
-        <v>0.723</v>
+        <v>0.4529</v>
       </c>
       <c r="E18" t="n">
-        <v>0.2661</v>
+        <v>1.2078</v>
       </c>
       <c r="F18" t="n">
-        <v>0.7339</v>
+        <v>-0.2078</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>0.1676</v>
+        <v>0.1176</v>
       </c>
       <c r="B19" t="n">
-        <v>0.2034</v>
+        <v>0.1559</v>
       </c>
       <c r="C19" t="n">
-        <v>0.1055</v>
+        <v>0.08110000000000001</v>
       </c>
       <c r="D19" t="n">
-        <v>0.7252999999999999</v>
+        <v>0.4656</v>
       </c>
       <c r="E19" t="n">
-        <v>0.2801</v>
+        <v>1.2516</v>
       </c>
       <c r="F19" t="n">
-        <v>0.7199</v>
+        <v>-0.2516</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>0.1694</v>
+        <v>0.12</v>
       </c>
       <c r="B20" t="n">
-        <v>0.2044</v>
+        <v>0.1566</v>
       </c>
       <c r="C20" t="n">
-        <v>0.1067</v>
+        <v>0.0832</v>
       </c>
       <c r="D20" t="n">
-        <v>0.731</v>
+        <v>0.4789</v>
       </c>
       <c r="E20" t="n">
-        <v>0.331</v>
+        <v>1.2994</v>
       </c>
       <c r="F20" t="n">
-        <v>0.669</v>
+        <v>-0.2994</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>0.1714</v>
+        <v>0.1226</v>
       </c>
       <c r="B21" t="n">
-        <v>0.2067</v>
+        <v>0.1576</v>
       </c>
       <c r="C21" t="n">
-        <v>0.1073</v>
+        <v>0.0854</v>
       </c>
       <c r="D21" t="n">
-        <v>0.7324000000000001</v>
+        <v>0.4927</v>
       </c>
       <c r="E21" t="n">
-        <v>0.3876</v>
+        <v>1.3511</v>
       </c>
       <c r="F21" t="n">
-        <v>0.6124000000000001</v>
+        <v>-0.3511</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>0.1736</v>
+        <v>0.1255</v>
       </c>
       <c r="B22" t="n">
-        <v>0.211</v>
+        <v>0.1588</v>
       </c>
       <c r="C22" t="n">
-        <v>0.1069</v>
+        <v>0.0876</v>
       </c>
       <c r="D22" t="n">
-        <v>0.7282999999999999</v>
+        <v>0.5067</v>
       </c>
       <c r="E22" t="n">
-        <v>0.4497</v>
+        <v>1.4067</v>
       </c>
       <c r="F22" t="n">
-        <v>0.5503</v>
+        <v>-0.4067</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>0.1761</v>
+        <v>0.1285</v>
       </c>
       <c r="B23" t="n">
-        <v>0.2174</v>
+        <v>0.1604</v>
       </c>
       <c r="C23" t="n">
-        <v>0.1052</v>
+        <v>0.08989999999999999</v>
       </c>
       <c r="D23" t="n">
-        <v>0.7181</v>
+        <v>0.5207000000000001</v>
       </c>
       <c r="E23" t="n">
-        <v>0.5173</v>
+        <v>1.4662</v>
       </c>
       <c r="F23" t="n">
-        <v>0.4827</v>
+        <v>-0.4662</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>0.1787</v>
+        <v>0.1317</v>
       </c>
       <c r="B24" t="n">
-        <v>0.2262</v>
+        <v>0.1622</v>
       </c>
       <c r="C24" t="n">
-        <v>0.1019</v>
+        <v>0.09229999999999999</v>
       </c>
       <c r="D24" t="n">
-        <v>0.7016</v>
+        <v>0.5347</v>
       </c>
       <c r="E24" t="n">
-        <v>0.5906</v>
+        <v>1.5297</v>
       </c>
       <c r="F24" t="n">
-        <v>0.4094</v>
+        <v>-0.5296999999999999</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>0.1815</v>
+        <v>0.1352</v>
       </c>
       <c r="B25" t="n">
-        <v>0.2377</v>
+        <v>0.1645</v>
       </c>
       <c r="C25" t="n">
-        <v>0.0968</v>
+        <v>0.0946</v>
       </c>
       <c r="D25" t="n">
-        <v>0.6795</v>
+        <v>0.5482</v>
       </c>
       <c r="E25" t="n">
-        <v>0.6694</v>
+        <v>1.5971</v>
       </c>
       <c r="F25" t="n">
-        <v>0.3306</v>
+        <v>-0.5971</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>0.1846</v>
+        <v>0.1388</v>
       </c>
       <c r="B26" t="n">
-        <v>0.252</v>
+        <v>0.1671</v>
       </c>
       <c r="C26" t="n">
-        <v>0.0893</v>
+        <v>0.0969</v>
       </c>
       <c r="D26" t="n">
-        <v>0.653</v>
+        <v>0.5613</v>
       </c>
       <c r="E26" t="n">
-        <v>0.7538</v>
+        <v>1.6685</v>
       </c>
       <c r="F26" t="n">
-        <v>0.2462</v>
+        <v>-0.6685</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>0.1878</v>
+        <v>0.1426</v>
       </c>
       <c r="B27" t="n">
-        <v>0.2691</v>
+        <v>0.1702</v>
       </c>
       <c r="C27" t="n">
-        <v>0.0791</v>
+        <v>0.0992</v>
       </c>
       <c r="D27" t="n">
-        <v>0.6235000000000001</v>
+        <v>0.5736</v>
       </c>
       <c r="E27" t="n">
-        <v>0.8437</v>
+        <v>1.7437</v>
       </c>
       <c r="F27" t="n">
-        <v>0.1563</v>
+        <v>-0.7437</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>0.1912</v>
+        <v>0.1467</v>
       </c>
       <c r="B28" t="n">
-        <v>0.2891</v>
+        <v>0.1737</v>
       </c>
       <c r="C28" t="n">
-        <v>0.0659</v>
+        <v>0.1014</v>
       </c>
       <c r="D28" t="n">
-        <v>0.5923</v>
+        <v>0.5851</v>
       </c>
       <c r="E28" t="n">
-        <v>0.9393</v>
+        <v>1.8229</v>
       </c>
       <c r="F28" t="n">
-        <v>0.0607</v>
+        <v>-0.8229</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>0.1948</v>
+        <v>0.1509</v>
       </c>
       <c r="B29" t="n">
-        <v>0.3117</v>
+        <v>0.1778</v>
       </c>
       <c r="C29" t="n">
-        <v>0.0491</v>
+        <v>0.1035</v>
       </c>
       <c r="D29" t="n">
-        <v>0.5609</v>
+        <v>0.5956</v>
       </c>
       <c r="E29" t="n">
-        <v>1.0404</v>
+        <v>1.906</v>
       </c>
       <c r="F29" t="n">
-        <v>-0.0404</v>
+        <v>-0.906</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>0.1987</v>
+        <v>0.1553</v>
       </c>
       <c r="B30" t="n">
-        <v>0.3371</v>
+        <v>0.1824</v>
       </c>
       <c r="C30" t="n">
-        <v>0.0283</v>
+        <v>0.1054</v>
       </c>
       <c r="D30" t="n">
-        <v>0.5301</v>
+        <v>0.605</v>
       </c>
       <c r="E30" t="n">
-        <v>1.147</v>
+        <v>1.9931</v>
       </c>
       <c r="F30" t="n">
-        <v>-0.147</v>
+        <v>-0.9931</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>0.2027</v>
+        <v>0.16</v>
       </c>
       <c r="B31" t="n">
-        <v>0.365</v>
+        <v>0.1874</v>
       </c>
       <c r="C31" t="n">
-        <v>0.0029</v>
+        <v>0.1073</v>
       </c>
       <c r="D31" t="n">
-        <v>0.5006</v>
+        <v>0.6133</v>
       </c>
       <c r="E31" t="n">
-        <v>1.2593</v>
+        <v>2.084</v>
       </c>
       <c r="F31" t="n">
-        <v>-0.2593</v>
+        <v>-1.084</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>0.2069</v>
+        <v>0.1648</v>
       </c>
       <c r="B32" t="n">
-        <v>0.3953</v>
+        <v>0.1931</v>
       </c>
       <c r="C32" t="n">
-        <v>-0.0275</v>
+        <v>0.1089</v>
       </c>
       <c r="D32" t="n">
-        <v>0.4729</v>
+        <v>0.6204</v>
       </c>
       <c r="E32" t="n">
-        <v>1.3771</v>
+        <v>2.1789</v>
       </c>
       <c r="F32" t="n">
-        <v>-0.3771</v>
+        <v>-1.1789</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>0.2114</v>
+        <v>0.1698</v>
       </c>
       <c r="B33" t="n">
-        <v>0.428</v>
+        <v>0.1993</v>
       </c>
       <c r="C33" t="n">
-        <v>-0.0634</v>
+        <v>0.1102</v>
       </c>
       <c r="D33" t="n">
-        <v>0.4471</v>
+        <v>0.6263</v>
       </c>
       <c r="E33" t="n">
-        <v>1.5005</v>
+        <v>2.2778</v>
       </c>
       <c r="F33" t="n">
-        <v>-0.5004999999999999</v>
+        <v>-1.2778</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>0.216</v>
+        <v>0.1751</v>
       </c>
       <c r="B34" t="n">
-        <v>0.463</v>
+        <v>0.2061</v>
       </c>
       <c r="C34" t="n">
-        <v>-0.1056</v>
+        <v>0.1113</v>
       </c>
       <c r="D34" t="n">
-        <v>0.4233</v>
+        <v>0.631</v>
       </c>
       <c r="E34" t="n">
-        <v>1.6294</v>
+        <v>2.3805</v>
       </c>
       <c r="F34" t="n">
-        <v>-0.6294</v>
+        <v>-1.3805</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>0.2208</v>
+        <v>0.1805</v>
       </c>
       <c r="B35" t="n">
-        <v>0.5002</v>
+        <v>0.2134</v>
       </c>
       <c r="C35" t="n">
-        <v>-0.1545</v>
+        <v>0.1121</v>
       </c>
       <c r="D35" t="n">
-        <v>0.4015</v>
+        <v>0.6347</v>
       </c>
       <c r="E35" t="n">
-        <v>1.764</v>
+        <v>2.4872</v>
       </c>
       <c r="F35" t="n">
-        <v>-0.764</v>
+        <v>-1.4872</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>0.2259</v>
+        <v>0.1861</v>
       </c>
       <c r="B36" t="n">
-        <v>0.5396</v>
+        <v>0.2214</v>
       </c>
       <c r="C36" t="n">
-        <v>-0.2108</v>
+        <v>0.1126</v>
       </c>
       <c r="D36" t="n">
-        <v>0.3815</v>
+        <v>0.6374</v>
       </c>
       <c r="E36" t="n">
-        <v>1.9041</v>
+        <v>2.5978</v>
       </c>
       <c r="F36" t="n">
-        <v>-0.9041</v>
+        <v>-1.5978</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>0.2311</v>
+        <v>0.1919</v>
       </c>
       <c r="B37" t="n">
-        <v>0.581</v>
+        <v>0.2299</v>
       </c>
       <c r="C37" t="n">
-        <v>-0.2752</v>
+        <v>0.1127</v>
       </c>
       <c r="D37" t="n">
-        <v>0.3633</v>
+        <v>0.6392</v>
       </c>
       <c r="E37" t="n">
-        <v>2.0497</v>
+        <v>2.7124</v>
       </c>
       <c r="F37" t="n">
-        <v>-1.0497</v>
+        <v>-1.7124</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>0.2365</v>
+        <v>0.198</v>
       </c>
       <c r="B38" t="n">
-        <v>0.6244</v>
+        <v>0.239</v>
       </c>
       <c r="C38" t="n">
-        <v>-0.3483</v>
+        <v>0.1123</v>
       </c>
       <c r="D38" t="n">
-        <v>0.3468</v>
+        <v>0.6402</v>
       </c>
       <c r="E38" t="n">
-        <v>2.201</v>
+        <v>2.8309</v>
       </c>
       <c r="F38" t="n">
-        <v>-1.201</v>
+        <v>-1.8309</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>0.2421</v>
+        <v>0.2042</v>
       </c>
       <c r="B39" t="n">
-        <v>0.6698</v>
+        <v>0.2486</v>
       </c>
       <c r="C39" t="n">
-        <v>-0.4308</v>
+        <v>0.1115</v>
       </c>
       <c r="D39" t="n">
-        <v>0.3316</v>
+        <v>0.6404</v>
       </c>
       <c r="E39" t="n">
-        <v>2.3578</v>
+        <v>2.9533</v>
       </c>
       <c r="F39" t="n">
-        <v>-1.3578</v>
+        <v>-1.9533</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>0.248</v>
+        <v>0.2106</v>
       </c>
       <c r="B40" t="n">
-        <v>0.7171999999999999</v>
+        <v>0.2588</v>
       </c>
       <c r="C40" t="n">
-        <v>-0.5235</v>
+        <v>0.1102</v>
       </c>
       <c r="D40" t="n">
-        <v>0.3179</v>
+        <v>0.64</v>
       </c>
       <c r="E40" t="n">
-        <v>2.5201</v>
+        <v>3.0796</v>
       </c>
       <c r="F40" t="n">
-        <v>-1.5201</v>
+        <v>-2.0796</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>0.254</v>
+        <v>0.2173</v>
       </c>
       <c r="B41" t="n">
-        <v>0.7665</v>
+        <v>0.2696</v>
       </c>
       <c r="C41" t="n">
-        <v>-0.6272</v>
+        <v>0.1082</v>
       </c>
       <c r="D41" t="n">
-        <v>0.3053</v>
+        <v>0.639</v>
       </c>
       <c r="E41" t="n">
-        <v>2.6881</v>
+        <v>3.2099</v>
       </c>
       <c r="F41" t="n">
-        <v>-1.6881</v>
+        <v>-2.2099</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>0.2602</v>
+        <v>0.2241</v>
       </c>
       <c r="B42" t="n">
-        <v>0.8176</v>
+        <v>0.2809</v>
       </c>
       <c r="C42" t="n">
-        <v>-0.7425</v>
+        <v>0.1057</v>
       </c>
       <c r="D42" t="n">
-        <v>0.2938</v>
+        <v>0.6375999999999999</v>
       </c>
       <c r="E42" t="n">
-        <v>2.8616</v>
+        <v>3.344</v>
       </c>
       <c r="F42" t="n">
-        <v>-1.8616</v>
+        <v>-2.344</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>0.2667</v>
+        <v>0.2311</v>
       </c>
       <c r="B43" t="n">
-        <v>0.8707</v>
+        <v>0.2928</v>
       </c>
       <c r="C43" t="n">
-        <v>-0.8704</v>
+        <v>0.1026</v>
       </c>
       <c r="D43" t="n">
-        <v>0.2833</v>
+        <v>0.6358</v>
       </c>
       <c r="E43" t="n">
-        <v>3.0407</v>
+        <v>3.4822</v>
       </c>
       <c r="F43" t="n">
-        <v>-2.0407</v>
+        <v>-2.4822</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>0.2733</v>
+        <v>0.2384</v>
       </c>
       <c r="B44" t="n">
-        <v>0.9255</v>
+        <v>0.3052</v>
       </c>
       <c r="C44" t="n">
-        <v>-1.0116</v>
+        <v>0.0987</v>
       </c>
       <c r="D44" t="n">
-        <v>0.2737</v>
+        <v>0.6336000000000001</v>
       </c>
       <c r="E44" t="n">
-        <v>3.2254</v>
+        <v>3.6242</v>
       </c>
       <c r="F44" t="n">
-        <v>-2.2254</v>
+        <v>-2.6242</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>0.2801</v>
+        <v>0.2458</v>
       </c>
       <c r="B45" t="n">
-        <v>0.9822</v>
+        <v>0.3181</v>
       </c>
       <c r="C45" t="n">
-        <v>-1.1671</v>
+        <v>0.094</v>
       </c>
       <c r="D45" t="n">
-        <v>0.2648</v>
+        <v>0.6313</v>
       </c>
       <c r="E45" t="n">
-        <v>3.4156</v>
+        <v>3.7702</v>
       </c>
       <c r="F45" t="n">
-        <v>-2.4156</v>
+        <v>-2.7702</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>0.2872</v>
+        <v>0.2534</v>
       </c>
       <c r="B46" t="n">
-        <v>1.0408</v>
+        <v>0.3315</v>
       </c>
       <c r="C46" t="n">
-        <v>-1.3376</v>
+        <v>0.0886</v>
       </c>
       <c r="D46" t="n">
-        <v>0.2567</v>
+        <v>0.6287</v>
       </c>
       <c r="E46" t="n">
-        <v>3.6114</v>
+        <v>3.9201</v>
       </c>
       <c r="F46" t="n">
-        <v>-2.6114</v>
+        <v>-2.9201</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>0.2944</v>
+        <v>0.2613</v>
       </c>
       <c r="B47" t="n">
-        <v>1.1011</v>
+        <v>0.3455</v>
       </c>
       <c r="C47" t="n">
-        <v>-1.5242</v>
+        <v>0.0822</v>
       </c>
       <c r="D47" t="n">
-        <v>0.2492</v>
+        <v>0.626</v>
       </c>
       <c r="E47" t="n">
-        <v>3.8128</v>
+        <v>4.0739</v>
       </c>
       <c r="F47" t="n">
-        <v>-2.8128</v>
+        <v>-3.0739</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>0.3018</v>
+        <v>0.2693</v>
       </c>
       <c r="B48" t="n">
-        <v>1.1632</v>
+        <v>0.3599</v>
       </c>
       <c r="C48" t="n">
-        <v>-1.7277</v>
+        <v>0.075</v>
       </c>
       <c r="D48" t="n">
-        <v>0.2423</v>
+        <v>0.6232</v>
       </c>
       <c r="E48" t="n">
-        <v>4.0198</v>
+        <v>4.2317</v>
       </c>
       <c r="F48" t="n">
-        <v>-3.0198</v>
+        <v>-3.2317</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>0.3094</v>
+        <v>0.2775</v>
       </c>
       <c r="B49" t="n">
-        <v>1.2271</v>
+        <v>0.3749</v>
       </c>
       <c r="C49" t="n">
-        <v>-1.9492</v>
+        <v>0.0667</v>
       </c>
       <c r="D49" t="n">
-        <v>0.2359</v>
+        <v>0.6203</v>
       </c>
       <c r="E49" t="n">
-        <v>4.2323</v>
+        <v>4.3934</v>
       </c>
       <c r="F49" t="n">
-        <v>-3.2323</v>
+        <v>-3.3934</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>0.3173</v>
+        <v>0.286</v>
       </c>
       <c r="B50" t="n">
-        <v>1.2928</v>
+        <v>0.3903</v>
       </c>
       <c r="C50" t="n">
-        <v>-2.1896</v>
+        <v>0.0574</v>
       </c>
       <c r="D50" t="n">
-        <v>0.2299</v>
+        <v>0.6173</v>
       </c>
       <c r="E50" t="n">
-        <v>4.4504</v>
+        <v>4.559</v>
       </c>
       <c r="F50" t="n">
-        <v>-3.4504</v>
+        <v>-3.559</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>0.3253</v>
+        <v>0.2946</v>
       </c>
       <c r="B51" t="n">
-        <v>1.3602</v>
+        <v>0.4062</v>
       </c>
       <c r="C51" t="n">
-        <v>-2.4499</v>
+        <v>0.047</v>
       </c>
       <c r="D51" t="n">
-        <v>0.2245</v>
+        <v>0.6143999999999999</v>
       </c>
       <c r="E51" t="n">
-        <v>4.674</v>
+        <v>4.7285</v>
       </c>
       <c r="F51" t="n">
-        <v>-3.674</v>
+        <v>-3.7285</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>0.3335</v>
+        <v>0.3034</v>
       </c>
       <c r="B52" t="n">
-        <v>1.4294</v>
+        <v>0.4226</v>
       </c>
       <c r="C52" t="n">
-        <v>-2.7312</v>
+        <v>0.0355</v>
       </c>
       <c r="D52" t="n">
-        <v>0.2193</v>
+        <v>0.6114000000000001</v>
       </c>
       <c r="E52" t="n">
-        <v>4.9033</v>
+        <v>4.902</v>
       </c>
       <c r="F52" t="n">
-        <v>-3.9033</v>
+        <v>-3.902</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>0.342</v>
+        <v>0.3125</v>
       </c>
       <c r="B53" t="n">
-        <v>1.5003</v>
+        <v>0.4395</v>
       </c>
       <c r="C53" t="n">
-        <v>-3.0346</v>
+        <v>0.0227</v>
       </c>
       <c r="D53" t="n">
-        <v>0.2146</v>
+        <v>0.6085</v>
       </c>
       <c r="E53" t="n">
-        <v>5.1381</v>
+        <v>5.0794</v>
       </c>
       <c r="F53" t="n">
-        <v>-4.1381</v>
+        <v>-4.0794</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>0.3506</v>
+        <v>0.3217</v>
       </c>
       <c r="B54" t="n">
-        <v>1.573</v>
+        <v>0.4569</v>
       </c>
       <c r="C54" t="n">
-        <v>-3.3611</v>
+        <v>0.0086</v>
       </c>
       <c r="D54" t="n">
-        <v>0.2102</v>
+        <v>0.6056</v>
       </c>
       <c r="E54" t="n">
-        <v>5.3784</v>
+        <v>5.2607</v>
       </c>
       <c r="F54" t="n">
-        <v>-4.3784</v>
+        <v>-4.2607</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>0.3594</v>
+        <v>0.3311</v>
       </c>
       <c r="B55" t="n">
-        <v>1.6475</v>
+        <v>0.4747</v>
       </c>
       <c r="C55" t="n">
-        <v>-3.7119</v>
+        <v>-0.0068</v>
       </c>
       <c r="D55" t="n">
-        <v>0.206</v>
+        <v>0.6028</v>
       </c>
       <c r="E55" t="n">
-        <v>5.6244</v>
+        <v>5.446</v>
       </c>
       <c r="F55" t="n">
-        <v>-4.6244</v>
+        <v>-4.446</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>0.3684</v>
+        <v>0.3407</v>
       </c>
       <c r="B56" t="n">
-        <v>1.7237</v>
+        <v>0.4929</v>
       </c>
       <c r="C56" t="n">
-        <v>-4.0881</v>
+        <v>-0.0237</v>
       </c>
       <c r="D56" t="n">
-        <v>0.2022</v>
+        <v>0.6</v>
       </c>
       <c r="E56" t="n">
-        <v>5.8759</v>
+        <v>5.6352</v>
       </c>
       <c r="F56" t="n">
-        <v>-4.8759</v>
+        <v>-4.6352</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>0.3777</v>
+        <v>0.3506</v>
       </c>
       <c r="B57" t="n">
-        <v>1.8016</v>
+        <v>0.5117</v>
       </c>
       <c r="C57" t="n">
-        <v>-4.4908</v>
+        <v>-0.0421</v>
       </c>
       <c r="D57" t="n">
-        <v>0.1985</v>
+        <v>0.5972</v>
       </c>
       <c r="E57" t="n">
-        <v>6.133</v>
+        <v>5.8283</v>
       </c>
       <c r="F57" t="n">
-        <v>-5.133</v>
+        <v>-4.8283</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>0.3871</v>
+        <v>0.3606</v>
       </c>
       <c r="B58" t="n">
-        <v>1.8812</v>
+        <v>0.5308</v>
       </c>
       <c r="C58" t="n">
-        <v>-4.9214</v>
+        <v>-0.0621</v>
       </c>
       <c r="D58" t="n">
-        <v>0.1951</v>
+        <v>0.5946</v>
       </c>
       <c r="E58" t="n">
-        <v>6.3956</v>
+        <v>6.0253</v>
       </c>
       <c r="F58" t="n">
-        <v>-5.3956</v>
+        <v>-5.0253</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>0.3967</v>
+        <v>0.3708</v>
       </c>
       <c r="B59" t="n">
-        <v>1.9626</v>
+        <v>0.5505</v>
       </c>
       <c r="C59" t="n">
-        <v>-5.381</v>
+        <v>-0.0837</v>
       </c>
       <c r="D59" t="n">
-        <v>0.192</v>
+        <v>0.5919</v>
       </c>
       <c r="E59" t="n">
-        <v>6.6639</v>
+        <v>6.2263</v>
       </c>
       <c r="F59" t="n">
-        <v>-5.6639</v>
+        <v>-5.2263</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>0.4066</v>
+        <v>0.3813</v>
       </c>
       <c r="B60" t="n">
-        <v>2.0457</v>
+        <v>0.5705</v>
       </c>
       <c r="C60" t="n">
-        <v>-5.8709</v>
+        <v>-0.107</v>
       </c>
       <c r="D60" t="n">
-        <v>0.189</v>
+        <v>0.5894</v>
       </c>
       <c r="E60" t="n">
-        <v>6.9377</v>
+        <v>6.4312</v>
       </c>
       <c r="F60" t="n">
-        <v>-5.9377</v>
+        <v>-5.4312</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>0.4166</v>
+        <v>0.3919</v>
       </c>
       <c r="B61" t="n">
-        <v>2.1305</v>
+        <v>0.591</v>
       </c>
       <c r="C61" t="n">
-        <v>-6.3923</v>
+        <v>-0.1321</v>
       </c>
       <c r="D61" t="n">
-        <v>0.1861</v>
+        <v>0.5869</v>
       </c>
       <c r="E61" t="n">
-        <v>7.217</v>
+        <v>6.64</v>
       </c>
       <c r="F61" t="n">
-        <v>-6.217</v>
+        <v>-5.64</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>0.4268</v>
+        <v>0.4027</v>
       </c>
       <c r="B62" t="n">
-        <v>2.2171</v>
+        <v>0.612</v>
       </c>
       <c r="C62" t="n">
-        <v>-6.9465</v>
+        <v>-0.1591</v>
       </c>
       <c r="D62" t="n">
-        <v>0.1835</v>
+        <v>0.5845</v>
       </c>
       <c r="E62" t="n">
-        <v>7.502</v>
+        <v>6.8528</v>
       </c>
       <c r="F62" t="n">
-        <v>-6.502</v>
+        <v>-5.8528</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>0.4373</v>
+        <v>0.4138</v>
       </c>
       <c r="B63" t="n">
-        <v>2.3054</v>
+        <v>0.6334</v>
       </c>
       <c r="C63" t="n">
-        <v>-7.535</v>
+        <v>-0.188</v>
       </c>
       <c r="D63" t="n">
-        <v>0.181</v>
+        <v>0.5822000000000001</v>
       </c>
       <c r="E63" t="n">
-        <v>7.7925</v>
+        <v>7.0695</v>
       </c>
       <c r="F63" t="n">
-        <v>-6.7925</v>
+        <v>-6.0695</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>0.4479</v>
+        <v>0.425</v>
       </c>
       <c r="B64" t="n">
-        <v>2.3954</v>
+        <v>0.6552</v>
       </c>
       <c r="C64" t="n">
-        <v>-8.158899999999999</v>
+        <v>-0.2189</v>
       </c>
       <c r="D64" t="n">
-        <v>0.1786</v>
+        <v>0.58</v>
       </c>
       <c r="E64" t="n">
-        <v>8.0886</v>
+        <v>7.2901</v>
       </c>
       <c r="F64" t="n">
-        <v>-7.0886</v>
+        <v>-6.2901</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>0.4587</v>
+        <v>0.4364</v>
       </c>
       <c r="B65" t="n">
-        <v>2.4871</v>
+        <v>0.6775</v>
       </c>
       <c r="C65" t="n">
-        <v>-8.819800000000001</v>
+        <v>-0.252</v>
       </c>
       <c r="D65" t="n">
-        <v>0.1764</v>
+        <v>0.5778</v>
       </c>
       <c r="E65" t="n">
-        <v>8.3902</v>
+        <v>7.5146</v>
       </c>
       <c r="F65" t="n">
-        <v>-7.3902</v>
+        <v>-6.5146</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>0.4697</v>
+        <v>0.4481</v>
       </c>
       <c r="B66" t="n">
-        <v>2.5805</v>
+        <v>0.7000999999999999</v>
       </c>
       <c r="C66" t="n">
-        <v>-9.5191</v>
+        <v>-0.2872</v>
       </c>
       <c r="D66" t="n">
-        <v>0.1743</v>
+        <v>0.5757</v>
       </c>
       <c r="E66" t="n">
-        <v>8.6975</v>
+        <v>7.7431</v>
       </c>
       <c r="F66" t="n">
-        <v>-7.6975</v>
+        <v>-6.7431</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>0.481</v>
+        <v>0.4599</v>
       </c>
       <c r="B67" t="n">
-        <v>2.6757</v>
+        <v>0.7233000000000001</v>
       </c>
       <c r="C67" t="n">
-        <v>-10.2581</v>
+        <v>-0.3248</v>
       </c>
       <c r="D67" t="n">
-        <v>0.1723</v>
+        <v>0.5736</v>
       </c>
       <c r="E67" t="n">
-        <v>9.010300000000001</v>
+        <v>7.9755</v>
       </c>
       <c r="F67" t="n">
-        <v>-8.010300000000001</v>
+        <v>-6.9755</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>0.4924</v>
+        <v>0.4719</v>
       </c>
       <c r="B68" t="n">
-        <v>2.7726</v>
+        <v>0.7468</v>
       </c>
       <c r="C68" t="n">
-        <v>-11.0383</v>
+        <v>-0.3647</v>
       </c>
       <c r="D68" t="n">
-        <v>0.1704</v>
+        <v>0.5717</v>
       </c>
       <c r="E68" t="n">
-        <v>9.3286</v>
+        <v>8.2118</v>
       </c>
       <c r="F68" t="n">
-        <v>-8.3286</v>
+        <v>-7.2118</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>0.504</v>
+        <v>0.4842</v>
       </c>
       <c r="B69" t="n">
-        <v>2.8711</v>
+        <v>0.7708</v>
       </c>
       <c r="C69" t="n">
-        <v>-11.8612</v>
+        <v>-0.407</v>
       </c>
       <c r="D69" t="n">
-        <v>0.1686</v>
+        <v>0.5698</v>
       </c>
       <c r="E69" t="n">
-        <v>9.6526</v>
+        <v>8.4521</v>
       </c>
       <c r="F69" t="n">
-        <v>-8.6526</v>
+        <v>-7.4521</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>0.5159</v>
+        <v>0.4966</v>
       </c>
       <c r="B70" t="n">
-        <v>2.9714</v>
+        <v>0.7952</v>
       </c>
       <c r="C70" t="n">
-        <v>-12.7283</v>
+        <v>-0.4518</v>
       </c>
       <c r="D70" t="n">
-        <v>0.1669</v>
+        <v>0.5679</v>
       </c>
       <c r="E70" t="n">
-        <v>9.982100000000001</v>
+        <v>8.696300000000001</v>
       </c>
       <c r="F70" t="n">
-        <v>-8.982100000000001</v>
+        <v>-7.6963</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>0.5279</v>
+        <v>0.5092</v>
       </c>
       <c r="B71" t="n">
-        <v>3.0734</v>
+        <v>0.82</v>
       </c>
       <c r="C71" t="n">
-        <v>-13.6412</v>
+        <v>-0.4993</v>
       </c>
       <c r="D71" t="n">
-        <v>0.1652</v>
+        <v>0.5661</v>
       </c>
       <c r="E71" t="n">
-        <v>10.3172</v>
+        <v>8.9444</v>
       </c>
       <c r="F71" t="n">
-        <v>-9.3172</v>
+        <v>-7.9444</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>0.5401</v>
+        <v>0.5221</v>
       </c>
       <c r="B72" t="n">
-        <v>3.1772</v>
+        <v>0.8452</v>
       </c>
       <c r="C72" t="n">
-        <v>-14.6014</v>
+        <v>-0.5495</v>
       </c>
       <c r="D72" t="n">
-        <v>0.1637</v>
+        <v>0.5644</v>
       </c>
       <c r="E72" t="n">
-        <v>10.6578</v>
+        <v>9.196400000000001</v>
       </c>
       <c r="F72" t="n">
-        <v>-9.6578</v>
+        <v>-8.196400000000001</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>0.5525</v>
+        <v>0.5351</v>
       </c>
       <c r="B73" t="n">
-        <v>3.2826</v>
+        <v>0.8709</v>
       </c>
       <c r="C73" t="n">
-        <v>-15.6106</v>
+        <v>-0.6025</v>
       </c>
       <c r="D73" t="n">
-        <v>0.1622</v>
+        <v>0.5628</v>
       </c>
       <c r="E73" t="n">
-        <v>11.0041</v>
+        <v>9.452400000000001</v>
       </c>
       <c r="F73" t="n">
-        <v>-10.0041</v>
+        <v>-8.452400000000001</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>0.5652</v>
+        <v>0.5483</v>
       </c>
       <c r="B74" t="n">
-        <v>3.3897</v>
+        <v>0.8969</v>
       </c>
       <c r="C74" t="n">
-        <v>-16.6702</v>
+        <v>-0.6584</v>
       </c>
       <c r="D74" t="n">
-        <v>0.1608</v>
+        <v>0.5611</v>
       </c>
       <c r="E74" t="n">
-        <v>11.3559</v>
+        <v>9.712300000000001</v>
       </c>
       <c r="F74" t="n">
-        <v>-10.3559</v>
+        <v>-8.712300000000001</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>0.578</v>
+        <v>0.5617</v>
       </c>
       <c r="B75" t="n">
-        <v>3.4986</v>
+        <v>0.9234</v>
       </c>
       <c r="C75" t="n">
-        <v>-17.782</v>
+        <v>-0.7174</v>
       </c>
       <c r="D75" t="n">
-        <v>0.1595</v>
+        <v>0.5596</v>
       </c>
       <c r="E75" t="n">
-        <v>11.7132</v>
+        <v>9.976100000000001</v>
       </c>
       <c r="F75" t="n">
-        <v>-10.7132</v>
+        <v>-8.976100000000001</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>0.591</v>
+        <v>0.5754</v>
       </c>
       <c r="B76" t="n">
-        <v>3.6091</v>
+        <v>0.9503</v>
       </c>
       <c r="C76" t="n">
-        <v>-18.9477</v>
+        <v>-0.7794</v>
       </c>
       <c r="D76" t="n">
-        <v>0.1582</v>
+        <v>0.5581</v>
       </c>
       <c r="E76" t="n">
-        <v>12.0762</v>
+        <v>10.2439</v>
       </c>
       <c r="F76" t="n">
-        <v>-11.0762</v>
+        <v>-9.2439</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>0.6042999999999999</v>
+        <v>0.5891999999999999</v>
       </c>
       <c r="B77" t="n">
-        <v>3.7214</v>
+        <v>0.9777</v>
       </c>
       <c r="C77" t="n">
-        <v>-20.1689</v>
+        <v>-0.8445</v>
       </c>
       <c r="D77" t="n">
-        <v>0.157</v>
+        <v>0.5566</v>
       </c>
       <c r="E77" t="n">
-        <v>12.4447</v>
+        <v>10.5155</v>
       </c>
       <c r="F77" t="n">
-        <v>-11.4447</v>
+        <v>-9.515499999999999</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>0.6177</v>
+        <v>0.6032</v>
       </c>
       <c r="B78" t="n">
-        <v>3.8354</v>
+        <v>1.0054</v>
       </c>
       <c r="C78" t="n">
-        <v>-21.4474</v>
+        <v>-0.913</v>
       </c>
       <c r="D78" t="n">
-        <v>0.1558</v>
+        <v>0.5552</v>
       </c>
       <c r="E78" t="n">
-        <v>12.8187</v>
+        <v>10.7912</v>
       </c>
       <c r="F78" t="n">
-        <v>-11.8187</v>
+        <v>-9.7912</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>0.6313</v>
+        <v>0.6175</v>
       </c>
       <c r="B79" t="n">
-        <v>3.951</v>
+        <v>1.0336</v>
       </c>
       <c r="C79" t="n">
-        <v>-22.7848</v>
+        <v>-0.9849</v>
       </c>
       <c r="D79" t="n">
-        <v>0.1547</v>
+        <v>0.5538999999999999</v>
       </c>
       <c r="E79" t="n">
-        <v>13.1984</v>
+        <v>11.0707</v>
       </c>
       <c r="F79" t="n">
-        <v>-12.1984</v>
+        <v>-10.0707</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>0.6452</v>
+        <v>0.6319</v>
       </c>
       <c r="B80" t="n">
-        <v>4.0684</v>
+        <v>1.0621</v>
       </c>
       <c r="C80" t="n">
-        <v>-24.183</v>
+        <v>-1.0603</v>
       </c>
       <c r="D80" t="n">
-        <v>0.1537</v>
+        <v>0.5526</v>
       </c>
       <c r="E80" t="n">
-        <v>13.5836</v>
+        <v>11.3542</v>
       </c>
       <c r="F80" t="n">
-        <v>-12.5836</v>
+        <v>-10.3542</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>0.6592</v>
+        <v>0.6465</v>
       </c>
       <c r="B81" t="n">
-        <v>4.1875</v>
+        <v>1.0911</v>
       </c>
       <c r="C81" t="n">
-        <v>-25.6438</v>
+        <v>-1.1393</v>
       </c>
       <c r="D81" t="n">
-        <v>0.1526</v>
+        <v>0.5513</v>
       </c>
       <c r="E81" t="n">
-        <v>13.9744</v>
+        <v>11.6416</v>
       </c>
       <c r="F81" t="n">
-        <v>-12.9744</v>
+        <v>-10.6416</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>0.6734</v>
+        <v>0.6614</v>
       </c>
       <c r="B82" t="n">
-        <v>4.3083</v>
+        <v>1.1205</v>
       </c>
       <c r="C82" t="n">
-        <v>-27.169</v>
+        <v>-1.2219</v>
       </c>
       <c r="D82" t="n">
-        <v>0.1517</v>
+        <v>0.5501</v>
       </c>
       <c r="E82" t="n">
-        <v>14.3708</v>
+        <v>11.9329</v>
       </c>
       <c r="F82" t="n">
-        <v>-13.3708</v>
+        <v>-10.9329</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>0.6878</v>
+        <v>0.6764</v>
       </c>
       <c r="B83" t="n">
-        <v>4.4308</v>
+        <v>1.1503</v>
       </c>
       <c r="C83" t="n">
-        <v>-28.7604</v>
+        <v>-1.3084</v>
       </c>
       <c r="D83" t="n">
-        <v>0.1507</v>
+        <v>0.5489000000000001</v>
       </c>
       <c r="E83" t="n">
-        <v>14.7727</v>
+        <v>12.2281</v>
       </c>
       <c r="F83" t="n">
-        <v>-13.7727</v>
+        <v>-11.2281</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>0.7025</v>
+        <v>0.6916</v>
       </c>
       <c r="B84" t="n">
-        <v>4.555</v>
+        <v>1.1805</v>
       </c>
       <c r="C84" t="n">
-        <v>-30.4199</v>
+        <v>-1.3988</v>
       </c>
       <c r="D84" t="n">
-        <v>0.1498</v>
+        <v>0.5477</v>
       </c>
       <c r="E84" t="n">
-        <v>15.1802</v>
+        <v>12.5273</v>
       </c>
       <c r="F84" t="n">
-        <v>-14.1802</v>
+        <v>-11.5273</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>0.7173</v>
+        <v>0.7071</v>
       </c>
       <c r="B85" t="n">
-        <v>4.6809</v>
+        <v>1.2111</v>
       </c>
       <c r="C85" t="n">
-        <v>-32.1495</v>
+        <v>-1.4933</v>
       </c>
       <c r="D85" t="n">
-        <v>0.149</v>
+        <v>0.5466</v>
       </c>
       <c r="E85" t="n">
-        <v>15.5933</v>
+        <v>12.8304</v>
       </c>
       <c r="F85" t="n">
-        <v>-14.5933</v>
+        <v>-11.8304</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>0.7323</v>
+        <v>0.7227</v>
       </c>
       <c r="B86" t="n">
-        <v>4.8086</v>
+        <v>1.2422</v>
       </c>
       <c r="C86" t="n">
-        <v>-33.951</v>
+        <v>-1.5918</v>
       </c>
       <c r="D86" t="n">
-        <v>0.1481</v>
+        <v>0.5456</v>
       </c>
       <c r="E86" t="n">
-        <v>16.0119</v>
+        <v>13.1375</v>
       </c>
       <c r="F86" t="n">
-        <v>-15.0119</v>
+        <v>-12.1375</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>0.7476</v>
+        <v>0.7385</v>
       </c>
       <c r="B87" t="n">
-        <v>4.9379</v>
+        <v>1.2736</v>
       </c>
       <c r="C87" t="n">
-        <v>-35.8264</v>
+        <v>-1.6947</v>
       </c>
       <c r="D87" t="n">
-        <v>0.1473</v>
+        <v>0.5445</v>
       </c>
       <c r="E87" t="n">
-        <v>16.4362</v>
+        <v>13.4484</v>
       </c>
       <c r="F87" t="n">
-        <v>-15.4362</v>
+        <v>-12.4484</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>0.763</v>
+        <v>0.7546</v>
       </c>
       <c r="B88" t="n">
-        <v>5.0689</v>
+        <v>1.3055</v>
       </c>
       <c r="C88" t="n">
-        <v>-37.7777</v>
+        <v>-1.8019</v>
       </c>
       <c r="D88" t="n">
-        <v>0.1466</v>
+        <v>0.5435</v>
       </c>
       <c r="E88" t="n">
-        <v>16.8659</v>
+        <v>13.7633</v>
       </c>
       <c r="F88" t="n">
-        <v>-15.8659</v>
+        <v>-12.7633</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>0.7786</v>
+        <v>0.7708</v>
       </c>
       <c r="B89" t="n">
-        <v>5.2016</v>
+        <v>1.3377</v>
       </c>
       <c r="C89" t="n">
-        <v>-39.8069</v>
+        <v>-1.9136</v>
       </c>
       <c r="D89" t="n">
-        <v>0.1458</v>
+        <v>0.5425</v>
       </c>
       <c r="E89" t="n">
-        <v>17.3013</v>
+        <v>14.0822</v>
       </c>
       <c r="F89" t="n">
-        <v>-16.3013</v>
+        <v>-13.0822</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>0.7944</v>
+        <v>0.7872</v>
       </c>
       <c r="B90" t="n">
-        <v>5.3361</v>
+        <v>1.3704</v>
       </c>
       <c r="C90" t="n">
-        <v>-41.916</v>
+        <v>-2.0299</v>
       </c>
       <c r="D90" t="n">
-        <v>0.1451</v>
+        <v>0.5416</v>
       </c>
       <c r="E90" t="n">
-        <v>17.7422</v>
+        <v>14.4049</v>
       </c>
       <c r="F90" t="n">
-        <v>-16.7422</v>
+        <v>-13.4049</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>0.8105</v>
+        <v>0.8038999999999999</v>
       </c>
       <c r="B91" t="n">
-        <v>5.4722</v>
+        <v>1.4035</v>
       </c>
       <c r="C91" t="n">
-        <v>-44.1071</v>
+        <v>-2.1509</v>
       </c>
       <c r="D91" t="n">
-        <v>0.1445</v>
+        <v>0.5407</v>
       </c>
       <c r="E91" t="n">
-        <v>18.1887</v>
+        <v>14.7316</v>
       </c>
       <c r="F91" t="n">
-        <v>-17.1887</v>
+        <v>-13.7316</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>0.8267</v>
+        <v>0.8207</v>
       </c>
       <c r="B92" t="n">
-        <v>5.61</v>
+        <v>1.437</v>
       </c>
       <c r="C92" t="n">
-        <v>-46.3823</v>
+        <v>-2.2767</v>
       </c>
       <c r="D92" t="n">
-        <v>0.1438</v>
+        <v>0.5397999999999999</v>
       </c>
       <c r="E92" t="n">
-        <v>18.6408</v>
+        <v>15.0622</v>
       </c>
       <c r="F92" t="n">
-        <v>-17.6408</v>
+        <v>-14.0622</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>0.8431</v>
+        <v>0.8377</v>
       </c>
       <c r="B93" t="n">
-        <v>5.7496</v>
+        <v>1.4709</v>
       </c>
       <c r="C93" t="n">
-        <v>-48.7436</v>
+        <v>-2.4075</v>
       </c>
       <c r="D93" t="n">
-        <v>0.1432</v>
+        <v>0.5389</v>
       </c>
       <c r="E93" t="n">
-        <v>19.0985</v>
+        <v>15.3968</v>
       </c>
       <c r="F93" t="n">
-        <v>-18.0985</v>
+        <v>-14.3968</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>0.8598</v>
+        <v>0.8549</v>
       </c>
       <c r="B94" t="n">
-        <v>5.8908</v>
+        <v>1.5052</v>
       </c>
       <c r="C94" t="n">
-        <v>-51.1932</v>
+        <v>-2.5434</v>
       </c>
       <c r="D94" t="n">
-        <v>0.1426</v>
+        <v>0.5381</v>
       </c>
       <c r="E94" t="n">
-        <v>19.5617</v>
+        <v>15.7352</v>
       </c>
       <c r="F94" t="n">
-        <v>-18.5617</v>
+        <v>-14.7352</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>0.8766</v>
+        <v>0.8724</v>
       </c>
       <c r="B95" t="n">
-        <v>6.0338</v>
+        <v>1.5399</v>
       </c>
       <c r="C95" t="n">
-        <v>-53.7333</v>
+        <v>-2.6845</v>
       </c>
       <c r="D95" t="n">
-        <v>0.142</v>
+        <v>0.5373</v>
       </c>
       <c r="E95" t="n">
-        <v>20.0305</v>
+        <v>16.0776</v>
       </c>
       <c r="F95" t="n">
-        <v>-19.0305</v>
+        <v>-15.0776</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>0.8935999999999999</v>
+        <v>0.89</v>
       </c>
       <c r="B96" t="n">
-        <v>6.1784</v>
+        <v>1.575</v>
       </c>
       <c r="C96" t="n">
-        <v>-56.3661</v>
+        <v>-2.8309</v>
       </c>
       <c r="D96" t="n">
-        <v>0.1414</v>
+        <v>0.5365</v>
       </c>
       <c r="E96" t="n">
-        <v>20.5048</v>
+        <v>16.4239</v>
       </c>
       <c r="F96" t="n">
-        <v>-19.5048</v>
+        <v>-15.4239</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>0.9109</v>
+        <v>0.9078000000000001</v>
       </c>
       <c r="B97" t="n">
-        <v>6.3248</v>
+        <v>1.6105</v>
       </c>
       <c r="C97" t="n">
-        <v>-59.0937</v>
+        <v>-2.9828</v>
       </c>
       <c r="D97" t="n">
-        <v>0.1409</v>
+        <v>0.5358000000000001</v>
       </c>
       <c r="E97" t="n">
-        <v>20.9848</v>
+        <v>16.7742</v>
       </c>
       <c r="F97" t="n">
-        <v>-19.9848</v>
+        <v>-15.7742</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>0.9283</v>
+        <v>0.9258999999999999</v>
       </c>
       <c r="B98" t="n">
-        <v>6.4729</v>
+        <v>1.6464</v>
       </c>
       <c r="C98" t="n">
-        <v>-61.9185</v>
+        <v>-3.1403</v>
       </c>
       <c r="D98" t="n">
-        <v>0.1403</v>
+        <v>0.535</v>
       </c>
       <c r="E98" t="n">
-        <v>21.4703</v>
+        <v>17.1284</v>
       </c>
       <c r="F98" t="n">
-        <v>-20.4703</v>
+        <v>-16.1284</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>0.9459</v>
+        <v>0.9441000000000001</v>
       </c>
       <c r="B99" t="n">
-        <v>6.6226</v>
+        <v>1.6828</v>
       </c>
       <c r="C99" t="n">
-        <v>-64.8426</v>
+        <v>-3.3035</v>
       </c>
       <c r="D99" t="n">
-        <v>0.1398</v>
+        <v>0.5343</v>
       </c>
       <c r="E99" t="n">
-        <v>21.9613</v>
+        <v>17.4865</v>
       </c>
       <c r="F99" t="n">
-        <v>-20.9613</v>
+        <v>-16.4865</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>0.9637</v>
+        <v>0.9625</v>
       </c>
       <c r="B100" t="n">
-        <v>6.7741</v>
+        <v>1.7195</v>
       </c>
       <c r="C100" t="n">
-        <v>-67.86839999999999</v>
+        <v>-3.4726</v>
       </c>
       <c r="D100" t="n">
-        <v>0.1393</v>
+        <v>0.5336</v>
       </c>
       <c r="E100" t="n">
-        <v>22.458</v>
+        <v>17.8485</v>
       </c>
       <c r="F100" t="n">
-        <v>-21.458</v>
+        <v>-16.8485</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="n">
-        <v>0.9818</v>
+        <v>0.9812</v>
       </c>
       <c r="B101" t="n">
-        <v>6.9272</v>
+        <v>1.7567</v>
       </c>
       <c r="C101" t="n">
-        <v>-70.9982</v>
+        <v>-3.6476</v>
       </c>
       <c r="D101" t="n">
-        <v>0.1388</v>
+        <v>0.5329</v>
       </c>
       <c r="E101" t="n">
-        <v>22.9602</v>
+        <v>18.2145</v>
       </c>
       <c r="F101" t="n">
-        <v>-21.9602</v>
+        <v>-17.2145</v>
       </c>
     </row>
     <row r="102">
@@ -28468,19 +28468,19 @@
         <v>1</v>
       </c>
       <c r="B102" t="n">
-        <v>7.0821</v>
+        <v>1.7942</v>
       </c>
       <c r="C102" t="n">
-        <v>-74.23439999999999</v>
+        <v>-3.8287</v>
       </c>
       <c r="D102" t="n">
-        <v>0.1384</v>
+        <v>0.5323</v>
       </c>
       <c r="E102" t="n">
-        <v>23.468</v>
+        <v>18.5844</v>
       </c>
       <c r="F102" t="n">
-        <v>-22.468</v>
+        <v>-17.5844</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
redesigned the plotter a bit and changed the test file to backend
</commit_message>
<xml_diff>
--- a/pythonCW/230023476PortfolioProblem.xlsx
+++ b/pythonCW/230023476PortfolioProblem.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="input" sheetId="1" state="visible" r:id="rId1"/>
@@ -29,6 +29,7 @@
     </font>
     <font>
       <name val="Calibri"/>
+      <family val="2"/>
       <b val="1"/>
       <sz val="11"/>
     </font>
@@ -431,7 +432,7 @@
   </sheetPr>
   <dimension ref="A1:AI242"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
made a new version with cooler frontend
</commit_message>
<xml_diff>
--- a/pythonCW/230023476PortfolioProblem.xlsx
+++ b/pythonCW/230023476PortfolioProblem.xlsx
@@ -26428,8 +26428,8 @@
     <col width="14.4" customWidth="1" min="2" max="2"/>
     <col width="10.8" customWidth="1" min="3" max="3"/>
     <col width="16.8" customWidth="1" min="4" max="4"/>
-    <col width="8.4" customWidth="1" min="5" max="5"/>
-    <col width="7.199999999999999" customWidth="1" min="6" max="6"/>
+    <col width="4.8" customWidth="1" min="5" max="5"/>
+    <col width="4.8" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -26455,2013 +26455,2013 @@
       </c>
       <c r="E1" s="3" t="inlineStr">
         <is>
-          <t>w_USA</t>
+          <t>w1</t>
         </is>
       </c>
       <c r="F1" s="3" t="inlineStr">
         <is>
-          <t>w_UK</t>
+          <t>w2</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.104</v>
+        <v>0.1601</v>
       </c>
       <c r="B2" t="n">
-        <v>0.1545</v>
+        <v>0.2118</v>
       </c>
       <c r="C2" t="n">
-        <v>0.0682</v>
+        <v>0.09279999999999999</v>
       </c>
       <c r="D2" t="n">
-        <v>0.3819</v>
+        <v>0.5433</v>
       </c>
       <c r="E2" t="n">
-        <v>0.9849</v>
+        <v>0.0721</v>
       </c>
       <c r="F2" t="n">
-        <v>0.0151</v>
+        <v>0.9278999999999999</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0.104</v>
+        <v>0.1601</v>
       </c>
       <c r="B3" t="n">
-        <v>0.1545</v>
+        <v>0.2118</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0682</v>
+        <v>0.0929</v>
       </c>
       <c r="D3" t="n">
-        <v>0.3821</v>
+        <v>0.5436</v>
       </c>
       <c r="E3" t="n">
-        <v>0.9855</v>
+        <v>0.073</v>
       </c>
       <c r="F3" t="n">
-        <v>0.0145</v>
+        <v>0.927</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0.1042</v>
+        <v>0.1603</v>
       </c>
       <c r="B4" t="n">
-        <v>0.1545</v>
+        <v>0.2114</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0684</v>
+        <v>0.09320000000000001</v>
       </c>
       <c r="D4" t="n">
-        <v>0.383</v>
+        <v>0.5451</v>
       </c>
       <c r="E4" t="n">
-        <v>0.9882</v>
+        <v>0.0769</v>
       </c>
       <c r="F4" t="n">
-        <v>0.0118</v>
+        <v>0.9231</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0.1043</v>
+        <v>0.1603</v>
       </c>
       <c r="B5" t="n">
-        <v>0.1545</v>
+        <v>0.2112</v>
       </c>
       <c r="C5" t="n">
-        <v>0.06850000000000001</v>
+        <v>0.0934</v>
       </c>
       <c r="D5" t="n">
-        <v>0.3836</v>
+        <v>0.5461</v>
       </c>
       <c r="E5" t="n">
-        <v>0.9901</v>
+        <v>0.0793</v>
       </c>
       <c r="F5" t="n">
-        <v>0.009900000000000001</v>
+        <v>0.9207</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0.1045</v>
+        <v>0.1606</v>
       </c>
       <c r="B6" t="n">
-        <v>0.1545</v>
+        <v>0.2106</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0687</v>
+        <v>0.0941</v>
       </c>
       <c r="D6" t="n">
-        <v>0.3854</v>
+        <v>0.5491</v>
       </c>
       <c r="E6" t="n">
-        <v>0.9954</v>
+        <v>0.0872</v>
       </c>
       <c r="F6" t="n">
-        <v>0.0046</v>
+        <v>0.9127999999999999</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0.1047</v>
+        <v>0.1608</v>
       </c>
       <c r="B7" t="n">
-        <v>0.1544</v>
+        <v>0.2103</v>
       </c>
       <c r="C7" t="n">
-        <v>0.0689</v>
+        <v>0.0945</v>
       </c>
       <c r="D7" t="n">
-        <v>0.3865</v>
+        <v>0.5506</v>
       </c>
       <c r="E7" t="n">
-        <v>0.9985000000000001</v>
+        <v>0.09130000000000001</v>
       </c>
       <c r="F7" t="n">
-        <v>0.0015</v>
+        <v>0.9087</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>0.1051</v>
+        <v>0.1612</v>
       </c>
       <c r="B8" t="n">
-        <v>0.1544</v>
+        <v>0.2094</v>
       </c>
       <c r="C8" t="n">
-        <v>0.0693</v>
+        <v>0.0954</v>
       </c>
       <c r="D8" t="n">
-        <v>0.3892</v>
+        <v>0.555</v>
       </c>
       <c r="E8" t="n">
-        <v>1.0066</v>
+        <v>0.1031</v>
       </c>
       <c r="F8" t="n">
-        <v>-0.0066</v>
+        <v>0.8969</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0.1053</v>
+        <v>0.1614</v>
       </c>
       <c r="B9" t="n">
-        <v>0.1544</v>
+        <v>0.209</v>
       </c>
       <c r="C9" t="n">
-        <v>0.0696</v>
+        <v>0.0959</v>
       </c>
       <c r="D9" t="n">
-        <v>0.3907</v>
+        <v>0.5570000000000001</v>
       </c>
       <c r="E9" t="n">
-        <v>1.011</v>
+        <v>0.1088</v>
       </c>
       <c r="F9" t="n">
-        <v>-0.011</v>
+        <v>0.8912</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>0.1059</v>
+        <v>0.162</v>
       </c>
       <c r="B10" t="n">
-        <v>0.1544</v>
+        <v>0.2079</v>
       </c>
       <c r="C10" t="n">
-        <v>0.0701</v>
+        <v>0.09710000000000001</v>
       </c>
       <c r="D10" t="n">
-        <v>0.3942</v>
+        <v>0.5626</v>
       </c>
       <c r="E10" t="n">
-        <v>1.0217</v>
+        <v>0.1246</v>
       </c>
       <c r="F10" t="n">
-        <v>-0.0217</v>
+        <v>0.8754</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>0.1062</v>
+        <v>0.1622</v>
       </c>
       <c r="B11" t="n">
-        <v>0.1544</v>
+        <v>0.2075</v>
       </c>
       <c r="C11" t="n">
-        <v>0.0704</v>
+        <v>0.0977</v>
       </c>
       <c r="D11" t="n">
-        <v>0.3961</v>
+        <v>0.5651</v>
       </c>
       <c r="E11" t="n">
-        <v>1.0273</v>
+        <v>0.1319</v>
       </c>
       <c r="F11" t="n">
-        <v>-0.0273</v>
+        <v>0.8681</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>0.1068</v>
+        <v>0.1629</v>
       </c>
       <c r="B12" t="n">
-        <v>0.1544</v>
+        <v>0.2064</v>
       </c>
       <c r="C12" t="n">
-        <v>0.0711</v>
+        <v>0.09909999999999999</v>
       </c>
       <c r="D12" t="n">
-        <v>0.4006</v>
+        <v>0.5715</v>
       </c>
       <c r="E12" t="n">
-        <v>1.0407</v>
+        <v>0.1516</v>
       </c>
       <c r="F12" t="n">
-        <v>-0.0407</v>
+        <v>0.8484</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>0.1072</v>
+        <v>0.1633</v>
       </c>
       <c r="B13" t="n">
-        <v>0.1544</v>
+        <v>0.2059</v>
       </c>
       <c r="C13" t="n">
-        <v>0.07140000000000001</v>
+        <v>0.0997</v>
       </c>
       <c r="D13" t="n">
-        <v>0.4028</v>
+        <v>0.5743</v>
       </c>
       <c r="E13" t="n">
-        <v>1.0475</v>
+        <v>0.1606</v>
       </c>
       <c r="F13" t="n">
-        <v>-0.0475</v>
+        <v>0.8394</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>0.1084</v>
+        <v>0.1641</v>
       </c>
       <c r="B14" t="n">
-        <v>0.1544</v>
+        <v>0.2049</v>
       </c>
       <c r="C14" t="n">
-        <v>0.0727</v>
+        <v>0.1011</v>
       </c>
       <c r="D14" t="n">
-        <v>0.4107</v>
+        <v>0.5813</v>
       </c>
       <c r="E14" t="n">
-        <v>1.0717</v>
+        <v>0.1842</v>
       </c>
       <c r="F14" t="n">
-        <v>-0.0717</v>
+        <v>0.8158</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>0.1099</v>
+        <v>0.1645</v>
       </c>
       <c r="B15" t="n">
-        <v>0.1545</v>
+        <v>0.2045</v>
       </c>
       <c r="C15" t="n">
-        <v>0.074</v>
+        <v>0.1017</v>
       </c>
       <c r="D15" t="n">
-        <v>0.4197</v>
+        <v>0.5842000000000001</v>
       </c>
       <c r="E15" t="n">
-        <v>1.0999</v>
+        <v>0.1949</v>
       </c>
       <c r="F15" t="n">
-        <v>-0.0999</v>
+        <v>0.8051</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>0.1115</v>
+        <v>0.1655</v>
       </c>
       <c r="B16" t="n">
-        <v>0.1547</v>
+        <v>0.2038</v>
       </c>
       <c r="C16" t="n">
-        <v>0.0756</v>
+        <v>0.1032</v>
       </c>
       <c r="D16" t="n">
-        <v>0.4298</v>
+        <v>0.5911</v>
       </c>
       <c r="E16" t="n">
-        <v>1.1319</v>
+        <v>0.2224</v>
       </c>
       <c r="F16" t="n">
-        <v>-0.1319</v>
+        <v>0.7776</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>0.1133</v>
+        <v>0.1659</v>
       </c>
       <c r="B17" t="n">
-        <v>0.1549</v>
+        <v>0.2036</v>
       </c>
       <c r="C17" t="n">
-        <v>0.07729999999999999</v>
+        <v>0.1037</v>
       </c>
       <c r="D17" t="n">
-        <v>0.4409</v>
+        <v>0.5939</v>
       </c>
       <c r="E17" t="n">
-        <v>1.1679</v>
+        <v>0.2347</v>
       </c>
       <c r="F17" t="n">
-        <v>-0.1679</v>
+        <v>0.7653</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>0.1153</v>
+        <v>0.1671</v>
       </c>
       <c r="B18" t="n">
-        <v>0.1553</v>
+        <v>0.2034</v>
       </c>
       <c r="C18" t="n">
-        <v>0.07920000000000001</v>
+        <v>0.105</v>
       </c>
       <c r="D18" t="n">
-        <v>0.4529</v>
+        <v>0.6001</v>
       </c>
       <c r="E18" t="n">
-        <v>1.2078</v>
+        <v>0.2661</v>
       </c>
       <c r="F18" t="n">
-        <v>-0.2078</v>
+        <v>0.7339</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>0.1176</v>
+        <v>0.1676</v>
       </c>
       <c r="B19" t="n">
-        <v>0.1559</v>
+        <v>0.2034</v>
       </c>
       <c r="C19" t="n">
-        <v>0.08110000000000001</v>
+        <v>0.1055</v>
       </c>
       <c r="D19" t="n">
-        <v>0.4656</v>
+        <v>0.6024</v>
       </c>
       <c r="E19" t="n">
-        <v>1.2516</v>
+        <v>0.2801</v>
       </c>
       <c r="F19" t="n">
-        <v>-0.2516</v>
+        <v>0.7199</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>0.12</v>
+        <v>0.1694</v>
       </c>
       <c r="B20" t="n">
-        <v>0.1566</v>
+        <v>0.2044</v>
       </c>
       <c r="C20" t="n">
-        <v>0.0832</v>
+        <v>0.1067</v>
       </c>
       <c r="D20" t="n">
-        <v>0.4789</v>
+        <v>0.6087</v>
       </c>
       <c r="E20" t="n">
-        <v>1.2994</v>
+        <v>0.331</v>
       </c>
       <c r="F20" t="n">
-        <v>-0.2994</v>
+        <v>0.669</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>0.1226</v>
+        <v>0.1714</v>
       </c>
       <c r="B21" t="n">
-        <v>0.1576</v>
+        <v>0.2067</v>
       </c>
       <c r="C21" t="n">
-        <v>0.0854</v>
+        <v>0.1073</v>
       </c>
       <c r="D21" t="n">
-        <v>0.4927</v>
+        <v>0.6115</v>
       </c>
       <c r="E21" t="n">
-        <v>1.3511</v>
+        <v>0.3876</v>
       </c>
       <c r="F21" t="n">
-        <v>-0.3511</v>
+        <v>0.6124000000000001</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>0.1255</v>
+        <v>0.1736</v>
       </c>
       <c r="B22" t="n">
-        <v>0.1588</v>
+        <v>0.211</v>
       </c>
       <c r="C22" t="n">
-        <v>0.0876</v>
+        <v>0.1069</v>
       </c>
       <c r="D22" t="n">
-        <v>0.5067</v>
+        <v>0.6098</v>
       </c>
       <c r="E22" t="n">
-        <v>1.4067</v>
+        <v>0.4497</v>
       </c>
       <c r="F22" t="n">
-        <v>-0.4067</v>
+        <v>0.5503</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>0.1285</v>
+        <v>0.1761</v>
       </c>
       <c r="B23" t="n">
-        <v>0.1604</v>
+        <v>0.2174</v>
       </c>
       <c r="C23" t="n">
-        <v>0.08989999999999999</v>
+        <v>0.1052</v>
       </c>
       <c r="D23" t="n">
-        <v>0.5207000000000001</v>
+        <v>0.603</v>
       </c>
       <c r="E23" t="n">
-        <v>1.4662</v>
+        <v>0.5173</v>
       </c>
       <c r="F23" t="n">
-        <v>-0.4662</v>
+        <v>0.4827</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>0.1317</v>
+        <v>0.1787</v>
       </c>
       <c r="B24" t="n">
-        <v>0.1622</v>
+        <v>0.2262</v>
       </c>
       <c r="C24" t="n">
-        <v>0.09229999999999999</v>
+        <v>0.1019</v>
       </c>
       <c r="D24" t="n">
-        <v>0.5347</v>
+        <v>0.5911</v>
       </c>
       <c r="E24" t="n">
-        <v>1.5297</v>
+        <v>0.5906</v>
       </c>
       <c r="F24" t="n">
-        <v>-0.5296999999999999</v>
+        <v>0.4094</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>0.1352</v>
+        <v>0.1815</v>
       </c>
       <c r="B25" t="n">
-        <v>0.1645</v>
+        <v>0.2377</v>
       </c>
       <c r="C25" t="n">
-        <v>0.0946</v>
+        <v>0.0968</v>
       </c>
       <c r="D25" t="n">
-        <v>0.5482</v>
+        <v>0.5744</v>
       </c>
       <c r="E25" t="n">
-        <v>1.5971</v>
+        <v>0.6694</v>
       </c>
       <c r="F25" t="n">
-        <v>-0.5971</v>
+        <v>0.3306</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>0.1388</v>
+        <v>0.1846</v>
       </c>
       <c r="B26" t="n">
-        <v>0.1671</v>
+        <v>0.252</v>
       </c>
       <c r="C26" t="n">
-        <v>0.0969</v>
+        <v>0.0893</v>
       </c>
       <c r="D26" t="n">
-        <v>0.5613</v>
+        <v>0.5538</v>
       </c>
       <c r="E26" t="n">
-        <v>1.6685</v>
+        <v>0.7538</v>
       </c>
       <c r="F26" t="n">
-        <v>-0.6685</v>
+        <v>0.2462</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>0.1426</v>
+        <v>0.1878</v>
       </c>
       <c r="B27" t="n">
-        <v>0.1702</v>
+        <v>0.2691</v>
       </c>
       <c r="C27" t="n">
-        <v>0.0992</v>
+        <v>0.0791</v>
       </c>
       <c r="D27" t="n">
-        <v>0.5736</v>
+        <v>0.5306</v>
       </c>
       <c r="E27" t="n">
-        <v>1.7437</v>
+        <v>0.8437</v>
       </c>
       <c r="F27" t="n">
-        <v>-0.7437</v>
+        <v>0.1563</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>0.1467</v>
+        <v>0.1912</v>
       </c>
       <c r="B28" t="n">
-        <v>0.1737</v>
+        <v>0.2891</v>
       </c>
       <c r="C28" t="n">
-        <v>0.1014</v>
+        <v>0.0659</v>
       </c>
       <c r="D28" t="n">
-        <v>0.5851</v>
+        <v>0.5059</v>
       </c>
       <c r="E28" t="n">
-        <v>1.8229</v>
+        <v>0.9393</v>
       </c>
       <c r="F28" t="n">
-        <v>-0.8229</v>
+        <v>0.0607</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>0.1509</v>
+        <v>0.1948</v>
       </c>
       <c r="B29" t="n">
-        <v>0.1778</v>
+        <v>0.3117</v>
       </c>
       <c r="C29" t="n">
-        <v>0.1035</v>
+        <v>0.0491</v>
       </c>
       <c r="D29" t="n">
-        <v>0.5956</v>
+        <v>0.4807</v>
       </c>
       <c r="E29" t="n">
-        <v>1.906</v>
+        <v>1.0404</v>
       </c>
       <c r="F29" t="n">
-        <v>-0.906</v>
+        <v>-0.0404</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>0.1553</v>
+        <v>0.1987</v>
       </c>
       <c r="B30" t="n">
-        <v>0.1824</v>
+        <v>0.3371</v>
       </c>
       <c r="C30" t="n">
-        <v>0.1054</v>
+        <v>0.0283</v>
       </c>
       <c r="D30" t="n">
-        <v>0.605</v>
+        <v>0.4559</v>
       </c>
       <c r="E30" t="n">
-        <v>1.9931</v>
+        <v>1.147</v>
       </c>
       <c r="F30" t="n">
-        <v>-0.9931</v>
+        <v>-0.147</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>0.16</v>
+        <v>0.2027</v>
       </c>
       <c r="B31" t="n">
-        <v>0.1874</v>
+        <v>0.365</v>
       </c>
       <c r="C31" t="n">
-        <v>0.1073</v>
+        <v>0.0029</v>
       </c>
       <c r="D31" t="n">
-        <v>0.6133</v>
+        <v>0.4321</v>
       </c>
       <c r="E31" t="n">
-        <v>2.084</v>
+        <v>1.2593</v>
       </c>
       <c r="F31" t="n">
-        <v>-1.084</v>
+        <v>-0.2593</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>0.1648</v>
+        <v>0.2069</v>
       </c>
       <c r="B32" t="n">
-        <v>0.1931</v>
+        <v>0.3953</v>
       </c>
       <c r="C32" t="n">
-        <v>0.1089</v>
+        <v>-0.0275</v>
       </c>
       <c r="D32" t="n">
-        <v>0.6204</v>
+        <v>0.4096</v>
       </c>
       <c r="E32" t="n">
-        <v>2.1789</v>
+        <v>1.3771</v>
       </c>
       <c r="F32" t="n">
-        <v>-1.1789</v>
+        <v>-0.3771</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>0.1698</v>
+        <v>0.2114</v>
       </c>
       <c r="B33" t="n">
-        <v>0.1993</v>
+        <v>0.428</v>
       </c>
       <c r="C33" t="n">
-        <v>0.1102</v>
+        <v>-0.0634</v>
       </c>
       <c r="D33" t="n">
-        <v>0.6263</v>
+        <v>0.3887</v>
       </c>
       <c r="E33" t="n">
-        <v>2.2778</v>
+        <v>1.5005</v>
       </c>
       <c r="F33" t="n">
-        <v>-1.2778</v>
+        <v>-0.5004999999999999</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>0.1751</v>
+        <v>0.216</v>
       </c>
       <c r="B34" t="n">
-        <v>0.2061</v>
+        <v>0.463</v>
       </c>
       <c r="C34" t="n">
-        <v>0.1113</v>
+        <v>-0.1056</v>
       </c>
       <c r="D34" t="n">
-        <v>0.631</v>
+        <v>0.3693</v>
       </c>
       <c r="E34" t="n">
-        <v>2.3805</v>
+        <v>1.6294</v>
       </c>
       <c r="F34" t="n">
-        <v>-1.3805</v>
+        <v>-0.6294</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>0.1805</v>
+        <v>0.2208</v>
       </c>
       <c r="B35" t="n">
-        <v>0.2134</v>
+        <v>0.5002</v>
       </c>
       <c r="C35" t="n">
-        <v>0.1121</v>
+        <v>-0.1545</v>
       </c>
       <c r="D35" t="n">
-        <v>0.6347</v>
+        <v>0.3515</v>
       </c>
       <c r="E35" t="n">
-        <v>2.4872</v>
+        <v>1.764</v>
       </c>
       <c r="F35" t="n">
-        <v>-1.4872</v>
+        <v>-0.764</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>0.1861</v>
+        <v>0.2259</v>
       </c>
       <c r="B36" t="n">
-        <v>0.2214</v>
+        <v>0.5396</v>
       </c>
       <c r="C36" t="n">
-        <v>0.1126</v>
+        <v>-0.2108</v>
       </c>
       <c r="D36" t="n">
-        <v>0.6374</v>
+        <v>0.3352</v>
       </c>
       <c r="E36" t="n">
-        <v>2.5978</v>
+        <v>1.9041</v>
       </c>
       <c r="F36" t="n">
-        <v>-1.5978</v>
+        <v>-0.9041</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>0.1919</v>
+        <v>0.2311</v>
       </c>
       <c r="B37" t="n">
-        <v>0.2299</v>
+        <v>0.581</v>
       </c>
       <c r="C37" t="n">
-        <v>0.1127</v>
+        <v>-0.2752</v>
       </c>
       <c r="D37" t="n">
-        <v>0.6392</v>
+        <v>0.3203</v>
       </c>
       <c r="E37" t="n">
-        <v>2.7124</v>
+        <v>2.0497</v>
       </c>
       <c r="F37" t="n">
-        <v>-1.7124</v>
+        <v>-1.0497</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>0.198</v>
+        <v>0.2365</v>
       </c>
       <c r="B38" t="n">
-        <v>0.239</v>
+        <v>0.6244</v>
       </c>
       <c r="C38" t="n">
-        <v>0.1123</v>
+        <v>-0.3483</v>
       </c>
       <c r="D38" t="n">
-        <v>0.6402</v>
+        <v>0.3067</v>
       </c>
       <c r="E38" t="n">
-        <v>2.8309</v>
+        <v>2.201</v>
       </c>
       <c r="F38" t="n">
-        <v>-1.8309</v>
+        <v>-1.201</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>0.2042</v>
+        <v>0.2421</v>
       </c>
       <c r="B39" t="n">
-        <v>0.2486</v>
+        <v>0.6698</v>
       </c>
       <c r="C39" t="n">
-        <v>0.1115</v>
+        <v>-0.4308</v>
       </c>
       <c r="D39" t="n">
-        <v>0.6404</v>
+        <v>0.2943</v>
       </c>
       <c r="E39" t="n">
-        <v>2.9533</v>
+        <v>2.3578</v>
       </c>
       <c r="F39" t="n">
-        <v>-1.9533</v>
+        <v>-1.3578</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>0.2106</v>
+        <v>0.248</v>
       </c>
       <c r="B40" t="n">
-        <v>0.2588</v>
+        <v>0.7171999999999999</v>
       </c>
       <c r="C40" t="n">
-        <v>0.1102</v>
+        <v>-0.5235</v>
       </c>
       <c r="D40" t="n">
-        <v>0.64</v>
+        <v>0.283</v>
       </c>
       <c r="E40" t="n">
-        <v>3.0796</v>
+        <v>2.5201</v>
       </c>
       <c r="F40" t="n">
-        <v>-2.0796</v>
+        <v>-1.5201</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>0.2173</v>
+        <v>0.254</v>
       </c>
       <c r="B41" t="n">
-        <v>0.2696</v>
+        <v>0.7665</v>
       </c>
       <c r="C41" t="n">
-        <v>0.1082</v>
+        <v>-0.6272</v>
       </c>
       <c r="D41" t="n">
-        <v>0.639</v>
+        <v>0.2727</v>
       </c>
       <c r="E41" t="n">
-        <v>3.2099</v>
+        <v>2.6881</v>
       </c>
       <c r="F41" t="n">
-        <v>-2.2099</v>
+        <v>-1.6881</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>0.2241</v>
+        <v>0.2602</v>
       </c>
       <c r="B42" t="n">
-        <v>0.2809</v>
+        <v>0.8176</v>
       </c>
       <c r="C42" t="n">
-        <v>0.1057</v>
+        <v>-0.7425</v>
       </c>
       <c r="D42" t="n">
-        <v>0.6375999999999999</v>
+        <v>0.2632</v>
       </c>
       <c r="E42" t="n">
-        <v>3.344</v>
+        <v>2.8616</v>
       </c>
       <c r="F42" t="n">
-        <v>-2.344</v>
+        <v>-1.8616</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>0.2311</v>
+        <v>0.2667</v>
       </c>
       <c r="B43" t="n">
-        <v>0.2928</v>
+        <v>0.8707</v>
       </c>
       <c r="C43" t="n">
-        <v>0.1026</v>
+        <v>-0.8704</v>
       </c>
       <c r="D43" t="n">
-        <v>0.6358</v>
+        <v>0.2546</v>
       </c>
       <c r="E43" t="n">
-        <v>3.4822</v>
+        <v>3.0407</v>
       </c>
       <c r="F43" t="n">
-        <v>-2.4822</v>
+        <v>-2.0407</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>0.2384</v>
+        <v>0.2733</v>
       </c>
       <c r="B44" t="n">
-        <v>0.3052</v>
+        <v>0.9255</v>
       </c>
       <c r="C44" t="n">
-        <v>0.0987</v>
+        <v>-1.0116</v>
       </c>
       <c r="D44" t="n">
-        <v>0.6336000000000001</v>
+        <v>0.2467</v>
       </c>
       <c r="E44" t="n">
-        <v>3.6242</v>
+        <v>3.2254</v>
       </c>
       <c r="F44" t="n">
-        <v>-2.6242</v>
+        <v>-2.2254</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>0.2458</v>
+        <v>0.2801</v>
       </c>
       <c r="B45" t="n">
-        <v>0.3181</v>
+        <v>0.9822</v>
       </c>
       <c r="C45" t="n">
-        <v>0.094</v>
+        <v>-1.1671</v>
       </c>
       <c r="D45" t="n">
-        <v>0.6313</v>
+        <v>0.2394</v>
       </c>
       <c r="E45" t="n">
-        <v>3.7702</v>
+        <v>3.4156</v>
       </c>
       <c r="F45" t="n">
-        <v>-2.7702</v>
+        <v>-2.4156</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>0.2534</v>
+        <v>0.2872</v>
       </c>
       <c r="B46" t="n">
-        <v>0.3315</v>
+        <v>1.0408</v>
       </c>
       <c r="C46" t="n">
-        <v>0.0886</v>
+        <v>-1.3376</v>
       </c>
       <c r="D46" t="n">
-        <v>0.6287</v>
+        <v>0.2327</v>
       </c>
       <c r="E46" t="n">
-        <v>3.9201</v>
+        <v>3.6114</v>
       </c>
       <c r="F46" t="n">
-        <v>-2.9201</v>
+        <v>-2.6114</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>0.2613</v>
+        <v>0.2944</v>
       </c>
       <c r="B47" t="n">
-        <v>0.3455</v>
+        <v>1.1011</v>
       </c>
       <c r="C47" t="n">
-        <v>0.0822</v>
+        <v>-1.5242</v>
       </c>
       <c r="D47" t="n">
-        <v>0.626</v>
+        <v>0.2265</v>
       </c>
       <c r="E47" t="n">
-        <v>4.0739</v>
+        <v>3.8128</v>
       </c>
       <c r="F47" t="n">
-        <v>-3.0739</v>
+        <v>-2.8128</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>0.2693</v>
+        <v>0.3018</v>
       </c>
       <c r="B48" t="n">
-        <v>0.3599</v>
+        <v>1.1632</v>
       </c>
       <c r="C48" t="n">
-        <v>0.075</v>
+        <v>-1.7277</v>
       </c>
       <c r="D48" t="n">
-        <v>0.6232</v>
+        <v>0.2208</v>
       </c>
       <c r="E48" t="n">
-        <v>4.2317</v>
+        <v>4.0198</v>
       </c>
       <c r="F48" t="n">
-        <v>-3.2317</v>
+        <v>-3.0198</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>0.2775</v>
+        <v>0.3094</v>
       </c>
       <c r="B49" t="n">
-        <v>0.3749</v>
+        <v>1.2271</v>
       </c>
       <c r="C49" t="n">
-        <v>0.0667</v>
+        <v>-1.9492</v>
       </c>
       <c r="D49" t="n">
-        <v>0.6203</v>
+        <v>0.2155</v>
       </c>
       <c r="E49" t="n">
-        <v>4.3934</v>
+        <v>4.2323</v>
       </c>
       <c r="F49" t="n">
-        <v>-3.3934</v>
+        <v>-3.2323</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>0.286</v>
+        <v>0.3173</v>
       </c>
       <c r="B50" t="n">
-        <v>0.3903</v>
+        <v>1.2928</v>
       </c>
       <c r="C50" t="n">
-        <v>0.0574</v>
+        <v>-2.1896</v>
       </c>
       <c r="D50" t="n">
-        <v>0.6173</v>
+        <v>0.2106</v>
       </c>
       <c r="E50" t="n">
-        <v>4.559</v>
+        <v>4.4504</v>
       </c>
       <c r="F50" t="n">
-        <v>-3.559</v>
+        <v>-3.4504</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>0.2946</v>
+        <v>0.3253</v>
       </c>
       <c r="B51" t="n">
-        <v>0.4062</v>
+        <v>1.3602</v>
       </c>
       <c r="C51" t="n">
-        <v>0.047</v>
+        <v>-2.4499</v>
       </c>
       <c r="D51" t="n">
-        <v>0.6143999999999999</v>
+        <v>0.2061</v>
       </c>
       <c r="E51" t="n">
-        <v>4.7285</v>
+        <v>4.674</v>
       </c>
       <c r="F51" t="n">
-        <v>-3.7285</v>
+        <v>-3.674</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>0.3034</v>
+        <v>0.3335</v>
       </c>
       <c r="B52" t="n">
-        <v>0.4226</v>
+        <v>1.4294</v>
       </c>
       <c r="C52" t="n">
-        <v>0.0355</v>
+        <v>-2.7312</v>
       </c>
       <c r="D52" t="n">
-        <v>0.6114000000000001</v>
+        <v>0.2019</v>
       </c>
       <c r="E52" t="n">
-        <v>4.902</v>
+        <v>4.9033</v>
       </c>
       <c r="F52" t="n">
-        <v>-3.902</v>
+        <v>-3.9033</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>0.3125</v>
+        <v>0.342</v>
       </c>
       <c r="B53" t="n">
-        <v>0.4395</v>
+        <v>1.5003</v>
       </c>
       <c r="C53" t="n">
-        <v>0.0227</v>
+        <v>-3.0346</v>
       </c>
       <c r="D53" t="n">
-        <v>0.6085</v>
+        <v>0.1979</v>
       </c>
       <c r="E53" t="n">
-        <v>5.0794</v>
+        <v>5.1381</v>
       </c>
       <c r="F53" t="n">
-        <v>-4.0794</v>
+        <v>-4.1381</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>0.3217</v>
+        <v>0.3506</v>
       </c>
       <c r="B54" t="n">
-        <v>0.4569</v>
+        <v>1.573</v>
       </c>
       <c r="C54" t="n">
-        <v>0.0086</v>
+        <v>-3.3611</v>
       </c>
       <c r="D54" t="n">
-        <v>0.6056</v>
+        <v>0.1943</v>
       </c>
       <c r="E54" t="n">
-        <v>5.2607</v>
+        <v>5.3784</v>
       </c>
       <c r="F54" t="n">
-        <v>-4.2607</v>
+        <v>-4.3784</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>0.3311</v>
+        <v>0.3594</v>
       </c>
       <c r="B55" t="n">
-        <v>0.4747</v>
+        <v>1.6475</v>
       </c>
       <c r="C55" t="n">
-        <v>-0.0068</v>
+        <v>-3.7119</v>
       </c>
       <c r="D55" t="n">
-        <v>0.6028</v>
+        <v>0.1908</v>
       </c>
       <c r="E55" t="n">
-        <v>5.446</v>
+        <v>5.6244</v>
       </c>
       <c r="F55" t="n">
-        <v>-4.446</v>
+        <v>-4.6244</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>0.3407</v>
+        <v>0.3684</v>
       </c>
       <c r="B56" t="n">
-        <v>0.4929</v>
+        <v>1.7237</v>
       </c>
       <c r="C56" t="n">
-        <v>-0.0237</v>
+        <v>-4.0881</v>
       </c>
       <c r="D56" t="n">
-        <v>0.6</v>
+        <v>0.1877</v>
       </c>
       <c r="E56" t="n">
-        <v>5.6352</v>
+        <v>5.8759</v>
       </c>
       <c r="F56" t="n">
-        <v>-4.6352</v>
+        <v>-4.8759</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>0.3506</v>
+        <v>0.3777</v>
       </c>
       <c r="B57" t="n">
-        <v>0.5117</v>
+        <v>1.8016</v>
       </c>
       <c r="C57" t="n">
-        <v>-0.0421</v>
+        <v>-4.4908</v>
       </c>
       <c r="D57" t="n">
-        <v>0.5972</v>
+        <v>0.1847</v>
       </c>
       <c r="E57" t="n">
-        <v>5.8283</v>
+        <v>6.133</v>
       </c>
       <c r="F57" t="n">
-        <v>-4.8283</v>
+        <v>-5.133</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>0.3606</v>
+        <v>0.3871</v>
       </c>
       <c r="B58" t="n">
-        <v>0.5308</v>
+        <v>1.8812</v>
       </c>
       <c r="C58" t="n">
-        <v>-0.0621</v>
+        <v>-4.9214</v>
       </c>
       <c r="D58" t="n">
-        <v>0.5946</v>
+        <v>0.1819</v>
       </c>
       <c r="E58" t="n">
-        <v>6.0253</v>
+        <v>6.3956</v>
       </c>
       <c r="F58" t="n">
-        <v>-5.0253</v>
+        <v>-5.3956</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>0.3708</v>
+        <v>0.3967</v>
       </c>
       <c r="B59" t="n">
-        <v>0.5505</v>
+        <v>1.9626</v>
       </c>
       <c r="C59" t="n">
-        <v>-0.0837</v>
+        <v>-5.381</v>
       </c>
       <c r="D59" t="n">
-        <v>0.5919</v>
+        <v>0.1792</v>
       </c>
       <c r="E59" t="n">
-        <v>6.2263</v>
+        <v>6.6639</v>
       </c>
       <c r="F59" t="n">
-        <v>-5.2263</v>
+        <v>-5.6639</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>0.3813</v>
+        <v>0.4066</v>
       </c>
       <c r="B60" t="n">
-        <v>0.5705</v>
+        <v>2.0457</v>
       </c>
       <c r="C60" t="n">
-        <v>-0.107</v>
+        <v>-5.8709</v>
       </c>
       <c r="D60" t="n">
-        <v>0.5894</v>
+        <v>0.1767</v>
       </c>
       <c r="E60" t="n">
-        <v>6.4312</v>
+        <v>6.9377</v>
       </c>
       <c r="F60" t="n">
-        <v>-5.4312</v>
+        <v>-5.9377</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>0.3919</v>
+        <v>0.4166</v>
       </c>
       <c r="B61" t="n">
-        <v>0.591</v>
+        <v>2.1305</v>
       </c>
       <c r="C61" t="n">
-        <v>-0.1321</v>
+        <v>-6.3923</v>
       </c>
       <c r="D61" t="n">
-        <v>0.5869</v>
+        <v>0.1744</v>
       </c>
       <c r="E61" t="n">
-        <v>6.64</v>
+        <v>7.217</v>
       </c>
       <c r="F61" t="n">
-        <v>-5.64</v>
+        <v>-6.217</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>0.4027</v>
+        <v>0.4268</v>
       </c>
       <c r="B62" t="n">
-        <v>0.612</v>
+        <v>2.2171</v>
       </c>
       <c r="C62" t="n">
-        <v>-0.1591</v>
+        <v>-6.9465</v>
       </c>
       <c r="D62" t="n">
-        <v>0.5845</v>
+        <v>0.1722</v>
       </c>
       <c r="E62" t="n">
-        <v>6.8528</v>
+        <v>7.502</v>
       </c>
       <c r="F62" t="n">
-        <v>-5.8528</v>
+        <v>-6.502</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>0.4138</v>
+        <v>0.4373</v>
       </c>
       <c r="B63" t="n">
-        <v>0.6334</v>
+        <v>2.3054</v>
       </c>
       <c r="C63" t="n">
-        <v>-0.188</v>
+        <v>-7.535</v>
       </c>
       <c r="D63" t="n">
-        <v>0.5822000000000001</v>
+        <v>0.1701</v>
       </c>
       <c r="E63" t="n">
-        <v>7.0695</v>
+        <v>7.7925</v>
       </c>
       <c r="F63" t="n">
-        <v>-6.0695</v>
+        <v>-6.7925</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>0.425</v>
+        <v>0.4479</v>
       </c>
       <c r="B64" t="n">
-        <v>0.6552</v>
+        <v>2.3954</v>
       </c>
       <c r="C64" t="n">
-        <v>-0.2189</v>
+        <v>-8.158899999999999</v>
       </c>
       <c r="D64" t="n">
-        <v>0.58</v>
+        <v>0.1682</v>
       </c>
       <c r="E64" t="n">
-        <v>7.2901</v>
+        <v>8.0886</v>
       </c>
       <c r="F64" t="n">
-        <v>-6.2901</v>
+        <v>-7.0886</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>0.4364</v>
+        <v>0.4587</v>
       </c>
       <c r="B65" t="n">
-        <v>0.6775</v>
+        <v>2.4871</v>
       </c>
       <c r="C65" t="n">
-        <v>-0.252</v>
+        <v>-8.819800000000001</v>
       </c>
       <c r="D65" t="n">
-        <v>0.5778</v>
+        <v>0.1663</v>
       </c>
       <c r="E65" t="n">
-        <v>7.5146</v>
+        <v>8.3902</v>
       </c>
       <c r="F65" t="n">
-        <v>-6.5146</v>
+        <v>-7.3902</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>0.4481</v>
+        <v>0.4697</v>
       </c>
       <c r="B66" t="n">
-        <v>0.7000999999999999</v>
+        <v>2.5805</v>
       </c>
       <c r="C66" t="n">
-        <v>-0.2872</v>
+        <v>-9.5191</v>
       </c>
       <c r="D66" t="n">
-        <v>0.5757</v>
+        <v>0.1646</v>
       </c>
       <c r="E66" t="n">
-        <v>7.7431</v>
+        <v>8.6975</v>
       </c>
       <c r="F66" t="n">
-        <v>-6.7431</v>
+        <v>-7.6975</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>0.4599</v>
+        <v>0.481</v>
       </c>
       <c r="B67" t="n">
-        <v>0.7233000000000001</v>
+        <v>2.6757</v>
       </c>
       <c r="C67" t="n">
-        <v>-0.3248</v>
+        <v>-10.2581</v>
       </c>
       <c r="D67" t="n">
-        <v>0.5736</v>
+        <v>0.1629</v>
       </c>
       <c r="E67" t="n">
-        <v>7.9755</v>
+        <v>9.010300000000001</v>
       </c>
       <c r="F67" t="n">
-        <v>-6.9755</v>
+        <v>-8.010300000000001</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>0.4719</v>
+        <v>0.4924</v>
       </c>
       <c r="B68" t="n">
-        <v>0.7468</v>
+        <v>2.7726</v>
       </c>
       <c r="C68" t="n">
-        <v>-0.3647</v>
+        <v>-11.0383</v>
       </c>
       <c r="D68" t="n">
-        <v>0.5717</v>
+        <v>0.1614</v>
       </c>
       <c r="E68" t="n">
-        <v>8.2118</v>
+        <v>9.3286</v>
       </c>
       <c r="F68" t="n">
-        <v>-7.2118</v>
+        <v>-8.3286</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>0.4842</v>
+        <v>0.504</v>
       </c>
       <c r="B69" t="n">
-        <v>0.7708</v>
+        <v>2.8711</v>
       </c>
       <c r="C69" t="n">
-        <v>-0.407</v>
+        <v>-11.8612</v>
       </c>
       <c r="D69" t="n">
-        <v>0.5698</v>
+        <v>0.1599</v>
       </c>
       <c r="E69" t="n">
-        <v>8.4521</v>
+        <v>9.6526</v>
       </c>
       <c r="F69" t="n">
-        <v>-7.4521</v>
+        <v>-8.6526</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>0.4966</v>
+        <v>0.5159</v>
       </c>
       <c r="B70" t="n">
-        <v>0.7952</v>
+        <v>2.9714</v>
       </c>
       <c r="C70" t="n">
-        <v>-0.4518</v>
+        <v>-12.7283</v>
       </c>
       <c r="D70" t="n">
-        <v>0.5679</v>
+        <v>0.1585</v>
       </c>
       <c r="E70" t="n">
-        <v>8.696300000000001</v>
+        <v>9.982100000000001</v>
       </c>
       <c r="F70" t="n">
-        <v>-7.6963</v>
+        <v>-8.982100000000001</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>0.5092</v>
+        <v>0.5279</v>
       </c>
       <c r="B71" t="n">
-        <v>0.82</v>
+        <v>3.0734</v>
       </c>
       <c r="C71" t="n">
-        <v>-0.4993</v>
+        <v>-13.6412</v>
       </c>
       <c r="D71" t="n">
-        <v>0.5661</v>
+        <v>0.1571</v>
       </c>
       <c r="E71" t="n">
-        <v>8.9444</v>
+        <v>10.3172</v>
       </c>
       <c r="F71" t="n">
-        <v>-7.9444</v>
+        <v>-9.3172</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>0.5221</v>
+        <v>0.5401</v>
       </c>
       <c r="B72" t="n">
-        <v>0.8452</v>
+        <v>3.1772</v>
       </c>
       <c r="C72" t="n">
-        <v>-0.5495</v>
+        <v>-14.6014</v>
       </c>
       <c r="D72" t="n">
-        <v>0.5644</v>
+        <v>0.1558</v>
       </c>
       <c r="E72" t="n">
-        <v>9.196400000000001</v>
+        <v>10.6578</v>
       </c>
       <c r="F72" t="n">
-        <v>-8.196400000000001</v>
+        <v>-9.6578</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>0.5351</v>
+        <v>0.5525</v>
       </c>
       <c r="B73" t="n">
-        <v>0.8709</v>
+        <v>3.2826</v>
       </c>
       <c r="C73" t="n">
-        <v>-0.6025</v>
+        <v>-15.6106</v>
       </c>
       <c r="D73" t="n">
-        <v>0.5628</v>
+        <v>0.1546</v>
       </c>
       <c r="E73" t="n">
-        <v>9.452400000000001</v>
+        <v>11.0041</v>
       </c>
       <c r="F73" t="n">
-        <v>-8.452400000000001</v>
+        <v>-10.0041</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>0.5483</v>
+        <v>0.5652</v>
       </c>
       <c r="B74" t="n">
-        <v>0.8969</v>
+        <v>3.3897</v>
       </c>
       <c r="C74" t="n">
-        <v>-0.6584</v>
+        <v>-16.6702</v>
       </c>
       <c r="D74" t="n">
-        <v>0.5611</v>
+        <v>0.1535</v>
       </c>
       <c r="E74" t="n">
-        <v>9.712300000000001</v>
+        <v>11.3559</v>
       </c>
       <c r="F74" t="n">
-        <v>-8.712300000000001</v>
+        <v>-10.3559</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>0.5617</v>
+        <v>0.578</v>
       </c>
       <c r="B75" t="n">
-        <v>0.9234</v>
+        <v>3.4986</v>
       </c>
       <c r="C75" t="n">
-        <v>-0.7174</v>
+        <v>-17.782</v>
       </c>
       <c r="D75" t="n">
-        <v>0.5596</v>
+        <v>0.1523</v>
       </c>
       <c r="E75" t="n">
-        <v>9.976100000000001</v>
+        <v>11.7132</v>
       </c>
       <c r="F75" t="n">
-        <v>-8.976100000000001</v>
+        <v>-10.7132</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>0.5754</v>
+        <v>0.591</v>
       </c>
       <c r="B76" t="n">
-        <v>0.9503</v>
+        <v>3.6091</v>
       </c>
       <c r="C76" t="n">
-        <v>-0.7794</v>
+        <v>-18.9477</v>
       </c>
       <c r="D76" t="n">
-        <v>0.5581</v>
+        <v>0.1513</v>
       </c>
       <c r="E76" t="n">
-        <v>10.2439</v>
+        <v>12.0762</v>
       </c>
       <c r="F76" t="n">
-        <v>-9.2439</v>
+        <v>-11.0762</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>0.5891999999999999</v>
+        <v>0.6042999999999999</v>
       </c>
       <c r="B77" t="n">
-        <v>0.9777</v>
+        <v>3.7214</v>
       </c>
       <c r="C77" t="n">
-        <v>-0.8445</v>
+        <v>-20.1689</v>
       </c>
       <c r="D77" t="n">
-        <v>0.5566</v>
+        <v>0.1503</v>
       </c>
       <c r="E77" t="n">
-        <v>10.5155</v>
+        <v>12.4447</v>
       </c>
       <c r="F77" t="n">
-        <v>-9.515499999999999</v>
+        <v>-11.4447</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>0.6032</v>
+        <v>0.6177</v>
       </c>
       <c r="B78" t="n">
-        <v>1.0054</v>
+        <v>3.8354</v>
       </c>
       <c r="C78" t="n">
-        <v>-0.913</v>
+        <v>-21.4474</v>
       </c>
       <c r="D78" t="n">
-        <v>0.5552</v>
+        <v>0.1493</v>
       </c>
       <c r="E78" t="n">
-        <v>10.7912</v>
+        <v>12.8187</v>
       </c>
       <c r="F78" t="n">
-        <v>-9.7912</v>
+        <v>-11.8187</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>0.6175</v>
+        <v>0.6313</v>
       </c>
       <c r="B79" t="n">
-        <v>1.0336</v>
+        <v>3.951</v>
       </c>
       <c r="C79" t="n">
-        <v>-0.9849</v>
+        <v>-22.7848</v>
       </c>
       <c r="D79" t="n">
-        <v>0.5538999999999999</v>
+        <v>0.1484</v>
       </c>
       <c r="E79" t="n">
-        <v>11.0707</v>
+        <v>13.1984</v>
       </c>
       <c r="F79" t="n">
-        <v>-10.0707</v>
+        <v>-12.1984</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>0.6319</v>
+        <v>0.6452</v>
       </c>
       <c r="B80" t="n">
-        <v>1.0621</v>
+        <v>4.0684</v>
       </c>
       <c r="C80" t="n">
-        <v>-1.0603</v>
+        <v>-24.183</v>
       </c>
       <c r="D80" t="n">
-        <v>0.5526</v>
+        <v>0.1475</v>
       </c>
       <c r="E80" t="n">
-        <v>11.3542</v>
+        <v>13.5836</v>
       </c>
       <c r="F80" t="n">
-        <v>-10.3542</v>
+        <v>-12.5836</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>0.6465</v>
+        <v>0.6592</v>
       </c>
       <c r="B81" t="n">
-        <v>1.0911</v>
+        <v>4.1875</v>
       </c>
       <c r="C81" t="n">
-        <v>-1.1393</v>
+        <v>-25.6438</v>
       </c>
       <c r="D81" t="n">
-        <v>0.5513</v>
+        <v>0.1467</v>
       </c>
       <c r="E81" t="n">
-        <v>11.6416</v>
+        <v>13.9744</v>
       </c>
       <c r="F81" t="n">
-        <v>-10.6416</v>
+        <v>-12.9744</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>0.6614</v>
+        <v>0.6734</v>
       </c>
       <c r="B82" t="n">
-        <v>1.1205</v>
+        <v>4.3083</v>
       </c>
       <c r="C82" t="n">
-        <v>-1.2219</v>
+        <v>-27.169</v>
       </c>
       <c r="D82" t="n">
-        <v>0.5501</v>
+        <v>0.1459</v>
       </c>
       <c r="E82" t="n">
-        <v>11.9329</v>
+        <v>14.3708</v>
       </c>
       <c r="F82" t="n">
-        <v>-10.9329</v>
+        <v>-13.3708</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>0.6764</v>
+        <v>0.6878</v>
       </c>
       <c r="B83" t="n">
-        <v>1.1503</v>
+        <v>4.4308</v>
       </c>
       <c r="C83" t="n">
-        <v>-1.3084</v>
+        <v>-28.7604</v>
       </c>
       <c r="D83" t="n">
-        <v>0.5489000000000001</v>
+        <v>0.1451</v>
       </c>
       <c r="E83" t="n">
-        <v>12.2281</v>
+        <v>14.7727</v>
       </c>
       <c r="F83" t="n">
-        <v>-11.2281</v>
+        <v>-13.7727</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>0.6916</v>
+        <v>0.7025</v>
       </c>
       <c r="B84" t="n">
-        <v>1.1805</v>
+        <v>4.555</v>
       </c>
       <c r="C84" t="n">
-        <v>-1.3988</v>
+        <v>-30.4199</v>
       </c>
       <c r="D84" t="n">
-        <v>0.5477</v>
+        <v>0.1443</v>
       </c>
       <c r="E84" t="n">
-        <v>12.5273</v>
+        <v>15.1802</v>
       </c>
       <c r="F84" t="n">
-        <v>-11.5273</v>
+        <v>-14.1802</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>0.7071</v>
+        <v>0.7173</v>
       </c>
       <c r="B85" t="n">
-        <v>1.2111</v>
+        <v>4.6809</v>
       </c>
       <c r="C85" t="n">
-        <v>-1.4933</v>
+        <v>-32.1495</v>
       </c>
       <c r="D85" t="n">
-        <v>0.5466</v>
+        <v>0.1436</v>
       </c>
       <c r="E85" t="n">
-        <v>12.8304</v>
+        <v>15.5933</v>
       </c>
       <c r="F85" t="n">
-        <v>-11.8304</v>
+        <v>-14.5933</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>0.7227</v>
+        <v>0.7323</v>
       </c>
       <c r="B86" t="n">
-        <v>1.2422</v>
+        <v>4.8086</v>
       </c>
       <c r="C86" t="n">
-        <v>-1.5918</v>
+        <v>-33.951</v>
       </c>
       <c r="D86" t="n">
-        <v>0.5456</v>
+        <v>0.1429</v>
       </c>
       <c r="E86" t="n">
-        <v>13.1375</v>
+        <v>16.0119</v>
       </c>
       <c r="F86" t="n">
-        <v>-12.1375</v>
+        <v>-15.0119</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>0.7385</v>
+        <v>0.7476</v>
       </c>
       <c r="B87" t="n">
-        <v>1.2736</v>
+        <v>4.9379</v>
       </c>
       <c r="C87" t="n">
-        <v>-1.6947</v>
+        <v>-35.8264</v>
       </c>
       <c r="D87" t="n">
-        <v>0.5445</v>
+        <v>0.1423</v>
       </c>
       <c r="E87" t="n">
-        <v>13.4484</v>
+        <v>16.4362</v>
       </c>
       <c r="F87" t="n">
-        <v>-12.4484</v>
+        <v>-15.4362</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>0.7546</v>
+        <v>0.763</v>
       </c>
       <c r="B88" t="n">
-        <v>1.3055</v>
+        <v>5.0689</v>
       </c>
       <c r="C88" t="n">
-        <v>-1.8019</v>
+        <v>-37.7777</v>
       </c>
       <c r="D88" t="n">
-        <v>0.5435</v>
+        <v>0.1416</v>
       </c>
       <c r="E88" t="n">
-        <v>13.7633</v>
+        <v>16.8659</v>
       </c>
       <c r="F88" t="n">
-        <v>-12.7633</v>
+        <v>-15.8659</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>0.7708</v>
+        <v>0.7786</v>
       </c>
       <c r="B89" t="n">
-        <v>1.3377</v>
+        <v>5.2016</v>
       </c>
       <c r="C89" t="n">
-        <v>-1.9136</v>
+        <v>-39.8069</v>
       </c>
       <c r="D89" t="n">
-        <v>0.5425</v>
+        <v>0.141</v>
       </c>
       <c r="E89" t="n">
-        <v>14.0822</v>
+        <v>17.3013</v>
       </c>
       <c r="F89" t="n">
-        <v>-13.0822</v>
+        <v>-16.3013</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>0.7872</v>
+        <v>0.7944</v>
       </c>
       <c r="B90" t="n">
-        <v>1.3704</v>
+        <v>5.3361</v>
       </c>
       <c r="C90" t="n">
-        <v>-2.0299</v>
+        <v>-41.916</v>
       </c>
       <c r="D90" t="n">
-        <v>0.5416</v>
+        <v>0.1404</v>
       </c>
       <c r="E90" t="n">
-        <v>14.4049</v>
+        <v>17.7422</v>
       </c>
       <c r="F90" t="n">
-        <v>-13.4049</v>
+        <v>-16.7422</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>0.8038999999999999</v>
+        <v>0.8105</v>
       </c>
       <c r="B91" t="n">
-        <v>1.4035</v>
+        <v>5.4722</v>
       </c>
       <c r="C91" t="n">
-        <v>-2.1509</v>
+        <v>-44.1071</v>
       </c>
       <c r="D91" t="n">
-        <v>0.5407</v>
+        <v>0.1399</v>
       </c>
       <c r="E91" t="n">
-        <v>14.7316</v>
+        <v>18.1887</v>
       </c>
       <c r="F91" t="n">
-        <v>-13.7316</v>
+        <v>-17.1887</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>0.8207</v>
+        <v>0.8267</v>
       </c>
       <c r="B92" t="n">
-        <v>1.437</v>
+        <v>5.61</v>
       </c>
       <c r="C92" t="n">
-        <v>-2.2767</v>
+        <v>-46.3823</v>
       </c>
       <c r="D92" t="n">
-        <v>0.5397999999999999</v>
+        <v>0.1393</v>
       </c>
       <c r="E92" t="n">
-        <v>15.0622</v>
+        <v>18.6408</v>
       </c>
       <c r="F92" t="n">
-        <v>-14.0622</v>
+        <v>-17.6408</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>0.8377</v>
+        <v>0.8431</v>
       </c>
       <c r="B93" t="n">
-        <v>1.4709</v>
+        <v>5.7496</v>
       </c>
       <c r="C93" t="n">
-        <v>-2.4075</v>
+        <v>-48.7436</v>
       </c>
       <c r="D93" t="n">
-        <v>0.5389</v>
+        <v>0.1388</v>
       </c>
       <c r="E93" t="n">
-        <v>15.3968</v>
+        <v>19.0985</v>
       </c>
       <c r="F93" t="n">
-        <v>-14.3968</v>
+        <v>-18.0985</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>0.8549</v>
+        <v>0.8598</v>
       </c>
       <c r="B94" t="n">
-        <v>1.5052</v>
+        <v>5.8908</v>
       </c>
       <c r="C94" t="n">
-        <v>-2.5434</v>
+        <v>-51.1932</v>
       </c>
       <c r="D94" t="n">
-        <v>0.5381</v>
+        <v>0.1383</v>
       </c>
       <c r="E94" t="n">
-        <v>15.7352</v>
+        <v>19.5617</v>
       </c>
       <c r="F94" t="n">
-        <v>-14.7352</v>
+        <v>-18.5617</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>0.8724</v>
+        <v>0.8766</v>
       </c>
       <c r="B95" t="n">
-        <v>1.5399</v>
+        <v>6.0338</v>
       </c>
       <c r="C95" t="n">
-        <v>-2.6845</v>
+        <v>-53.7333</v>
       </c>
       <c r="D95" t="n">
-        <v>0.5373</v>
+        <v>0.1378</v>
       </c>
       <c r="E95" t="n">
-        <v>16.0776</v>
+        <v>20.0305</v>
       </c>
       <c r="F95" t="n">
-        <v>-15.0776</v>
+        <v>-19.0305</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>0.89</v>
+        <v>0.8935999999999999</v>
       </c>
       <c r="B96" t="n">
-        <v>1.575</v>
+        <v>6.1784</v>
       </c>
       <c r="C96" t="n">
-        <v>-2.8309</v>
+        <v>-56.3661</v>
       </c>
       <c r="D96" t="n">
-        <v>0.5365</v>
+        <v>0.1374</v>
       </c>
       <c r="E96" t="n">
-        <v>16.4239</v>
+        <v>20.5048</v>
       </c>
       <c r="F96" t="n">
-        <v>-15.4239</v>
+        <v>-19.5048</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>0.9078000000000001</v>
+        <v>0.9109</v>
       </c>
       <c r="B97" t="n">
-        <v>1.6105</v>
+        <v>6.3248</v>
       </c>
       <c r="C97" t="n">
-        <v>-2.9828</v>
+        <v>-59.0937</v>
       </c>
       <c r="D97" t="n">
-        <v>0.5358000000000001</v>
+        <v>0.1369</v>
       </c>
       <c r="E97" t="n">
-        <v>16.7742</v>
+        <v>20.9848</v>
       </c>
       <c r="F97" t="n">
-        <v>-15.7742</v>
+        <v>-19.9848</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>0.9258999999999999</v>
+        <v>0.9283</v>
       </c>
       <c r="B98" t="n">
-        <v>1.6464</v>
+        <v>6.4729</v>
       </c>
       <c r="C98" t="n">
-        <v>-3.1403</v>
+        <v>-61.9185</v>
       </c>
       <c r="D98" t="n">
-        <v>0.535</v>
+        <v>0.1365</v>
       </c>
       <c r="E98" t="n">
-        <v>17.1284</v>
+        <v>21.4703</v>
       </c>
       <c r="F98" t="n">
-        <v>-16.1284</v>
+        <v>-20.4703</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>0.9441000000000001</v>
+        <v>0.9459</v>
       </c>
       <c r="B99" t="n">
-        <v>1.6828</v>
+        <v>6.6226</v>
       </c>
       <c r="C99" t="n">
-        <v>-3.3035</v>
+        <v>-64.8426</v>
       </c>
       <c r="D99" t="n">
-        <v>0.5343</v>
+        <v>0.136</v>
       </c>
       <c r="E99" t="n">
-        <v>17.4865</v>
+        <v>21.9613</v>
       </c>
       <c r="F99" t="n">
-        <v>-16.4865</v>
+        <v>-20.9613</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>0.9625</v>
+        <v>0.9637</v>
       </c>
       <c r="B100" t="n">
-        <v>1.7195</v>
+        <v>6.7741</v>
       </c>
       <c r="C100" t="n">
-        <v>-3.4726</v>
+        <v>-67.86839999999999</v>
       </c>
       <c r="D100" t="n">
-        <v>0.5336</v>
+        <v>0.1356</v>
       </c>
       <c r="E100" t="n">
-        <v>17.8485</v>
+        <v>22.458</v>
       </c>
       <c r="F100" t="n">
-        <v>-16.8485</v>
+        <v>-21.458</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="n">
-        <v>0.9812</v>
+        <v>0.9818</v>
       </c>
       <c r="B101" t="n">
-        <v>1.7567</v>
+        <v>6.9272</v>
       </c>
       <c r="C101" t="n">
-        <v>-3.6476</v>
+        <v>-70.9982</v>
       </c>
       <c r="D101" t="n">
-        <v>0.5329</v>
+        <v>0.1352</v>
       </c>
       <c r="E101" t="n">
-        <v>18.2145</v>
+        <v>22.9602</v>
       </c>
       <c r="F101" t="n">
-        <v>-17.2145</v>
+        <v>-21.9602</v>
       </c>
     </row>
     <row r="102">
@@ -28469,19 +28469,19 @@
         <v>1</v>
       </c>
       <c r="B102" t="n">
-        <v>1.7942</v>
+        <v>7.0821</v>
       </c>
       <c r="C102" t="n">
-        <v>-3.8287</v>
+        <v>-74.23439999999999</v>
       </c>
       <c r="D102" t="n">
-        <v>0.5323</v>
+        <v>0.1348</v>
       </c>
       <c r="E102" t="n">
-        <v>18.5844</v>
+        <v>23.468</v>
       </c>
       <c r="F102" t="n">
-        <v>-17.5844</v>
+        <v>-22.468</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed floats and validation in backend init
</commit_message>
<xml_diff>
--- a/pythonCW/230023476PortfolioProblem.xlsx
+++ b/pythonCW/230023476PortfolioProblem.xlsx
@@ -26466,62 +26466,62 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.1601</v>
+        <v>0.16</v>
       </c>
       <c r="B2" t="n">
-        <v>0.2118</v>
+        <v>0.212</v>
       </c>
       <c r="C2" t="n">
-        <v>0.09279999999999999</v>
+        <v>0.0926</v>
       </c>
       <c r="D2" t="n">
-        <v>0.5433</v>
+        <v>0.5424</v>
       </c>
       <c r="E2" t="n">
-        <v>0.0721</v>
+        <v>0.0702</v>
       </c>
       <c r="F2" t="n">
-        <v>0.9278999999999999</v>
+        <v>0.9298</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0.1601</v>
+        <v>0.16</v>
       </c>
       <c r="B3" t="n">
-        <v>0.2118</v>
+        <v>0.2119</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0929</v>
+        <v>0.0927</v>
       </c>
       <c r="D3" t="n">
-        <v>0.5436</v>
+        <v>0.5427999999999999</v>
       </c>
       <c r="E3" t="n">
-        <v>0.073</v>
+        <v>0.07099999999999999</v>
       </c>
       <c r="F3" t="n">
-        <v>0.927</v>
+        <v>0.929</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0.1603</v>
+        <v>0.1602</v>
       </c>
       <c r="B4" t="n">
-        <v>0.2114</v>
+        <v>0.2116</v>
       </c>
       <c r="C4" t="n">
-        <v>0.09320000000000001</v>
+        <v>0.093</v>
       </c>
       <c r="D4" t="n">
-        <v>0.5451</v>
+        <v>0.5443</v>
       </c>
       <c r="E4" t="n">
-        <v>0.0769</v>
+        <v>0.075</v>
       </c>
       <c r="F4" t="n">
-        <v>0.9231</v>
+        <v>0.925</v>
       </c>
     </row>
     <row r="5">
@@ -26529,273 +26529,273 @@
         <v>0.1603</v>
       </c>
       <c r="B5" t="n">
-        <v>0.2112</v>
+        <v>0.2114</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0934</v>
+        <v>0.09320000000000001</v>
       </c>
       <c r="D5" t="n">
-        <v>0.5461</v>
+        <v>0.5453</v>
       </c>
       <c r="E5" t="n">
-        <v>0.0793</v>
+        <v>0.0775</v>
       </c>
       <c r="F5" t="n">
-        <v>0.9207</v>
+        <v>0.9225</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0.1606</v>
+        <v>0.1605</v>
       </c>
       <c r="B6" t="n">
-        <v>0.2106</v>
+        <v>0.2107</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0941</v>
+        <v>0.0939</v>
       </c>
       <c r="D6" t="n">
-        <v>0.5491</v>
+        <v>0.5482</v>
       </c>
       <c r="E6" t="n">
-        <v>0.0872</v>
+        <v>0.0854</v>
       </c>
       <c r="F6" t="n">
-        <v>0.9127999999999999</v>
+        <v>0.9146</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0.1608</v>
+        <v>0.1607</v>
       </c>
       <c r="B7" t="n">
-        <v>0.2103</v>
+        <v>0.2104</v>
       </c>
       <c r="C7" t="n">
-        <v>0.0945</v>
+        <v>0.09429999999999999</v>
       </c>
       <c r="D7" t="n">
-        <v>0.5506</v>
+        <v>0.5498</v>
       </c>
       <c r="E7" t="n">
-        <v>0.09130000000000001</v>
+        <v>0.0897</v>
       </c>
       <c r="F7" t="n">
-        <v>0.9087</v>
+        <v>0.9103</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>0.1612</v>
+        <v>0.1611</v>
       </c>
       <c r="B8" t="n">
-        <v>0.2094</v>
+        <v>0.2095</v>
       </c>
       <c r="C8" t="n">
-        <v>0.0954</v>
+        <v>0.0953</v>
       </c>
       <c r="D8" t="n">
-        <v>0.555</v>
+        <v>0.5542</v>
       </c>
       <c r="E8" t="n">
-        <v>0.1031</v>
+        <v>0.1014</v>
       </c>
       <c r="F8" t="n">
-        <v>0.8969</v>
+        <v>0.8986</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0.1614</v>
+        <v>0.1613</v>
       </c>
       <c r="B9" t="n">
-        <v>0.209</v>
+        <v>0.2091</v>
       </c>
       <c r="C9" t="n">
-        <v>0.0959</v>
+        <v>0.09569999999999999</v>
       </c>
       <c r="D9" t="n">
-        <v>0.5570000000000001</v>
+        <v>0.5563</v>
       </c>
       <c r="E9" t="n">
-        <v>0.1088</v>
+        <v>0.1074</v>
       </c>
       <c r="F9" t="n">
-        <v>0.8912</v>
+        <v>0.8925999999999999</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>0.162</v>
+        <v>0.1619</v>
       </c>
       <c r="B10" t="n">
-        <v>0.2079</v>
+        <v>0.208</v>
       </c>
       <c r="C10" t="n">
-        <v>0.09710000000000001</v>
+        <v>0.097</v>
       </c>
       <c r="D10" t="n">
-        <v>0.5626</v>
+        <v>0.5618</v>
       </c>
       <c r="E10" t="n">
-        <v>0.1246</v>
+        <v>0.1231</v>
       </c>
       <c r="F10" t="n">
-        <v>0.8754</v>
+        <v>0.8769</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>0.1622</v>
+        <v>0.1621</v>
       </c>
       <c r="B11" t="n">
         <v>0.2075</v>
       </c>
       <c r="C11" t="n">
-        <v>0.0977</v>
+        <v>0.0975</v>
       </c>
       <c r="D11" t="n">
-        <v>0.5651</v>
+        <v>0.5644</v>
       </c>
       <c r="E11" t="n">
-        <v>0.1319</v>
+        <v>0.1308</v>
       </c>
       <c r="F11" t="n">
-        <v>0.8681</v>
+        <v>0.8692</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>0.1629</v>
+        <v>0.1628</v>
       </c>
       <c r="B12" t="n">
         <v>0.2064</v>
       </c>
       <c r="C12" t="n">
-        <v>0.09909999999999999</v>
+        <v>0.0989</v>
       </c>
       <c r="D12" t="n">
-        <v>0.5715</v>
+        <v>0.5708</v>
       </c>
       <c r="E12" t="n">
-        <v>0.1516</v>
+        <v>0.1504</v>
       </c>
       <c r="F12" t="n">
-        <v>0.8484</v>
+        <v>0.8496</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>0.1633</v>
+        <v>0.1632</v>
       </c>
       <c r="B13" t="n">
-        <v>0.2059</v>
+        <v>0.206</v>
       </c>
       <c r="C13" t="n">
-        <v>0.0997</v>
+        <v>0.09950000000000001</v>
       </c>
       <c r="D13" t="n">
-        <v>0.5743</v>
+        <v>0.5738</v>
       </c>
       <c r="E13" t="n">
-        <v>0.1606</v>
+        <v>0.1599</v>
       </c>
       <c r="F13" t="n">
-        <v>0.8394</v>
+        <v>0.8401</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>0.1641</v>
+        <v>0.164</v>
       </c>
       <c r="B14" t="n">
-        <v>0.2049</v>
+        <v>0.205</v>
       </c>
       <c r="C14" t="n">
-        <v>0.1011</v>
+        <v>0.101</v>
       </c>
       <c r="D14" t="n">
-        <v>0.5813</v>
+        <v>0.5807</v>
       </c>
       <c r="E14" t="n">
-        <v>0.1842</v>
+        <v>0.1833</v>
       </c>
       <c r="F14" t="n">
-        <v>0.8158</v>
+        <v>0.8167</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>0.1645</v>
+        <v>0.1644</v>
       </c>
       <c r="B15" t="n">
-        <v>0.2045</v>
+        <v>0.2046</v>
       </c>
       <c r="C15" t="n">
-        <v>0.1017</v>
+        <v>0.1016</v>
       </c>
       <c r="D15" t="n">
-        <v>0.5842000000000001</v>
+        <v>0.5837</v>
       </c>
       <c r="E15" t="n">
-        <v>0.1949</v>
+        <v>0.1945</v>
       </c>
       <c r="F15" t="n">
-        <v>0.8051</v>
+        <v>0.8055</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>0.1655</v>
+        <v>0.1654</v>
       </c>
       <c r="B16" t="n">
         <v>0.2038</v>
       </c>
       <c r="C16" t="n">
-        <v>0.1032</v>
+        <v>0.1031</v>
       </c>
       <c r="D16" t="n">
-        <v>0.5911</v>
+        <v>0.5906</v>
       </c>
       <c r="E16" t="n">
-        <v>0.2224</v>
+        <v>0.2219</v>
       </c>
       <c r="F16" t="n">
-        <v>0.7776</v>
+        <v>0.7781</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>0.1659</v>
+        <v>0.1658</v>
       </c>
       <c r="B17" t="n">
         <v>0.2036</v>
       </c>
       <c r="C17" t="n">
-        <v>0.1037</v>
+        <v>0.1036</v>
       </c>
       <c r="D17" t="n">
-        <v>0.5939</v>
+        <v>0.5935</v>
       </c>
       <c r="E17" t="n">
-        <v>0.2347</v>
+        <v>0.2348</v>
       </c>
       <c r="F17" t="n">
-        <v>0.7653</v>
+        <v>0.7652</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>0.1671</v>
+        <v>0.1669</v>
       </c>
       <c r="B18" t="n">
         <v>0.2034</v>
       </c>
       <c r="C18" t="n">
-        <v>0.105</v>
+        <v>0.1049</v>
       </c>
       <c r="D18" t="n">
-        <v>0.6001</v>
+        <v>0.5996</v>
       </c>
       <c r="E18" t="n">
         <v>0.2661</v>
@@ -26806,62 +26806,62 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>0.1676</v>
+        <v>0.1675</v>
       </c>
       <c r="B19" t="n">
         <v>0.2034</v>
       </c>
       <c r="C19" t="n">
-        <v>0.1055</v>
+        <v>0.1054</v>
       </c>
       <c r="D19" t="n">
-        <v>0.6024</v>
+        <v>0.602</v>
       </c>
       <c r="E19" t="n">
-        <v>0.2801</v>
+        <v>0.2807</v>
       </c>
       <c r="F19" t="n">
-        <v>0.7199</v>
+        <v>0.7193000000000001</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>0.1694</v>
+        <v>0.1693</v>
       </c>
       <c r="B20" t="n">
         <v>0.2044</v>
       </c>
       <c r="C20" t="n">
-        <v>0.1067</v>
+        <v>0.1066</v>
       </c>
       <c r="D20" t="n">
-        <v>0.6087</v>
+        <v>0.6081</v>
       </c>
       <c r="E20" t="n">
-        <v>0.331</v>
+        <v>0.3323</v>
       </c>
       <c r="F20" t="n">
-        <v>0.669</v>
+        <v>0.6677</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>0.1714</v>
+        <v>0.1713</v>
       </c>
       <c r="B21" t="n">
-        <v>0.2067</v>
+        <v>0.2068</v>
       </c>
       <c r="C21" t="n">
-        <v>0.1073</v>
+        <v>0.1071</v>
       </c>
       <c r="D21" t="n">
-        <v>0.6115</v>
+        <v>0.6107</v>
       </c>
       <c r="E21" t="n">
-        <v>0.3876</v>
+        <v>0.3895</v>
       </c>
       <c r="F21" t="n">
-        <v>0.6124000000000001</v>
+        <v>0.6105</v>
       </c>
     </row>
     <row r="22">
@@ -26869,139 +26869,139 @@
         <v>0.1736</v>
       </c>
       <c r="B22" t="n">
-        <v>0.211</v>
+        <v>0.2112</v>
       </c>
       <c r="C22" t="n">
-        <v>0.1069</v>
+        <v>0.1067</v>
       </c>
       <c r="D22" t="n">
-        <v>0.6098</v>
+        <v>0.6088</v>
       </c>
       <c r="E22" t="n">
-        <v>0.4497</v>
+        <v>0.4523</v>
       </c>
       <c r="F22" t="n">
-        <v>0.5503</v>
+        <v>0.5477</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>0.1761</v>
+        <v>0.176</v>
       </c>
       <c r="B23" t="n">
-        <v>0.2174</v>
+        <v>0.2177</v>
       </c>
       <c r="C23" t="n">
-        <v>0.1052</v>
+        <v>0.1049</v>
       </c>
       <c r="D23" t="n">
-        <v>0.603</v>
+        <v>0.6016</v>
       </c>
       <c r="E23" t="n">
-        <v>0.5173</v>
+        <v>0.5208</v>
       </c>
       <c r="F23" t="n">
-        <v>0.4827</v>
+        <v>0.4792</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>0.1787</v>
+        <v>0.1786</v>
       </c>
       <c r="B24" t="n">
-        <v>0.2262</v>
+        <v>0.2268</v>
       </c>
       <c r="C24" t="n">
-        <v>0.1019</v>
+        <v>0.1015</v>
       </c>
       <c r="D24" t="n">
-        <v>0.5911</v>
+        <v>0.5891999999999999</v>
       </c>
       <c r="E24" t="n">
-        <v>0.5906</v>
+        <v>0.5949</v>
       </c>
       <c r="F24" t="n">
-        <v>0.4094</v>
+        <v>0.4051</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>0.1815</v>
+        <v>0.1814</v>
       </c>
       <c r="B25" t="n">
-        <v>0.2377</v>
+        <v>0.2385</v>
       </c>
       <c r="C25" t="n">
-        <v>0.0968</v>
+        <v>0.0961</v>
       </c>
       <c r="D25" t="n">
-        <v>0.5744</v>
+        <v>0.572</v>
       </c>
       <c r="E25" t="n">
-        <v>0.6694</v>
+        <v>0.6746</v>
       </c>
       <c r="F25" t="n">
-        <v>0.3306</v>
+        <v>0.3254</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>0.1846</v>
+        <v>0.1845</v>
       </c>
       <c r="B26" t="n">
-        <v>0.252</v>
+        <v>0.2531</v>
       </c>
       <c r="C26" t="n">
-        <v>0.0893</v>
+        <v>0.08840000000000001</v>
       </c>
       <c r="D26" t="n">
-        <v>0.5538</v>
+        <v>0.551</v>
       </c>
       <c r="E26" t="n">
-        <v>0.7538</v>
+        <v>0.76</v>
       </c>
       <c r="F26" t="n">
-        <v>0.2462</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>0.1878</v>
+        <v>0.1877</v>
       </c>
       <c r="B27" t="n">
-        <v>0.2691</v>
+        <v>0.2706</v>
       </c>
       <c r="C27" t="n">
-        <v>0.0791</v>
+        <v>0.0779</v>
       </c>
       <c r="D27" t="n">
-        <v>0.5306</v>
+        <v>0.5274</v>
       </c>
       <c r="E27" t="n">
-        <v>0.8437</v>
+        <v>0.851</v>
       </c>
       <c r="F27" t="n">
-        <v>0.1563</v>
+        <v>0.149</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>0.1912</v>
+        <v>0.1911</v>
       </c>
       <c r="B28" t="n">
-        <v>0.2891</v>
+        <v>0.2909</v>
       </c>
       <c r="C28" t="n">
-        <v>0.0659</v>
+        <v>0.06419999999999999</v>
       </c>
       <c r="D28" t="n">
-        <v>0.5059</v>
+        <v>0.5024</v>
       </c>
       <c r="E28" t="n">
-        <v>0.9393</v>
+        <v>0.9476</v>
       </c>
       <c r="F28" t="n">
-        <v>0.0607</v>
+        <v>0.0524</v>
       </c>
     </row>
     <row r="29">
@@ -27009,59 +27009,59 @@
         <v>0.1948</v>
       </c>
       <c r="B29" t="n">
-        <v>0.3117</v>
+        <v>0.3139</v>
       </c>
       <c r="C29" t="n">
-        <v>0.0491</v>
+        <v>0.0469</v>
       </c>
       <c r="D29" t="n">
-        <v>0.4807</v>
+        <v>0.4771</v>
       </c>
       <c r="E29" t="n">
-        <v>1.0404</v>
+        <v>1.0499</v>
       </c>
       <c r="F29" t="n">
-        <v>-0.0404</v>
+        <v>-0.0499</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>0.1987</v>
+        <v>0.1986</v>
       </c>
       <c r="B30" t="n">
-        <v>0.3371</v>
+        <v>0.3397</v>
       </c>
       <c r="C30" t="n">
-        <v>0.0283</v>
+        <v>0.0255</v>
       </c>
       <c r="D30" t="n">
-        <v>0.4559</v>
+        <v>0.4522</v>
       </c>
       <c r="E30" t="n">
-        <v>1.147</v>
+        <v>1.1578</v>
       </c>
       <c r="F30" t="n">
-        <v>-0.147</v>
+        <v>-0.1578</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>0.2027</v>
+        <v>0.2026</v>
       </c>
       <c r="B31" t="n">
-        <v>0.365</v>
+        <v>0.368</v>
       </c>
       <c r="C31" t="n">
-        <v>0.0029</v>
+        <v>-0.0005</v>
       </c>
       <c r="D31" t="n">
-        <v>0.4321</v>
+        <v>0.4283</v>
       </c>
       <c r="E31" t="n">
-        <v>1.2593</v>
+        <v>1.2713</v>
       </c>
       <c r="F31" t="n">
-        <v>-0.2593</v>
+        <v>-0.2713</v>
       </c>
     </row>
     <row r="32">
@@ -27069,59 +27069,59 @@
         <v>0.2069</v>
       </c>
       <c r="B32" t="n">
-        <v>0.3953</v>
+        <v>0.3988</v>
       </c>
       <c r="C32" t="n">
-        <v>-0.0275</v>
+        <v>-0.0317</v>
       </c>
       <c r="D32" t="n">
-        <v>0.4096</v>
+        <v>0.4058</v>
       </c>
       <c r="E32" t="n">
-        <v>1.3771</v>
+        <v>1.3905</v>
       </c>
       <c r="F32" t="n">
-        <v>-0.3771</v>
+        <v>-0.3905</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>0.2114</v>
+        <v>0.2113</v>
       </c>
       <c r="B33" t="n">
-        <v>0.428</v>
+        <v>0.432</v>
       </c>
       <c r="C33" t="n">
-        <v>-0.0634</v>
+        <v>-0.0687</v>
       </c>
       <c r="D33" t="n">
-        <v>0.3887</v>
+        <v>0.3849</v>
       </c>
       <c r="E33" t="n">
-        <v>1.5005</v>
+        <v>1.5153</v>
       </c>
       <c r="F33" t="n">
-        <v>-0.5004999999999999</v>
+        <v>-0.5153</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>0.216</v>
+        <v>0.2159</v>
       </c>
       <c r="B34" t="n">
-        <v>0.463</v>
+        <v>0.4675</v>
       </c>
       <c r="C34" t="n">
-        <v>-0.1056</v>
+        <v>-0.1119</v>
       </c>
       <c r="D34" t="n">
-        <v>0.3693</v>
+        <v>0.3656</v>
       </c>
       <c r="E34" t="n">
-        <v>1.6294</v>
+        <v>1.6458</v>
       </c>
       <c r="F34" t="n">
-        <v>-0.6294</v>
+        <v>-0.6458</v>
       </c>
     </row>
     <row r="35">
@@ -27129,79 +27129,79 @@
         <v>0.2208</v>
       </c>
       <c r="B35" t="n">
-        <v>0.5002</v>
+        <v>0.5052</v>
       </c>
       <c r="C35" t="n">
-        <v>-0.1545</v>
+        <v>-0.1621</v>
       </c>
       <c r="D35" t="n">
-        <v>0.3515</v>
+        <v>0.3479</v>
       </c>
       <c r="E35" t="n">
-        <v>1.764</v>
+        <v>1.7818</v>
       </c>
       <c r="F35" t="n">
-        <v>-0.764</v>
+        <v>-0.7818000000000001</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>0.2259</v>
+        <v>0.2258</v>
       </c>
       <c r="B36" t="n">
-        <v>0.5396</v>
+        <v>0.5451</v>
       </c>
       <c r="C36" t="n">
-        <v>-0.2108</v>
+        <v>-0.2199</v>
       </c>
       <c r="D36" t="n">
-        <v>0.3352</v>
+        <v>0.3317</v>
       </c>
       <c r="E36" t="n">
-        <v>1.9041</v>
+        <v>1.9235</v>
       </c>
       <c r="F36" t="n">
-        <v>-0.9041</v>
+        <v>-0.9235</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>0.2311</v>
+        <v>0.231</v>
       </c>
       <c r="B37" t="n">
-        <v>0.581</v>
+        <v>0.587</v>
       </c>
       <c r="C37" t="n">
-        <v>-0.2752</v>
+        <v>-0.2859</v>
       </c>
       <c r="D37" t="n">
-        <v>0.3203</v>
+        <v>0.3169</v>
       </c>
       <c r="E37" t="n">
-        <v>2.0497</v>
+        <v>2.0709</v>
       </c>
       <c r="F37" t="n">
-        <v>-1.0497</v>
+        <v>-1.0709</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>0.2365</v>
+        <v>0.2364</v>
       </c>
       <c r="B38" t="n">
-        <v>0.6244</v>
+        <v>0.631</v>
       </c>
       <c r="C38" t="n">
-        <v>-0.3483</v>
+        <v>-0.3608</v>
       </c>
       <c r="D38" t="n">
-        <v>0.3067</v>
+        <v>0.3034</v>
       </c>
       <c r="E38" t="n">
-        <v>2.201</v>
+        <v>2.2238</v>
       </c>
       <c r="F38" t="n">
-        <v>-1.201</v>
+        <v>-1.2238</v>
       </c>
     </row>
     <row r="39">
@@ -27209,59 +27209,59 @@
         <v>0.2421</v>
       </c>
       <c r="B39" t="n">
-        <v>0.6698</v>
+        <v>0.677</v>
       </c>
       <c r="C39" t="n">
-        <v>-0.4308</v>
+        <v>-0.4454</v>
       </c>
       <c r="D39" t="n">
-        <v>0.2943</v>
+        <v>0.2911</v>
       </c>
       <c r="E39" t="n">
-        <v>2.3578</v>
+        <v>2.3824</v>
       </c>
       <c r="F39" t="n">
-        <v>-1.3578</v>
+        <v>-1.3824</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>0.248</v>
+        <v>0.2479</v>
       </c>
       <c r="B40" t="n">
-        <v>0.7171999999999999</v>
+        <v>0.7249</v>
       </c>
       <c r="C40" t="n">
-        <v>-0.5235</v>
+        <v>-0.5404</v>
       </c>
       <c r="D40" t="n">
-        <v>0.283</v>
+        <v>0.2799</v>
       </c>
       <c r="E40" t="n">
-        <v>2.5201</v>
+        <v>2.5467</v>
       </c>
       <c r="F40" t="n">
-        <v>-1.5201</v>
+        <v>-1.5467</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>0.254</v>
+        <v>0.2539</v>
       </c>
       <c r="B41" t="n">
-        <v>0.7665</v>
+        <v>0.7748</v>
       </c>
       <c r="C41" t="n">
-        <v>-0.6272</v>
+        <v>-0.6466</v>
       </c>
       <c r="D41" t="n">
-        <v>0.2727</v>
+        <v>0.2697</v>
       </c>
       <c r="E41" t="n">
-        <v>2.6881</v>
+        <v>2.7166</v>
       </c>
       <c r="F41" t="n">
-        <v>-1.6881</v>
+        <v>-1.7166</v>
       </c>
     </row>
     <row r="42">
@@ -27269,59 +27269,59 @@
         <v>0.2602</v>
       </c>
       <c r="B42" t="n">
-        <v>0.8176</v>
+        <v>0.8266</v>
       </c>
       <c r="C42" t="n">
-        <v>-0.7425</v>
+        <v>-0.7648</v>
       </c>
       <c r="D42" t="n">
-        <v>0.2632</v>
+        <v>0.2603</v>
       </c>
       <c r="E42" t="n">
-        <v>2.8616</v>
+        <v>2.8921</v>
       </c>
       <c r="F42" t="n">
-        <v>-1.8616</v>
+        <v>-1.8921</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>0.2667</v>
+        <v>0.2666</v>
       </c>
       <c r="B43" t="n">
-        <v>0.8707</v>
+        <v>0.8803</v>
       </c>
       <c r="C43" t="n">
-        <v>-0.8704</v>
+        <v>-0.8958</v>
       </c>
       <c r="D43" t="n">
-        <v>0.2546</v>
+        <v>0.2517</v>
       </c>
       <c r="E43" t="n">
-        <v>3.0407</v>
+        <v>3.0732</v>
       </c>
       <c r="F43" t="n">
-        <v>-2.0407</v>
+        <v>-2.0732</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>0.2733</v>
+        <v>0.2732</v>
       </c>
       <c r="B44" t="n">
-        <v>0.9255</v>
+        <v>0.9358</v>
       </c>
       <c r="C44" t="n">
-        <v>-1.0116</v>
+        <v>-1.0405</v>
       </c>
       <c r="D44" t="n">
-        <v>0.2467</v>
+        <v>0.2439</v>
       </c>
       <c r="E44" t="n">
-        <v>3.2254</v>
+        <v>3.26</v>
       </c>
       <c r="F44" t="n">
-        <v>-2.2254</v>
+        <v>-2.26</v>
       </c>
     </row>
     <row r="45">
@@ -27329,59 +27329,59 @@
         <v>0.2801</v>
       </c>
       <c r="B45" t="n">
-        <v>0.9822</v>
+        <v>0.9932</v>
       </c>
       <c r="C45" t="n">
-        <v>-1.1671</v>
+        <v>-1.1997</v>
       </c>
       <c r="D45" t="n">
-        <v>0.2394</v>
+        <v>0.2367</v>
       </c>
       <c r="E45" t="n">
-        <v>3.4156</v>
+        <v>3.4524</v>
       </c>
       <c r="F45" t="n">
-        <v>-2.4156</v>
+        <v>-2.4524</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>0.2872</v>
+        <v>0.2871</v>
       </c>
       <c r="B46" t="n">
-        <v>1.0408</v>
+        <v>1.0524</v>
       </c>
       <c r="C46" t="n">
-        <v>-1.3376</v>
+        <v>-1.3744</v>
       </c>
       <c r="D46" t="n">
-        <v>0.2327</v>
+        <v>0.23</v>
       </c>
       <c r="E46" t="n">
-        <v>3.6114</v>
+        <v>3.6504</v>
       </c>
       <c r="F46" t="n">
-        <v>-2.6114</v>
+        <v>-2.6504</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>0.2944</v>
+        <v>0.2943</v>
       </c>
       <c r="B47" t="n">
-        <v>1.1011</v>
+        <v>1.1135</v>
       </c>
       <c r="C47" t="n">
-        <v>-1.5242</v>
+        <v>-1.5654</v>
       </c>
       <c r="D47" t="n">
-        <v>0.2265</v>
+        <v>0.2239</v>
       </c>
       <c r="E47" t="n">
-        <v>3.8128</v>
+        <v>3.8541</v>
       </c>
       <c r="F47" t="n">
-        <v>-2.8128</v>
+        <v>-2.8541</v>
       </c>
     </row>
     <row r="48">
@@ -27389,19 +27389,19 @@
         <v>0.3018</v>
       </c>
       <c r="B48" t="n">
-        <v>1.1632</v>
+        <v>1.1763</v>
       </c>
       <c r="C48" t="n">
-        <v>-1.7277</v>
+        <v>-1.7739</v>
       </c>
       <c r="D48" t="n">
-        <v>0.2208</v>
+        <v>0.2183</v>
       </c>
       <c r="E48" t="n">
-        <v>4.0198</v>
+        <v>4.0634</v>
       </c>
       <c r="F48" t="n">
-        <v>-3.0198</v>
+        <v>-3.0634</v>
       </c>
     </row>
     <row r="49">
@@ -27409,59 +27409,59 @@
         <v>0.3094</v>
       </c>
       <c r="B49" t="n">
-        <v>1.2271</v>
+        <v>1.241</v>
       </c>
       <c r="C49" t="n">
-        <v>-1.9492</v>
+        <v>-2.0006</v>
       </c>
       <c r="D49" t="n">
-        <v>0.2155</v>
+        <v>0.213</v>
       </c>
       <c r="E49" t="n">
-        <v>4.2323</v>
+        <v>4.2784</v>
       </c>
       <c r="F49" t="n">
-        <v>-3.2323</v>
+        <v>-3.2784</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>0.3173</v>
+        <v>0.3172</v>
       </c>
       <c r="B50" t="n">
-        <v>1.2928</v>
+        <v>1.3074</v>
       </c>
       <c r="C50" t="n">
-        <v>-2.1896</v>
+        <v>-2.2468</v>
       </c>
       <c r="D50" t="n">
-        <v>0.2106</v>
+        <v>0.2082</v>
       </c>
       <c r="E50" t="n">
-        <v>4.4504</v>
+        <v>4.4989</v>
       </c>
       <c r="F50" t="n">
-        <v>-3.4504</v>
+        <v>-3.4989</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>0.3253</v>
+        <v>0.3252</v>
       </c>
       <c r="B51" t="n">
-        <v>1.3602</v>
+        <v>1.3756</v>
       </c>
       <c r="C51" t="n">
-        <v>-2.4499</v>
+        <v>-2.5133</v>
       </c>
       <c r="D51" t="n">
-        <v>0.2061</v>
+        <v>0.2037</v>
       </c>
       <c r="E51" t="n">
-        <v>4.674</v>
+        <v>4.7252</v>
       </c>
       <c r="F51" t="n">
-        <v>-3.674</v>
+        <v>-3.7252</v>
       </c>
     </row>
     <row r="52">
@@ -27469,59 +27469,59 @@
         <v>0.3335</v>
       </c>
       <c r="B52" t="n">
-        <v>1.4294</v>
+        <v>1.4456</v>
       </c>
       <c r="C52" t="n">
-        <v>-2.7312</v>
+        <v>-2.8013</v>
       </c>
       <c r="D52" t="n">
-        <v>0.2019</v>
+        <v>0.1995</v>
       </c>
       <c r="E52" t="n">
-        <v>4.9033</v>
+        <v>4.957</v>
       </c>
       <c r="F52" t="n">
-        <v>-3.9033</v>
+        <v>-3.957</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>0.342</v>
+        <v>0.3419</v>
       </c>
       <c r="B53" t="n">
-        <v>1.5003</v>
+        <v>1.5174</v>
       </c>
       <c r="C53" t="n">
-        <v>-3.0346</v>
+        <v>-3.1119</v>
       </c>
       <c r="D53" t="n">
-        <v>0.1979</v>
+        <v>0.1957</v>
       </c>
       <c r="E53" t="n">
-        <v>5.1381</v>
+        <v>5.1945</v>
       </c>
       <c r="F53" t="n">
-        <v>-4.1381</v>
+        <v>-4.1945</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>0.3506</v>
+        <v>0.3505</v>
       </c>
       <c r="B54" t="n">
-        <v>1.573</v>
+        <v>1.5909</v>
       </c>
       <c r="C54" t="n">
-        <v>-3.3611</v>
+        <v>-3.4461</v>
       </c>
       <c r="D54" t="n">
-        <v>0.1943</v>
+        <v>0.192</v>
       </c>
       <c r="E54" t="n">
-        <v>5.3784</v>
+        <v>5.4376</v>
       </c>
       <c r="F54" t="n">
-        <v>-4.3784</v>
+        <v>-4.4376</v>
       </c>
     </row>
     <row r="55">
@@ -27529,19 +27529,19 @@
         <v>0.3594</v>
       </c>
       <c r="B55" t="n">
-        <v>1.6475</v>
+        <v>1.6662</v>
       </c>
       <c r="C55" t="n">
-        <v>-3.7119</v>
+        <v>-3.8052</v>
       </c>
       <c r="D55" t="n">
-        <v>0.1908</v>
+        <v>0.1887</v>
       </c>
       <c r="E55" t="n">
-        <v>5.6244</v>
+        <v>5.6863</v>
       </c>
       <c r="F55" t="n">
-        <v>-4.6244</v>
+        <v>-4.6863</v>
       </c>
     </row>
     <row r="56">
@@ -27549,39 +27549,39 @@
         <v>0.3684</v>
       </c>
       <c r="B56" t="n">
-        <v>1.7237</v>
+        <v>1.7433</v>
       </c>
       <c r="C56" t="n">
-        <v>-4.0881</v>
+        <v>-4.1903</v>
       </c>
       <c r="D56" t="n">
-        <v>0.1877</v>
+        <v>0.1855</v>
       </c>
       <c r="E56" t="n">
-        <v>5.8759</v>
+        <v>5.9407</v>
       </c>
       <c r="F56" t="n">
-        <v>-4.8759</v>
+        <v>-4.9407</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>0.3777</v>
+        <v>0.3776</v>
       </c>
       <c r="B57" t="n">
-        <v>1.8016</v>
+        <v>1.8221</v>
       </c>
       <c r="C57" t="n">
-        <v>-4.4908</v>
+        <v>-4.6025</v>
       </c>
       <c r="D57" t="n">
-        <v>0.1847</v>
+        <v>0.1825</v>
       </c>
       <c r="E57" t="n">
-        <v>6.133</v>
+        <v>6.2007</v>
       </c>
       <c r="F57" t="n">
-        <v>-5.133</v>
+        <v>-5.2007</v>
       </c>
     </row>
     <row r="58">
@@ -27589,19 +27589,19 @@
         <v>0.3871</v>
       </c>
       <c r="B58" t="n">
-        <v>1.8812</v>
+        <v>1.9027</v>
       </c>
       <c r="C58" t="n">
-        <v>-4.9214</v>
+        <v>-5.0433</v>
       </c>
       <c r="D58" t="n">
-        <v>0.1819</v>
+        <v>0.1798</v>
       </c>
       <c r="E58" t="n">
-        <v>6.3956</v>
+        <v>6.4664</v>
       </c>
       <c r="F58" t="n">
-        <v>-5.3956</v>
+        <v>-5.4664</v>
       </c>
     </row>
     <row r="59">
@@ -27609,59 +27609,59 @@
         <v>0.3967</v>
       </c>
       <c r="B59" t="n">
-        <v>1.9626</v>
+        <v>1.985</v>
       </c>
       <c r="C59" t="n">
-        <v>-5.381</v>
+        <v>-5.5137</v>
       </c>
       <c r="D59" t="n">
-        <v>0.1792</v>
+        <v>0.1772</v>
       </c>
       <c r="E59" t="n">
-        <v>6.6639</v>
+        <v>6.7377</v>
       </c>
       <c r="F59" t="n">
-        <v>-5.6639</v>
+        <v>-5.7377</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>0.4066</v>
+        <v>0.4065</v>
       </c>
       <c r="B60" t="n">
-        <v>2.0457</v>
+        <v>2.0691</v>
       </c>
       <c r="C60" t="n">
-        <v>-5.8709</v>
+        <v>-6.015</v>
       </c>
       <c r="D60" t="n">
-        <v>0.1767</v>
+        <v>0.1747</v>
       </c>
       <c r="E60" t="n">
-        <v>6.9377</v>
+        <v>7.0146</v>
       </c>
       <c r="F60" t="n">
-        <v>-5.9377</v>
+        <v>-6.0146</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>0.4166</v>
+        <v>0.4165</v>
       </c>
       <c r="B61" t="n">
-        <v>2.1305</v>
+        <v>2.1549</v>
       </c>
       <c r="C61" t="n">
-        <v>-6.3923</v>
+        <v>-6.5487</v>
       </c>
       <c r="D61" t="n">
-        <v>0.1744</v>
+        <v>0.1724</v>
       </c>
       <c r="E61" t="n">
-        <v>7.217</v>
+        <v>7.2971</v>
       </c>
       <c r="F61" t="n">
-        <v>-6.217</v>
+        <v>-6.2971</v>
       </c>
     </row>
     <row r="62">
@@ -27669,59 +27669,59 @@
         <v>0.4268</v>
       </c>
       <c r="B62" t="n">
-        <v>2.2171</v>
+        <v>2.2424</v>
       </c>
       <c r="C62" t="n">
-        <v>-6.9465</v>
+        <v>-7.1159</v>
       </c>
       <c r="D62" t="n">
-        <v>0.1722</v>
+        <v>0.1703</v>
       </c>
       <c r="E62" t="n">
-        <v>7.502</v>
+        <v>7.5853</v>
       </c>
       <c r="F62" t="n">
-        <v>-6.502</v>
+        <v>-6.5853</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>0.4373</v>
+        <v>0.4372</v>
       </c>
       <c r="B63" t="n">
-        <v>2.3054</v>
+        <v>2.3317</v>
       </c>
       <c r="C63" t="n">
-        <v>-7.535</v>
+        <v>-7.7182</v>
       </c>
       <c r="D63" t="n">
-        <v>0.1701</v>
+        <v>0.1682</v>
       </c>
       <c r="E63" t="n">
-        <v>7.7925</v>
+        <v>7.8791</v>
       </c>
       <c r="F63" t="n">
-        <v>-6.7925</v>
+        <v>-6.8791</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>0.4479</v>
+        <v>0.4478</v>
       </c>
       <c r="B64" t="n">
-        <v>2.3954</v>
+        <v>2.4228</v>
       </c>
       <c r="C64" t="n">
-        <v>-8.158899999999999</v>
+        <v>-8.3567</v>
       </c>
       <c r="D64" t="n">
-        <v>0.1682</v>
+        <v>0.1663</v>
       </c>
       <c r="E64" t="n">
-        <v>8.0886</v>
+        <v>8.178599999999999</v>
       </c>
       <c r="F64" t="n">
-        <v>-7.0886</v>
+        <v>-7.1786</v>
       </c>
     </row>
     <row r="65">
@@ -27729,19 +27729,19 @@
         <v>0.4587</v>
       </c>
       <c r="B65" t="n">
-        <v>2.4871</v>
+        <v>2.5155</v>
       </c>
       <c r="C65" t="n">
-        <v>-8.819800000000001</v>
+        <v>-9.033099999999999</v>
       </c>
       <c r="D65" t="n">
-        <v>0.1663</v>
+        <v>0.1644</v>
       </c>
       <c r="E65" t="n">
-        <v>8.3902</v>
+        <v>8.483700000000001</v>
       </c>
       <c r="F65" t="n">
-        <v>-7.3902</v>
+        <v>-7.4837</v>
       </c>
     </row>
     <row r="66">
@@ -27749,39 +27749,39 @@
         <v>0.4697</v>
       </c>
       <c r="B66" t="n">
-        <v>2.5805</v>
+        <v>2.61</v>
       </c>
       <c r="C66" t="n">
-        <v>-9.5191</v>
+        <v>-9.7486</v>
       </c>
       <c r="D66" t="n">
-        <v>0.1646</v>
+        <v>0.1627</v>
       </c>
       <c r="E66" t="n">
-        <v>8.6975</v>
+        <v>8.7944</v>
       </c>
       <c r="F66" t="n">
-        <v>-7.6975</v>
+        <v>-7.7944</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>0.481</v>
+        <v>0.4809</v>
       </c>
       <c r="B67" t="n">
-        <v>2.6757</v>
+        <v>2.7063</v>
       </c>
       <c r="C67" t="n">
-        <v>-10.2581</v>
+        <v>-10.5049</v>
       </c>
       <c r="D67" t="n">
-        <v>0.1629</v>
+        <v>0.1611</v>
       </c>
       <c r="E67" t="n">
-        <v>9.010300000000001</v>
+        <v>9.1107</v>
       </c>
       <c r="F67" t="n">
-        <v>-8.010300000000001</v>
+        <v>-8.1107</v>
       </c>
     </row>
     <row r="68">
@@ -27789,19 +27789,19 @@
         <v>0.4924</v>
       </c>
       <c r="B68" t="n">
-        <v>2.7726</v>
+        <v>2.8042</v>
       </c>
       <c r="C68" t="n">
-        <v>-11.0383</v>
+        <v>-11.3033</v>
       </c>
       <c r="D68" t="n">
-        <v>0.1614</v>
+        <v>0.1595</v>
       </c>
       <c r="E68" t="n">
-        <v>9.3286</v>
+        <v>9.432700000000001</v>
       </c>
       <c r="F68" t="n">
-        <v>-8.3286</v>
+        <v>-8.432700000000001</v>
       </c>
     </row>
     <row r="69">
@@ -27809,39 +27809,39 @@
         <v>0.504</v>
       </c>
       <c r="B69" t="n">
-        <v>2.8711</v>
+        <v>2.9039</v>
       </c>
       <c r="C69" t="n">
-        <v>-11.8612</v>
+        <v>-12.1454</v>
       </c>
       <c r="D69" t="n">
-        <v>0.1599</v>
+        <v>0.1581</v>
       </c>
       <c r="E69" t="n">
-        <v>9.6526</v>
+        <v>9.760400000000001</v>
       </c>
       <c r="F69" t="n">
-        <v>-8.6526</v>
+        <v>-8.760400000000001</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>0.5159</v>
+        <v>0.5158</v>
       </c>
       <c r="B70" t="n">
-        <v>2.9714</v>
+        <v>3.0054</v>
       </c>
       <c r="C70" t="n">
-        <v>-12.7283</v>
+        <v>-13.0327</v>
       </c>
       <c r="D70" t="n">
-        <v>0.1585</v>
+        <v>0.1567</v>
       </c>
       <c r="E70" t="n">
-        <v>9.982100000000001</v>
+        <v>10.0936</v>
       </c>
       <c r="F70" t="n">
-        <v>-8.982100000000001</v>
+        <v>-9.0936</v>
       </c>
     </row>
     <row r="71">
@@ -27849,19 +27849,19 @@
         <v>0.5279</v>
       </c>
       <c r="B71" t="n">
-        <v>3.0734</v>
+        <v>3.1086</v>
       </c>
       <c r="C71" t="n">
-        <v>-13.6412</v>
+        <v>-13.9668</v>
       </c>
       <c r="D71" t="n">
-        <v>0.1571</v>
+        <v>0.1553</v>
       </c>
       <c r="E71" t="n">
-        <v>10.3172</v>
+        <v>10.4325</v>
       </c>
       <c r="F71" t="n">
-        <v>-9.3172</v>
+        <v>-9.432499999999999</v>
       </c>
     </row>
     <row r="72">
@@ -27869,19 +27869,19 @@
         <v>0.5401</v>
       </c>
       <c r="B72" t="n">
-        <v>3.1772</v>
+        <v>3.2135</v>
       </c>
       <c r="C72" t="n">
-        <v>-14.6014</v>
+        <v>-14.9494</v>
       </c>
       <c r="D72" t="n">
-        <v>0.1558</v>
+        <v>0.1541</v>
       </c>
       <c r="E72" t="n">
-        <v>10.6578</v>
+        <v>10.777</v>
       </c>
       <c r="F72" t="n">
-        <v>-9.6578</v>
+        <v>-9.776999999999999</v>
       </c>
     </row>
     <row r="73">
@@ -27889,39 +27889,39 @@
         <v>0.5525</v>
       </c>
       <c r="B73" t="n">
-        <v>3.2826</v>
+        <v>3.3201</v>
       </c>
       <c r="C73" t="n">
-        <v>-15.6106</v>
+        <v>-15.9819</v>
       </c>
       <c r="D73" t="n">
-        <v>0.1546</v>
+        <v>0.1529</v>
       </c>
       <c r="E73" t="n">
-        <v>11.0041</v>
+        <v>11.1272</v>
       </c>
       <c r="F73" t="n">
-        <v>-10.0041</v>
+        <v>-10.1272</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>0.5652</v>
+        <v>0.5651</v>
       </c>
       <c r="B74" t="n">
-        <v>3.3897</v>
+        <v>3.4284</v>
       </c>
       <c r="C74" t="n">
-        <v>-16.6702</v>
+        <v>-17.0662</v>
       </c>
       <c r="D74" t="n">
-        <v>0.1535</v>
+        <v>0.1517</v>
       </c>
       <c r="E74" t="n">
-        <v>11.3559</v>
+        <v>11.483</v>
       </c>
       <c r="F74" t="n">
-        <v>-10.3559</v>
+        <v>-10.483</v>
       </c>
     </row>
     <row r="75">
@@ -27929,19 +27929,19 @@
         <v>0.578</v>
       </c>
       <c r="B75" t="n">
-        <v>3.4986</v>
+        <v>3.5385</v>
       </c>
       <c r="C75" t="n">
-        <v>-17.782</v>
+        <v>-18.2038</v>
       </c>
       <c r="D75" t="n">
-        <v>0.1523</v>
+        <v>0.1506</v>
       </c>
       <c r="E75" t="n">
-        <v>11.7132</v>
+        <v>11.8444</v>
       </c>
       <c r="F75" t="n">
-        <v>-10.7132</v>
+        <v>-10.8444</v>
       </c>
     </row>
     <row r="76">
@@ -27949,39 +27949,39 @@
         <v>0.591</v>
       </c>
       <c r="B76" t="n">
-        <v>3.6091</v>
+        <v>3.6503</v>
       </c>
       <c r="C76" t="n">
-        <v>-18.9477</v>
+        <v>-19.3965</v>
       </c>
       <c r="D76" t="n">
-        <v>0.1513</v>
+        <v>0.1496</v>
       </c>
       <c r="E76" t="n">
-        <v>12.0762</v>
+        <v>12.2114</v>
       </c>
       <c r="F76" t="n">
-        <v>-11.0762</v>
+        <v>-11.2114</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>0.6042999999999999</v>
+        <v>0.6042</v>
       </c>
       <c r="B77" t="n">
-        <v>3.7214</v>
+        <v>3.7639</v>
       </c>
       <c r="C77" t="n">
-        <v>-20.1689</v>
+        <v>-20.646</v>
       </c>
       <c r="D77" t="n">
-        <v>0.1503</v>
+        <v>0.1486</v>
       </c>
       <c r="E77" t="n">
-        <v>12.4447</v>
+        <v>12.5841</v>
       </c>
       <c r="F77" t="n">
-        <v>-11.4447</v>
+        <v>-11.5841</v>
       </c>
     </row>
     <row r="78">
@@ -27989,19 +27989,19 @@
         <v>0.6177</v>
       </c>
       <c r="B78" t="n">
-        <v>3.8354</v>
+        <v>3.8792</v>
       </c>
       <c r="C78" t="n">
-        <v>-21.4474</v>
+        <v>-21.9541</v>
       </c>
       <c r="D78" t="n">
-        <v>0.1493</v>
+        <v>0.1476</v>
       </c>
       <c r="E78" t="n">
-        <v>12.8187</v>
+        <v>12.9625</v>
       </c>
       <c r="F78" t="n">
-        <v>-11.8187</v>
+        <v>-11.9625</v>
       </c>
     </row>
     <row r="79">
@@ -28009,39 +28009,39 @@
         <v>0.6313</v>
       </c>
       <c r="B79" t="n">
-        <v>3.951</v>
+        <v>3.9961</v>
       </c>
       <c r="C79" t="n">
-        <v>-22.7848</v>
+        <v>-23.3225</v>
       </c>
       <c r="D79" t="n">
-        <v>0.1484</v>
+        <v>0.1467</v>
       </c>
       <c r="E79" t="n">
-        <v>13.1984</v>
+        <v>13.3464</v>
       </c>
       <c r="F79" t="n">
-        <v>-12.1984</v>
+        <v>-12.3464</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>0.6452</v>
+        <v>0.6451</v>
       </c>
       <c r="B80" t="n">
-        <v>4.0684</v>
+        <v>4.1149</v>
       </c>
       <c r="C80" t="n">
-        <v>-24.183</v>
+        <v>-24.7531</v>
       </c>
       <c r="D80" t="n">
-        <v>0.1475</v>
+        <v>0.1458</v>
       </c>
       <c r="E80" t="n">
-        <v>13.5836</v>
+        <v>13.736</v>
       </c>
       <c r="F80" t="n">
-        <v>-12.5836</v>
+        <v>-12.736</v>
       </c>
     </row>
     <row r="81">
@@ -28049,19 +28049,19 @@
         <v>0.6592</v>
       </c>
       <c r="B81" t="n">
-        <v>4.1875</v>
+        <v>4.2353</v>
       </c>
       <c r="C81" t="n">
-        <v>-25.6438</v>
+        <v>-26.2477</v>
       </c>
       <c r="D81" t="n">
-        <v>0.1467</v>
+        <v>0.145</v>
       </c>
       <c r="E81" t="n">
-        <v>13.9744</v>
+        <v>14.1312</v>
       </c>
       <c r="F81" t="n">
-        <v>-12.9744</v>
+        <v>-13.1312</v>
       </c>
     </row>
     <row r="82">
@@ -28069,19 +28069,19 @@
         <v>0.6734</v>
       </c>
       <c r="B82" t="n">
-        <v>4.3083</v>
+        <v>4.3575</v>
       </c>
       <c r="C82" t="n">
-        <v>-27.169</v>
+        <v>-27.8081</v>
       </c>
       <c r="D82" t="n">
-        <v>0.1459</v>
+        <v>0.1442</v>
       </c>
       <c r="E82" t="n">
-        <v>14.3708</v>
+        <v>14.5321</v>
       </c>
       <c r="F82" t="n">
-        <v>-13.3708</v>
+        <v>-13.5321</v>
       </c>
     </row>
     <row r="83">
@@ -28089,19 +28089,19 @@
         <v>0.6878</v>
       </c>
       <c r="B83" t="n">
-        <v>4.4308</v>
+        <v>4.4814</v>
       </c>
       <c r="C83" t="n">
-        <v>-28.7604</v>
+        <v>-29.4363</v>
       </c>
       <c r="D83" t="n">
-        <v>0.1451</v>
+        <v>0.1434</v>
       </c>
       <c r="E83" t="n">
-        <v>14.7727</v>
+        <v>14.9386</v>
       </c>
       <c r="F83" t="n">
-        <v>-13.7727</v>
+        <v>-13.9386</v>
       </c>
     </row>
     <row r="84">
@@ -28109,19 +28109,19 @@
         <v>0.7025</v>
       </c>
       <c r="B84" t="n">
-        <v>4.555</v>
+        <v>4.607</v>
       </c>
       <c r="C84" t="n">
-        <v>-30.4199</v>
+        <v>-31.1342</v>
       </c>
       <c r="D84" t="n">
-        <v>0.1443</v>
+        <v>0.1427</v>
       </c>
       <c r="E84" t="n">
-        <v>15.1802</v>
+        <v>15.3507</v>
       </c>
       <c r="F84" t="n">
-        <v>-14.1802</v>
+        <v>-14.3507</v>
       </c>
     </row>
     <row r="85">
@@ -28129,19 +28129,19 @@
         <v>0.7173</v>
       </c>
       <c r="B85" t="n">
-        <v>4.6809</v>
+        <v>4.7343</v>
       </c>
       <c r="C85" t="n">
-        <v>-32.1495</v>
+        <v>-32.9037</v>
       </c>
       <c r="D85" t="n">
-        <v>0.1436</v>
+        <v>0.142</v>
       </c>
       <c r="E85" t="n">
-        <v>15.5933</v>
+        <v>15.7685</v>
       </c>
       <c r="F85" t="n">
-        <v>-14.5933</v>
+        <v>-14.7685</v>
       </c>
     </row>
     <row r="86">
@@ -28149,39 +28149,39 @@
         <v>0.7323</v>
       </c>
       <c r="B86" t="n">
-        <v>4.8086</v>
+        <v>4.8634</v>
       </c>
       <c r="C86" t="n">
-        <v>-33.951</v>
+        <v>-34.7468</v>
       </c>
       <c r="D86" t="n">
-        <v>0.1429</v>
+        <v>0.1413</v>
       </c>
       <c r="E86" t="n">
-        <v>16.0119</v>
+        <v>16.1919</v>
       </c>
       <c r="F86" t="n">
-        <v>-15.0119</v>
+        <v>-15.1919</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>0.7476</v>
+        <v>0.7475000000000001</v>
       </c>
       <c r="B87" t="n">
-        <v>4.9379</v>
+        <v>4.9942</v>
       </c>
       <c r="C87" t="n">
-        <v>-35.8264</v>
+        <v>-36.6655</v>
       </c>
       <c r="D87" t="n">
-        <v>0.1423</v>
+        <v>0.1407</v>
       </c>
       <c r="E87" t="n">
-        <v>16.4362</v>
+        <v>16.6209</v>
       </c>
       <c r="F87" t="n">
-        <v>-15.4362</v>
+        <v>-15.6209</v>
       </c>
     </row>
     <row r="88">
@@ -28189,19 +28189,19 @@
         <v>0.763</v>
       </c>
       <c r="B88" t="n">
-        <v>5.0689</v>
+        <v>5.1267</v>
       </c>
       <c r="C88" t="n">
-        <v>-37.7777</v>
+        <v>-38.6618</v>
       </c>
       <c r="D88" t="n">
-        <v>0.1416</v>
+        <v>0.14</v>
       </c>
       <c r="E88" t="n">
-        <v>16.8659</v>
+        <v>17.0556</v>
       </c>
       <c r="F88" t="n">
-        <v>-15.8659</v>
+        <v>-16.0556</v>
       </c>
     </row>
     <row r="89">
@@ -28209,19 +28209,19 @@
         <v>0.7786</v>
       </c>
       <c r="B89" t="n">
-        <v>5.2016</v>
+        <v>5.261</v>
       </c>
       <c r="C89" t="n">
-        <v>-39.8069</v>
+        <v>-40.7378</v>
       </c>
       <c r="D89" t="n">
-        <v>0.141</v>
+        <v>0.1394</v>
       </c>
       <c r="E89" t="n">
-        <v>17.3013</v>
+        <v>17.4959</v>
       </c>
       <c r="F89" t="n">
-        <v>-16.3013</v>
+        <v>-16.4959</v>
       </c>
     </row>
     <row r="90">
@@ -28229,19 +28229,19 @@
         <v>0.7944</v>
       </c>
       <c r="B90" t="n">
-        <v>5.3361</v>
+        <v>5.3969</v>
       </c>
       <c r="C90" t="n">
-        <v>-41.916</v>
+        <v>-42.8956</v>
       </c>
       <c r="D90" t="n">
-        <v>0.1404</v>
+        <v>0.1389</v>
       </c>
       <c r="E90" t="n">
-        <v>17.7422</v>
+        <v>17.9418</v>
       </c>
       <c r="F90" t="n">
-        <v>-16.7422</v>
+        <v>-16.9418</v>
       </c>
     </row>
     <row r="91">
@@ -28249,19 +28249,19 @@
         <v>0.8105</v>
       </c>
       <c r="B91" t="n">
-        <v>5.4722</v>
+        <v>5.5346</v>
       </c>
       <c r="C91" t="n">
-        <v>-44.1071</v>
+        <v>-45.1372</v>
       </c>
       <c r="D91" t="n">
-        <v>0.1399</v>
+        <v>0.1383</v>
       </c>
       <c r="E91" t="n">
-        <v>18.1887</v>
+        <v>18.3934</v>
       </c>
       <c r="F91" t="n">
-        <v>-17.1887</v>
+        <v>-17.3934</v>
       </c>
     </row>
     <row r="92">
@@ -28269,19 +28269,19 @@
         <v>0.8267</v>
       </c>
       <c r="B92" t="n">
-        <v>5.61</v>
+        <v>5.674</v>
       </c>
       <c r="C92" t="n">
-        <v>-46.3823</v>
+        <v>-47.4647</v>
       </c>
       <c r="D92" t="n">
-        <v>0.1393</v>
+        <v>0.1378</v>
       </c>
       <c r="E92" t="n">
-        <v>18.6408</v>
+        <v>18.8506</v>
       </c>
       <c r="F92" t="n">
-        <v>-17.6408</v>
+        <v>-17.8506</v>
       </c>
     </row>
     <row r="93">
@@ -28289,19 +28289,19 @@
         <v>0.8431</v>
       </c>
       <c r="B93" t="n">
-        <v>5.7496</v>
+        <v>5.8151</v>
       </c>
       <c r="C93" t="n">
-        <v>-48.7436</v>
+        <v>-49.8804</v>
       </c>
       <c r="D93" t="n">
-        <v>0.1388</v>
+        <v>0.1372</v>
       </c>
       <c r="E93" t="n">
-        <v>19.0985</v>
+        <v>19.3134</v>
       </c>
       <c r="F93" t="n">
-        <v>-18.0985</v>
+        <v>-18.3134</v>
       </c>
     </row>
     <row r="94">
@@ -28309,19 +28309,19 @@
         <v>0.8598</v>
       </c>
       <c r="B94" t="n">
-        <v>5.8908</v>
+        <v>5.958</v>
       </c>
       <c r="C94" t="n">
-        <v>-51.1932</v>
+        <v>-52.3865</v>
       </c>
       <c r="D94" t="n">
-        <v>0.1383</v>
+        <v>0.1368</v>
       </c>
       <c r="E94" t="n">
-        <v>19.5617</v>
+        <v>19.7819</v>
       </c>
       <c r="F94" t="n">
-        <v>-18.5617</v>
+        <v>-18.7819</v>
       </c>
     </row>
     <row r="95">
@@ -28329,19 +28329,19 @@
         <v>0.8766</v>
       </c>
       <c r="B95" t="n">
-        <v>6.0338</v>
+        <v>6.1025</v>
       </c>
       <c r="C95" t="n">
-        <v>-53.7333</v>
+        <v>-54.9851</v>
       </c>
       <c r="D95" t="n">
-        <v>0.1378</v>
+        <v>0.1363</v>
       </c>
       <c r="E95" t="n">
-        <v>20.0305</v>
+        <v>20.256</v>
       </c>
       <c r="F95" t="n">
-        <v>-19.0305</v>
+        <v>-19.256</v>
       </c>
     </row>
     <row r="96">
@@ -28349,39 +28349,39 @@
         <v>0.8935999999999999</v>
       </c>
       <c r="B96" t="n">
-        <v>6.1784</v>
+        <v>6.2488</v>
       </c>
       <c r="C96" t="n">
-        <v>-56.3661</v>
+        <v>-57.6784</v>
       </c>
       <c r="D96" t="n">
-        <v>0.1374</v>
+        <v>0.1358</v>
       </c>
       <c r="E96" t="n">
-        <v>20.5048</v>
+        <v>20.7357</v>
       </c>
       <c r="F96" t="n">
-        <v>-19.5048</v>
+        <v>-19.7357</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>0.9109</v>
+        <v>0.9108000000000001</v>
       </c>
       <c r="B97" t="n">
-        <v>6.3248</v>
+        <v>6.3969</v>
       </c>
       <c r="C97" t="n">
-        <v>-59.0937</v>
+        <v>-60.4688</v>
       </c>
       <c r="D97" t="n">
-        <v>0.1369</v>
+        <v>0.1354</v>
       </c>
       <c r="E97" t="n">
-        <v>20.9848</v>
+        <v>21.2211</v>
       </c>
       <c r="F97" t="n">
-        <v>-19.9848</v>
+        <v>-20.2211</v>
       </c>
     </row>
     <row r="98">
@@ -28389,19 +28389,19 @@
         <v>0.9283</v>
       </c>
       <c r="B98" t="n">
-        <v>6.4729</v>
+        <v>6.5466</v>
       </c>
       <c r="C98" t="n">
-        <v>-61.9185</v>
+        <v>-63.3586</v>
       </c>
       <c r="D98" t="n">
-        <v>0.1365</v>
+        <v>0.1349</v>
       </c>
       <c r="E98" t="n">
-        <v>21.4703</v>
+        <v>21.7121</v>
       </c>
       <c r="F98" t="n">
-        <v>-20.4703</v>
+        <v>-20.7121</v>
       </c>
     </row>
     <row r="99">
@@ -28409,19 +28409,19 @@
         <v>0.9459</v>
       </c>
       <c r="B99" t="n">
-        <v>6.6226</v>
+        <v>6.6981</v>
       </c>
       <c r="C99" t="n">
-        <v>-64.8426</v>
+        <v>-66.34999999999999</v>
       </c>
       <c r="D99" t="n">
-        <v>0.136</v>
+        <v>0.1345</v>
       </c>
       <c r="E99" t="n">
-        <v>21.9613</v>
+        <v>22.2087</v>
       </c>
       <c r="F99" t="n">
-        <v>-20.9613</v>
+        <v>-21.2087</v>
       </c>
     </row>
     <row r="100">
@@ -28429,19 +28429,19 @@
         <v>0.9637</v>
       </c>
       <c r="B100" t="n">
-        <v>6.7741</v>
+        <v>6.8512</v>
       </c>
       <c r="C100" t="n">
-        <v>-67.86839999999999</v>
+        <v>-69.4453</v>
       </c>
       <c r="D100" t="n">
-        <v>0.1356</v>
+        <v>0.1341</v>
       </c>
       <c r="E100" t="n">
-        <v>22.458</v>
+        <v>22.711</v>
       </c>
       <c r="F100" t="n">
-        <v>-21.458</v>
+        <v>-21.711</v>
       </c>
     </row>
     <row r="101">
@@ -28449,19 +28449,19 @@
         <v>0.9818</v>
       </c>
       <c r="B101" t="n">
-        <v>6.9272</v>
+        <v>7.0061</v>
       </c>
       <c r="C101" t="n">
-        <v>-70.9982</v>
+        <v>-72.64709999999999</v>
       </c>
       <c r="D101" t="n">
-        <v>0.1352</v>
+        <v>0.1337</v>
       </c>
       <c r="E101" t="n">
-        <v>22.9602</v>
+        <v>23.2189</v>
       </c>
       <c r="F101" t="n">
-        <v>-21.9602</v>
+        <v>-22.2189</v>
       </c>
     </row>
     <row r="102">
@@ -28469,19 +28469,19 @@
         <v>1</v>
       </c>
       <c r="B102" t="n">
-        <v>7.0821</v>
+        <v>7.1628</v>
       </c>
       <c r="C102" t="n">
-        <v>-74.23439999999999</v>
+        <v>-75.9576</v>
       </c>
       <c r="D102" t="n">
-        <v>0.1348</v>
+        <v>0.1333</v>
       </c>
       <c r="E102" t="n">
-        <v>23.468</v>
+        <v>23.7324</v>
       </c>
       <c r="F102" t="n">
-        <v>-22.468</v>
+        <v>-22.7324</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
strated on an effective validation method for the frontend
</commit_message>
<xml_diff>
--- a/pythonCW/230023476PortfolioProblem.xlsx
+++ b/pythonCW/230023476PortfolioProblem.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="input" sheetId="1" state="visible" r:id="rId1"/>
@@ -78,10 +78,10 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -464,7 +464,7 @@
   </sheetPr>
   <dimension ref="A1:M122"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A122"/>
     </sheetView>
   </sheetViews>
@@ -541,7 +541,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="n">
+      <c r="A2" s="1" t="n">
         <v>41821</v>
       </c>
       <c r="B2" t="n">
@@ -582,7 +582,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="n">
+      <c r="A3" s="1" t="n">
         <v>41852</v>
       </c>
       <c r="B3" t="n">
@@ -623,7 +623,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="n">
+      <c r="A4" s="1" t="n">
         <v>41883</v>
       </c>
       <c r="B4" t="n">
@@ -664,7 +664,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="n">
+      <c r="A5" s="1" t="n">
         <v>41913</v>
       </c>
       <c r="B5" t="n">
@@ -705,7 +705,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="2" t="n">
+      <c r="A6" s="1" t="n">
         <v>41944</v>
       </c>
       <c r="B6" t="n">
@@ -746,7 +746,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="2" t="n">
+      <c r="A7" s="1" t="n">
         <v>41974</v>
       </c>
       <c r="B7" t="n">
@@ -787,7 +787,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="2" t="n">
+      <c r="A8" s="1" t="n">
         <v>42005</v>
       </c>
       <c r="B8" t="n">
@@ -828,7 +828,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="2" t="n">
+      <c r="A9" s="1" t="n">
         <v>42036</v>
       </c>
       <c r="B9" t="n">
@@ -869,7 +869,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="2" t="n">
+      <c r="A10" s="1" t="n">
         <v>42064</v>
       </c>
       <c r="B10" t="n">
@@ -910,7 +910,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="2" t="n">
+      <c r="A11" s="1" t="n">
         <v>42095</v>
       </c>
       <c r="B11" t="n">
@@ -951,7 +951,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="2" t="n">
+      <c r="A12" s="1" t="n">
         <v>42125</v>
       </c>
       <c r="B12" t="n">
@@ -992,7 +992,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="2" t="n">
+      <c r="A13" s="1" t="n">
         <v>42156</v>
       </c>
       <c r="B13" t="n">
@@ -1033,7 +1033,7 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="2" t="n">
+      <c r="A14" s="1" t="n">
         <v>42186</v>
       </c>
       <c r="B14" t="n">
@@ -1074,7 +1074,7 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="2" t="n">
+      <c r="A15" s="1" t="n">
         <v>42217</v>
       </c>
       <c r="B15" t="n">
@@ -1115,7 +1115,7 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="2" t="n">
+      <c r="A16" s="1" t="n">
         <v>42248</v>
       </c>
       <c r="B16" t="n">
@@ -1156,7 +1156,7 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="2" t="n">
+      <c r="A17" s="1" t="n">
         <v>42278</v>
       </c>
       <c r="B17" t="n">
@@ -1197,7 +1197,7 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="2" t="n">
+      <c r="A18" s="1" t="n">
         <v>42309</v>
       </c>
       <c r="B18" t="n">
@@ -1238,7 +1238,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="2" t="n">
+      <c r="A19" s="1" t="n">
         <v>42339</v>
       </c>
       <c r="B19" t="n">
@@ -1279,7 +1279,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="2" t="n">
+      <c r="A20" s="1" t="n">
         <v>42370</v>
       </c>
       <c r="B20" t="n">
@@ -1320,7 +1320,7 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="2" t="n">
+      <c r="A21" s="1" t="n">
         <v>42401</v>
       </c>
       <c r="B21" t="n">
@@ -1361,7 +1361,7 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="2" t="n">
+      <c r="A22" s="1" t="n">
         <v>42430</v>
       </c>
       <c r="B22" t="n">
@@ -1402,7 +1402,7 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="2" t="n">
+      <c r="A23" s="1" t="n">
         <v>42461</v>
       </c>
       <c r="B23" t="n">
@@ -1443,7 +1443,7 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="2" t="n">
+      <c r="A24" s="1" t="n">
         <v>42491</v>
       </c>
       <c r="B24" t="n">
@@ -1484,7 +1484,7 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="2" t="n">
+      <c r="A25" s="1" t="n">
         <v>42522</v>
       </c>
       <c r="B25" t="n">
@@ -1525,7 +1525,7 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="2" t="n">
+      <c r="A26" s="1" t="n">
         <v>42552</v>
       </c>
       <c r="B26" t="n">
@@ -1566,7 +1566,7 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="2" t="n">
+      <c r="A27" s="1" t="n">
         <v>42583</v>
       </c>
       <c r="B27" t="n">
@@ -1607,7 +1607,7 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="2" t="n">
+      <c r="A28" s="1" t="n">
         <v>42614</v>
       </c>
       <c r="B28" t="n">
@@ -1648,7 +1648,7 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="2" t="n">
+      <c r="A29" s="1" t="n">
         <v>42644</v>
       </c>
       <c r="B29" t="n">
@@ -1689,7 +1689,7 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="2" t="n">
+      <c r="A30" s="1" t="n">
         <v>42675</v>
       </c>
       <c r="B30" t="n">
@@ -1730,7 +1730,7 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="2" t="n">
+      <c r="A31" s="1" t="n">
         <v>42705</v>
       </c>
       <c r="B31" t="n">
@@ -1771,7 +1771,7 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="2" t="n">
+      <c r="A32" s="1" t="n">
         <v>42736</v>
       </c>
       <c r="B32" t="n">
@@ -1812,7 +1812,7 @@
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="2" t="n">
+      <c r="A33" s="1" t="n">
         <v>42767</v>
       </c>
       <c r="B33" t="n">
@@ -1853,7 +1853,7 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="2" t="n">
+      <c r="A34" s="1" t="n">
         <v>42795</v>
       </c>
       <c r="B34" t="n">
@@ -1894,7 +1894,7 @@
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="2" t="n">
+      <c r="A35" s="1" t="n">
         <v>42826</v>
       </c>
       <c r="B35" t="n">
@@ -1935,7 +1935,7 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="2" t="n">
+      <c r="A36" s="1" t="n">
         <v>42856</v>
       </c>
       <c r="B36" t="n">
@@ -1976,7 +1976,7 @@
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="2" t="n">
+      <c r="A37" s="1" t="n">
         <v>42887</v>
       </c>
       <c r="B37" t="n">
@@ -2017,7 +2017,7 @@
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="2" t="n">
+      <c r="A38" s="1" t="n">
         <v>42917</v>
       </c>
       <c r="B38" t="n">
@@ -2058,7 +2058,7 @@
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="2" t="n">
+      <c r="A39" s="1" t="n">
         <v>42948</v>
       </c>
       <c r="B39" t="n">
@@ -2099,7 +2099,7 @@
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="2" t="n">
+      <c r="A40" s="1" t="n">
         <v>42979</v>
       </c>
       <c r="B40" t="n">
@@ -2140,7 +2140,7 @@
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="2" t="n">
+      <c r="A41" s="1" t="n">
         <v>43009</v>
       </c>
       <c r="B41" t="n">
@@ -2181,7 +2181,7 @@
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="2" t="n">
+      <c r="A42" s="1" t="n">
         <v>43040</v>
       </c>
       <c r="B42" t="n">
@@ -2222,7 +2222,7 @@
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="2" t="n">
+      <c r="A43" s="1" t="n">
         <v>43070</v>
       </c>
       <c r="B43" t="n">
@@ -2263,7 +2263,7 @@
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="2" t="n">
+      <c r="A44" s="1" t="n">
         <v>43101</v>
       </c>
       <c r="B44" t="n">
@@ -2304,7 +2304,7 @@
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="2" t="n">
+      <c r="A45" s="1" t="n">
         <v>43132</v>
       </c>
       <c r="B45" t="n">
@@ -2345,7 +2345,7 @@
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="2" t="n">
+      <c r="A46" s="1" t="n">
         <v>43160</v>
       </c>
       <c r="B46" t="n">
@@ -2386,7 +2386,7 @@
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="2" t="n">
+      <c r="A47" s="1" t="n">
         <v>43191</v>
       </c>
       <c r="B47" t="n">
@@ -2427,7 +2427,7 @@
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="2" t="n">
+      <c r="A48" s="1" t="n">
         <v>43221</v>
       </c>
       <c r="B48" t="n">
@@ -2468,7 +2468,7 @@
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="2" t="n">
+      <c r="A49" s="1" t="n">
         <v>43252</v>
       </c>
       <c r="B49" t="n">
@@ -2509,7 +2509,7 @@
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="2" t="n">
+      <c r="A50" s="1" t="n">
         <v>43282</v>
       </c>
       <c r="B50" t="n">
@@ -2550,7 +2550,7 @@
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="2" t="n">
+      <c r="A51" s="1" t="n">
         <v>43313</v>
       </c>
       <c r="B51" t="n">
@@ -2591,7 +2591,7 @@
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="2" t="n">
+      <c r="A52" s="1" t="n">
         <v>43344</v>
       </c>
       <c r="B52" t="n">
@@ -2632,7 +2632,7 @@
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="2" t="n">
+      <c r="A53" s="1" t="n">
         <v>43374</v>
       </c>
       <c r="B53" t="n">
@@ -2673,7 +2673,7 @@
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="2" t="n">
+      <c r="A54" s="1" t="n">
         <v>43405</v>
       </c>
       <c r="B54" t="n">
@@ -2714,7 +2714,7 @@
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="2" t="n">
+      <c r="A55" s="1" t="n">
         <v>43435</v>
       </c>
       <c r="B55" t="n">
@@ -2755,7 +2755,7 @@
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="2" t="n">
+      <c r="A56" s="1" t="n">
         <v>43466</v>
       </c>
       <c r="B56" t="n">
@@ -2796,7 +2796,7 @@
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="2" t="n">
+      <c r="A57" s="1" t="n">
         <v>43497</v>
       </c>
       <c r="B57" t="n">
@@ -2837,7 +2837,7 @@
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="2" t="n">
+      <c r="A58" s="1" t="n">
         <v>43525</v>
       </c>
       <c r="B58" t="n">
@@ -2878,7 +2878,7 @@
       </c>
     </row>
     <row r="59">
-      <c r="A59" s="2" t="n">
+      <c r="A59" s="1" t="n">
         <v>43556</v>
       </c>
       <c r="B59" t="n">
@@ -2919,7 +2919,7 @@
       </c>
     </row>
     <row r="60">
-      <c r="A60" s="2" t="n">
+      <c r="A60" s="1" t="n">
         <v>43586</v>
       </c>
       <c r="B60" t="n">
@@ -2960,7 +2960,7 @@
       </c>
     </row>
     <row r="61">
-      <c r="A61" s="2" t="n">
+      <c r="A61" s="1" t="n">
         <v>43617</v>
       </c>
       <c r="B61" t="n">
@@ -3001,7 +3001,7 @@
       </c>
     </row>
     <row r="62">
-      <c r="A62" s="2" t="n">
+      <c r="A62" s="1" t="n">
         <v>43647</v>
       </c>
       <c r="B62" t="n">
@@ -3042,7 +3042,7 @@
       </c>
     </row>
     <row r="63">
-      <c r="A63" s="2" t="n">
+      <c r="A63" s="1" t="n">
         <v>43678</v>
       </c>
       <c r="B63" t="n">
@@ -3083,7 +3083,7 @@
       </c>
     </row>
     <row r="64">
-      <c r="A64" s="2" t="n">
+      <c r="A64" s="1" t="n">
         <v>43709</v>
       </c>
       <c r="B64" t="n">
@@ -3124,7 +3124,7 @@
       </c>
     </row>
     <row r="65">
-      <c r="A65" s="2" t="n">
+      <c r="A65" s="1" t="n">
         <v>43739</v>
       </c>
       <c r="B65" t="n">
@@ -3165,7 +3165,7 @@
       </c>
     </row>
     <row r="66">
-      <c r="A66" s="2" t="n">
+      <c r="A66" s="1" t="n">
         <v>43770</v>
       </c>
       <c r="B66" t="n">
@@ -3206,7 +3206,7 @@
       </c>
     </row>
     <row r="67">
-      <c r="A67" s="2" t="n">
+      <c r="A67" s="1" t="n">
         <v>43800</v>
       </c>
       <c r="B67" t="n">
@@ -3247,7 +3247,7 @@
       </c>
     </row>
     <row r="68">
-      <c r="A68" s="2" t="n">
+      <c r="A68" s="1" t="n">
         <v>43831</v>
       </c>
       <c r="B68" t="n">
@@ -3288,7 +3288,7 @@
       </c>
     </row>
     <row r="69">
-      <c r="A69" s="2" t="n">
+      <c r="A69" s="1" t="n">
         <v>43862</v>
       </c>
       <c r="B69" t="n">
@@ -3329,7 +3329,7 @@
       </c>
     </row>
     <row r="70">
-      <c r="A70" s="2" t="n">
+      <c r="A70" s="1" t="n">
         <v>43891</v>
       </c>
       <c r="B70" t="n">
@@ -3370,7 +3370,7 @@
       </c>
     </row>
     <row r="71">
-      <c r="A71" s="2" t="n">
+      <c r="A71" s="1" t="n">
         <v>43922</v>
       </c>
       <c r="B71" t="n">
@@ -3411,7 +3411,7 @@
       </c>
     </row>
     <row r="72">
-      <c r="A72" s="2" t="n">
+      <c r="A72" s="1" t="n">
         <v>43952</v>
       </c>
       <c r="B72" t="n">
@@ -3452,7 +3452,7 @@
       </c>
     </row>
     <row r="73">
-      <c r="A73" s="2" t="n">
+      <c r="A73" s="1" t="n">
         <v>43983</v>
       </c>
       <c r="B73" t="n">
@@ -3493,7 +3493,7 @@
       </c>
     </row>
     <row r="74">
-      <c r="A74" s="2" t="n">
+      <c r="A74" s="1" t="n">
         <v>44013</v>
       </c>
       <c r="B74" t="n">
@@ -3534,7 +3534,7 @@
       </c>
     </row>
     <row r="75">
-      <c r="A75" s="2" t="n">
+      <c r="A75" s="1" t="n">
         <v>44044</v>
       </c>
       <c r="B75" t="n">
@@ -3575,7 +3575,7 @@
       </c>
     </row>
     <row r="76">
-      <c r="A76" s="2" t="n">
+      <c r="A76" s="1" t="n">
         <v>44075</v>
       </c>
       <c r="B76" t="n">
@@ -3616,7 +3616,7 @@
       </c>
     </row>
     <row r="77">
-      <c r="A77" s="2" t="n">
+      <c r="A77" s="1" t="n">
         <v>44105</v>
       </c>
       <c r="B77" t="n">
@@ -3657,7 +3657,7 @@
       </c>
     </row>
     <row r="78">
-      <c r="A78" s="2" t="n">
+      <c r="A78" s="1" t="n">
         <v>44136</v>
       </c>
       <c r="B78" t="n">
@@ -3698,7 +3698,7 @@
       </c>
     </row>
     <row r="79">
-      <c r="A79" s="2" t="n">
+      <c r="A79" s="1" t="n">
         <v>44166</v>
       </c>
       <c r="B79" t="n">
@@ -3739,7 +3739,7 @@
       </c>
     </row>
     <row r="80">
-      <c r="A80" s="2" t="n">
+      <c r="A80" s="1" t="n">
         <v>44197</v>
       </c>
       <c r="B80" t="n">
@@ -3780,7 +3780,7 @@
       </c>
     </row>
     <row r="81">
-      <c r="A81" s="2" t="n">
+      <c r="A81" s="1" t="n">
         <v>44228</v>
       </c>
       <c r="B81" t="n">
@@ -3821,7 +3821,7 @@
       </c>
     </row>
     <row r="82">
-      <c r="A82" s="2" t="n">
+      <c r="A82" s="1" t="n">
         <v>44256</v>
       </c>
       <c r="B82" t="n">
@@ -3862,7 +3862,7 @@
       </c>
     </row>
     <row r="83">
-      <c r="A83" s="2" t="n">
+      <c r="A83" s="1" t="n">
         <v>44287</v>
       </c>
       <c r="B83" t="n">
@@ -3903,7 +3903,7 @@
       </c>
     </row>
     <row r="84">
-      <c r="A84" s="2" t="n">
+      <c r="A84" s="1" t="n">
         <v>44317</v>
       </c>
       <c r="B84" t="n">
@@ -3944,7 +3944,7 @@
       </c>
     </row>
     <row r="85">
-      <c r="A85" s="2" t="n">
+      <c r="A85" s="1" t="n">
         <v>44348</v>
       </c>
       <c r="B85" t="n">
@@ -3985,7 +3985,7 @@
       </c>
     </row>
     <row r="86">
-      <c r="A86" s="2" t="n">
+      <c r="A86" s="1" t="n">
         <v>44378</v>
       </c>
       <c r="B86" t="n">
@@ -4026,7 +4026,7 @@
       </c>
     </row>
     <row r="87">
-      <c r="A87" s="2" t="n">
+      <c r="A87" s="1" t="n">
         <v>44409</v>
       </c>
       <c r="B87" t="n">
@@ -4067,7 +4067,7 @@
       </c>
     </row>
     <row r="88">
-      <c r="A88" s="2" t="n">
+      <c r="A88" s="1" t="n">
         <v>44440</v>
       </c>
       <c r="B88" t="n">
@@ -4108,7 +4108,7 @@
       </c>
     </row>
     <row r="89">
-      <c r="A89" s="2" t="n">
+      <c r="A89" s="1" t="n">
         <v>44470</v>
       </c>
       <c r="B89" t="n">
@@ -4149,7 +4149,7 @@
       </c>
     </row>
     <row r="90">
-      <c r="A90" s="2" t="n">
+      <c r="A90" s="1" t="n">
         <v>44501</v>
       </c>
       <c r="B90" t="n">
@@ -4190,7 +4190,7 @@
       </c>
     </row>
     <row r="91">
-      <c r="A91" s="2" t="n">
+      <c r="A91" s="1" t="n">
         <v>44531</v>
       </c>
       <c r="B91" t="n">
@@ -4231,7 +4231,7 @@
       </c>
     </row>
     <row r="92">
-      <c r="A92" s="2" t="n">
+      <c r="A92" s="1" t="n">
         <v>44562</v>
       </c>
       <c r="B92" t="n">
@@ -4272,7 +4272,7 @@
       </c>
     </row>
     <row r="93">
-      <c r="A93" s="2" t="n">
+      <c r="A93" s="1" t="n">
         <v>44593</v>
       </c>
       <c r="B93" t="n">
@@ -4313,7 +4313,7 @@
       </c>
     </row>
     <row r="94">
-      <c r="A94" s="2" t="n">
+      <c r="A94" s="1" t="n">
         <v>44621</v>
       </c>
       <c r="B94" t="n">
@@ -4354,7 +4354,7 @@
       </c>
     </row>
     <row r="95">
-      <c r="A95" s="2" t="n">
+      <c r="A95" s="1" t="n">
         <v>44652</v>
       </c>
       <c r="B95" t="n">
@@ -4395,7 +4395,7 @@
       </c>
     </row>
     <row r="96">
-      <c r="A96" s="2" t="n">
+      <c r="A96" s="1" t="n">
         <v>44682</v>
       </c>
       <c r="B96" t="n">
@@ -4436,7 +4436,7 @@
       </c>
     </row>
     <row r="97">
-      <c r="A97" s="2" t="n">
+      <c r="A97" s="1" t="n">
         <v>44713</v>
       </c>
       <c r="B97" t="n">
@@ -4477,7 +4477,7 @@
       </c>
     </row>
     <row r="98">
-      <c r="A98" s="2" t="n">
+      <c r="A98" s="1" t="n">
         <v>44743</v>
       </c>
       <c r="B98" t="n">
@@ -4518,7 +4518,7 @@
       </c>
     </row>
     <row r="99">
-      <c r="A99" s="2" t="n">
+      <c r="A99" s="1" t="n">
         <v>44774</v>
       </c>
       <c r="B99" t="n">
@@ -4559,7 +4559,7 @@
       </c>
     </row>
     <row r="100">
-      <c r="A100" s="2" t="n">
+      <c r="A100" s="1" t="n">
         <v>44805</v>
       </c>
       <c r="B100" t="n">
@@ -4600,7 +4600,7 @@
       </c>
     </row>
     <row r="101">
-      <c r="A101" s="2" t="n">
+      <c r="A101" s="1" t="n">
         <v>44835</v>
       </c>
       <c r="B101" t="n">
@@ -4641,7 +4641,7 @@
       </c>
     </row>
     <row r="102">
-      <c r="A102" s="2" t="n">
+      <c r="A102" s="1" t="n">
         <v>44866</v>
       </c>
       <c r="B102" t="n">
@@ -4682,7 +4682,7 @@
       </c>
     </row>
     <row r="103">
-      <c r="A103" s="2" t="n">
+      <c r="A103" s="1" t="n">
         <v>44896</v>
       </c>
       <c r="B103" t="n">
@@ -4723,7 +4723,7 @@
       </c>
     </row>
     <row r="104">
-      <c r="A104" s="2" t="n">
+      <c r="A104" s="1" t="n">
         <v>44927</v>
       </c>
       <c r="B104" t="n">
@@ -4764,7 +4764,7 @@
       </c>
     </row>
     <row r="105">
-      <c r="A105" s="2" t="n">
+      <c r="A105" s="1" t="n">
         <v>44958</v>
       </c>
       <c r="B105" t="n">
@@ -4805,7 +4805,7 @@
       </c>
     </row>
     <row r="106">
-      <c r="A106" s="2" t="n">
+      <c r="A106" s="1" t="n">
         <v>44986</v>
       </c>
       <c r="B106" t="n">
@@ -4846,7 +4846,7 @@
       </c>
     </row>
     <row r="107">
-      <c r="A107" s="2" t="n">
+      <c r="A107" s="1" t="n">
         <v>45017</v>
       </c>
       <c r="B107" t="n">
@@ -4887,7 +4887,7 @@
       </c>
     </row>
     <row r="108">
-      <c r="A108" s="2" t="n">
+      <c r="A108" s="1" t="n">
         <v>45047</v>
       </c>
       <c r="B108" t="n">
@@ -4928,7 +4928,7 @@
       </c>
     </row>
     <row r="109">
-      <c r="A109" s="2" t="n">
+      <c r="A109" s="1" t="n">
         <v>45078</v>
       </c>
       <c r="B109" t="n">
@@ -4969,7 +4969,7 @@
       </c>
     </row>
     <row r="110">
-      <c r="A110" s="2" t="n">
+      <c r="A110" s="1" t="n">
         <v>45108</v>
       </c>
       <c r="B110" t="n">
@@ -5010,7 +5010,7 @@
       </c>
     </row>
     <row r="111">
-      <c r="A111" s="2" t="n">
+      <c r="A111" s="1" t="n">
         <v>45139</v>
       </c>
       <c r="B111" t="n">
@@ -5051,7 +5051,7 @@
       </c>
     </row>
     <row r="112">
-      <c r="A112" s="2" t="n">
+      <c r="A112" s="1" t="n">
         <v>45170</v>
       </c>
       <c r="B112" t="n">
@@ -5092,7 +5092,7 @@
       </c>
     </row>
     <row r="113">
-      <c r="A113" s="2" t="n">
+      <c r="A113" s="1" t="n">
         <v>45200</v>
       </c>
       <c r="B113" t="n">
@@ -5133,7 +5133,7 @@
       </c>
     </row>
     <row r="114">
-      <c r="A114" s="2" t="n">
+      <c r="A114" s="1" t="n">
         <v>45231</v>
       </c>
       <c r="B114" t="n">
@@ -5174,7 +5174,7 @@
       </c>
     </row>
     <row r="115">
-      <c r="A115" s="2" t="n">
+      <c r="A115" s="1" t="n">
         <v>45261</v>
       </c>
       <c r="B115" t="n">
@@ -5215,7 +5215,7 @@
       </c>
     </row>
     <row r="116">
-      <c r="A116" s="2" t="n">
+      <c r="A116" s="1" t="n">
         <v>45292</v>
       </c>
       <c r="B116" t="n">
@@ -5256,7 +5256,7 @@
       </c>
     </row>
     <row r="117">
-      <c r="A117" s="2" t="n">
+      <c r="A117" s="1" t="n">
         <v>45323</v>
       </c>
       <c r="B117" t="n">
@@ -5297,7 +5297,7 @@
       </c>
     </row>
     <row r="118">
-      <c r="A118" s="2" t="n">
+      <c r="A118" s="1" t="n">
         <v>45352</v>
       </c>
       <c r="B118" t="n">
@@ -5338,7 +5338,7 @@
       </c>
     </row>
     <row r="119">
-      <c r="A119" s="2" t="n">
+      <c r="A119" s="1" t="n">
         <v>45383</v>
       </c>
       <c r="B119" t="n">
@@ -5379,7 +5379,7 @@
       </c>
     </row>
     <row r="120">
-      <c r="A120" s="2" t="n">
+      <c r="A120" s="1" t="n">
         <v>45413</v>
       </c>
       <c r="B120" t="n">
@@ -5420,7 +5420,7 @@
       </c>
     </row>
     <row r="121">
-      <c r="A121" s="2" t="n">
+      <c r="A121" s="1" t="n">
         <v>45444</v>
       </c>
       <c r="B121" t="n">
@@ -5461,7 +5461,7 @@
       </c>
     </row>
     <row r="122">
-      <c r="A122" s="2" t="n">
+      <c r="A122" s="1" t="n">
         <v>45471</v>
       </c>
       <c r="B122" t="n">
@@ -5522,11 +5522,11 @@
   <cols>
     <col width="9.6" customWidth="1" min="1" max="1"/>
     <col width="14.4" customWidth="1" min="2" max="2"/>
-    <col width="10.8" customWidth="1" min="3" max="3"/>
-    <col width="16.8" customWidth="1" min="4" max="4"/>
-    <col width="9.6" customWidth="1" min="5" max="5"/>
-    <col width="9.6" customWidth="1" min="6" max="6"/>
-    <col width="9.6" customWidth="1" min="7" max="7"/>
+    <col width="16.8" customWidth="1" min="3" max="3"/>
+    <col width="10.8" customWidth="1" min="4" max="4"/>
+    <col width="4.8" customWidth="1" min="5" max="5"/>
+    <col width="4.8" customWidth="1" min="6" max="6"/>
+    <col width="4.8" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -5542,2328 +5542,2328 @@
       </c>
       <c r="C1" s="3" t="inlineStr">
         <is>
+          <t>Sharpe Ratio</t>
+        </is>
+      </c>
+      <c r="D1" s="3" t="inlineStr">
+        <is>
           <t>Utility</t>
         </is>
       </c>
-      <c r="D1" s="3" t="inlineStr">
-        <is>
-          <t>Sharpe Ratio</t>
-        </is>
-      </c>
       <c r="E1" s="3" t="inlineStr">
         <is>
-          <t>w_NVDA</t>
+          <t>w1</t>
         </is>
       </c>
       <c r="F1" s="3" t="inlineStr">
         <is>
-          <t>w_MSFT</t>
+          <t>w2</t>
         </is>
       </c>
       <c r="G1" s="3" t="inlineStr">
         <is>
-          <t>w_AAPL</t>
+          <t>w3</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.2105</v>
+        <v>0.1472</v>
       </c>
       <c r="B2" t="n">
-        <v>0.2061</v>
+        <v>0.1461</v>
       </c>
       <c r="C2" t="n">
-        <v>0.1468</v>
+        <v>0.6992</v>
       </c>
       <c r="D2" t="n">
-        <v>0.803</v>
+        <v>0.1045</v>
       </c>
       <c r="E2" t="n">
-        <v>-0.1408</v>
+        <v>-0.1052</v>
       </c>
       <c r="F2" t="n">
-        <v>0.8631</v>
+        <v>0.2323</v>
       </c>
       <c r="G2" t="n">
-        <v>0.2777</v>
+        <v>0.8729</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0.2106</v>
+        <v>0.1472</v>
       </c>
       <c r="B3" t="n">
-        <v>0.2061</v>
+        <v>0.1461</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1469</v>
+        <v>0.6996</v>
       </c>
       <c r="D3" t="n">
-        <v>0.8033</v>
+        <v>0.1045</v>
       </c>
       <c r="E3" t="n">
-        <v>-0.1406</v>
+        <v>-0.1045</v>
       </c>
       <c r="F3" t="n">
-        <v>0.8631</v>
+        <v>0.2322</v>
       </c>
       <c r="G3" t="n">
-        <v>0.2776</v>
+        <v>0.8723</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0.2107</v>
+        <v>0.1473</v>
       </c>
       <c r="B4" t="n">
-        <v>0.2061</v>
+        <v>0.1459</v>
       </c>
       <c r="C4" t="n">
-        <v>0.1469</v>
+        <v>0.7017</v>
       </c>
       <c r="D4" t="n">
-        <v>0.8036</v>
+        <v>0.1048</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.1405</v>
+        <v>-0.1012</v>
       </c>
       <c r="F4" t="n">
-        <v>0.863</v>
+        <v>0.2319</v>
       </c>
       <c r="G4" t="n">
-        <v>0.2775</v>
+        <v>0.8693</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0.2109</v>
+        <v>0.1474</v>
       </c>
       <c r="B5" t="n">
-        <v>0.2061</v>
+        <v>0.1457</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1471</v>
+        <v>0.7030999999999999</v>
       </c>
       <c r="D5" t="n">
-        <v>0.8047</v>
+        <v>0.105</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.1401</v>
+        <v>-0.09909999999999999</v>
       </c>
       <c r="F5" t="n">
-        <v>0.8628</v>
+        <v>0.2317</v>
       </c>
       <c r="G5" t="n">
-        <v>0.2772</v>
+        <v>0.8673999999999999</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0.211</v>
+        <v>0.1477</v>
       </c>
       <c r="B6" t="n">
-        <v>0.2061</v>
+        <v>0.1452</v>
       </c>
       <c r="C6" t="n">
-        <v>0.1473</v>
+        <v>0.7072000000000001</v>
       </c>
       <c r="D6" t="n">
-        <v>0.8053</v>
+        <v>0.1055</v>
       </c>
       <c r="E6" t="n">
-        <v>-0.1399</v>
+        <v>-0.0926</v>
       </c>
       <c r="F6" t="n">
-        <v>0.8628</v>
+        <v>0.2311</v>
       </c>
       <c r="G6" t="n">
-        <v>0.2771</v>
+        <v>0.8615</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0.2113</v>
+        <v>0.1479</v>
       </c>
       <c r="B7" t="n">
-        <v>0.2061</v>
+        <v>0.145</v>
       </c>
       <c r="C7" t="n">
-        <v>0.1476</v>
+        <v>0.7094</v>
       </c>
       <c r="D7" t="n">
-        <v>0.8070000000000001</v>
+        <v>0.1058</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.1392</v>
+        <v>-0.089</v>
       </c>
       <c r="F7" t="n">
-        <v>0.8625</v>
+        <v>0.2308</v>
       </c>
       <c r="G7" t="n">
-        <v>0.2767</v>
+        <v>0.8583</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>0.2115</v>
+        <v>0.1483</v>
       </c>
       <c r="B8" t="n">
-        <v>0.2061</v>
+        <v>0.1444</v>
       </c>
       <c r="C8" t="n">
-        <v>0.1478</v>
+        <v>0.7153</v>
       </c>
       <c r="D8" t="n">
-        <v>0.8079</v>
+        <v>0.1066</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.1388</v>
+        <v>-0.07920000000000001</v>
       </c>
       <c r="F8" t="n">
-        <v>0.8623</v>
+        <v>0.2299</v>
       </c>
       <c r="G8" t="n">
-        <v>0.2765</v>
+        <v>0.8494</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0.212</v>
+        <v>0.1485</v>
       </c>
       <c r="B9" t="n">
-        <v>0.2061</v>
+        <v>0.1441</v>
       </c>
       <c r="C9" t="n">
-        <v>0.1483</v>
+        <v>0.7183</v>
       </c>
       <c r="D9" t="n">
-        <v>0.8103</v>
+        <v>0.107</v>
       </c>
       <c r="E9" t="n">
-        <v>-0.1378</v>
+        <v>-0.0743</v>
       </c>
       <c r="F9" t="n">
-        <v>0.8619</v>
+        <v>0.2294</v>
       </c>
       <c r="G9" t="n">
-        <v>0.2759</v>
+        <v>0.8449</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>0.2122</v>
+        <v>0.1491</v>
       </c>
       <c r="B10" t="n">
-        <v>0.2061</v>
+        <v>0.1434</v>
       </c>
       <c r="C10" t="n">
-        <v>0.1485</v>
+        <v>0.7258</v>
       </c>
       <c r="D10" t="n">
-        <v>0.8115</v>
+        <v>0.1079</v>
       </c>
       <c r="E10" t="n">
-        <v>-0.1373</v>
+        <v>-0.0612</v>
       </c>
       <c r="F10" t="n">
-        <v>0.8617</v>
+        <v>0.2282</v>
       </c>
       <c r="G10" t="n">
-        <v>0.2756</v>
+        <v>0.833</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>0.2129</v>
+        <v>0.1493</v>
       </c>
       <c r="B11" t="n">
-        <v>0.2061</v>
+        <v>0.1431</v>
       </c>
       <c r="C11" t="n">
-        <v>0.1492</v>
+        <v>0.7292999999999999</v>
       </c>
       <c r="D11" t="n">
-        <v>0.8147</v>
+        <v>0.1084</v>
       </c>
       <c r="E11" t="n">
-        <v>-0.1361</v>
+        <v>-0.0548</v>
       </c>
       <c r="F11" t="n">
-        <v>0.8612</v>
+        <v>0.2276</v>
       </c>
       <c r="G11" t="n">
-        <v>0.2749</v>
+        <v>0.8272</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>0.2132</v>
+        <v>0.15</v>
       </c>
       <c r="B12" t="n">
-        <v>0.2061</v>
+        <v>0.1424</v>
       </c>
       <c r="C12" t="n">
-        <v>0.1495</v>
+        <v>0.7378</v>
       </c>
       <c r="D12" t="n">
-        <v>0.8161</v>
+        <v>0.1095</v>
       </c>
       <c r="E12" t="n">
-        <v>-0.1355</v>
+        <v>-0.0385</v>
       </c>
       <c r="F12" t="n">
-        <v>0.861</v>
+        <v>0.2261</v>
       </c>
       <c r="G12" t="n">
-        <v>0.2745</v>
+        <v>0.8124</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>0.2139</v>
+        <v>0.1504</v>
       </c>
       <c r="B13" t="n">
-        <v>0.206</v>
+        <v>0.1421</v>
       </c>
       <c r="C13" t="n">
-        <v>0.1503</v>
+        <v>0.7416</v>
       </c>
       <c r="D13" t="n">
-        <v>0.82</v>
+        <v>0.11</v>
       </c>
       <c r="E13" t="n">
-        <v>-0.1339</v>
+        <v>-0.0307</v>
       </c>
       <c r="F13" t="n">
-        <v>0.8603</v>
+        <v>0.2254</v>
       </c>
       <c r="G13" t="n">
-        <v>0.2736</v>
+        <v>0.8053</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>0.2143</v>
+        <v>0.1512</v>
       </c>
       <c r="B14" t="n">
-        <v>0.206</v>
+        <v>0.1415</v>
       </c>
       <c r="C14" t="n">
-        <v>0.1506</v>
+        <v>0.7506</v>
       </c>
       <c r="D14" t="n">
-        <v>0.8217</v>
+        <v>0.1112</v>
       </c>
       <c r="E14" t="n">
-        <v>-0.1332</v>
+        <v>-0.0111</v>
       </c>
       <c r="F14" t="n">
-        <v>0.86</v>
+        <v>0.2236</v>
       </c>
       <c r="G14" t="n">
-        <v>0.2732</v>
+        <v>0.7875</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>0.2152</v>
+        <v>0.1516</v>
       </c>
       <c r="B15" t="n">
-        <v>0.206</v>
+        <v>0.1413</v>
       </c>
       <c r="C15" t="n">
-        <v>0.1516</v>
+        <v>0.7544</v>
       </c>
       <c r="D15" t="n">
-        <v>0.8262</v>
+        <v>0.1117</v>
       </c>
       <c r="E15" t="n">
-        <v>-0.1314</v>
+        <v>-0.0019</v>
       </c>
       <c r="F15" t="n">
-        <v>0.8593</v>
+        <v>0.2227</v>
       </c>
       <c r="G15" t="n">
-        <v>0.2721</v>
+        <v>0.7792</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>0.2156</v>
+        <v>0.1526</v>
       </c>
       <c r="B16" t="n">
-        <v>0.206</v>
+        <v>0.141</v>
       </c>
       <c r="C16" t="n">
-        <v>0.152</v>
+        <v>0.7628</v>
       </c>
       <c r="D16" t="n">
-        <v>0.8283</v>
+        <v>0.1128</v>
       </c>
       <c r="E16" t="n">
-        <v>-0.1306</v>
+        <v>0.021</v>
       </c>
       <c r="F16" t="n">
-        <v>0.859</v>
+        <v>0.2206</v>
       </c>
       <c r="G16" t="n">
-        <v>0.2716</v>
+        <v>0.7584</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>0.2167</v>
+        <v>0.153</v>
       </c>
       <c r="B17" t="n">
-        <v>0.206</v>
+        <v>0.141</v>
       </c>
       <c r="C17" t="n">
-        <v>0.153</v>
+        <v>0.7662</v>
       </c>
       <c r="D17" t="n">
-        <v>0.8335</v>
+        <v>0.1133</v>
       </c>
       <c r="E17" t="n">
-        <v>-0.1284</v>
+        <v>0.0316</v>
       </c>
       <c r="F17" t="n">
-        <v>0.8581</v>
+        <v>0.2196</v>
       </c>
       <c r="G17" t="n">
-        <v>0.2703</v>
+        <v>0.7488</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
+        <v>0.1541</v>
+      </c>
+      <c r="B18" t="n">
+        <v>0.1412</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0.7731</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0.1143</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0.0577</v>
+      </c>
+      <c r="F18" t="n">
         <v>0.2172</v>
       </c>
-      <c r="B18" t="n">
-        <v>0.206</v>
-      </c>
-      <c r="C18" t="n">
-        <v>0.1535</v>
-      </c>
-      <c r="D18" t="n">
-        <v>0.8358</v>
-      </c>
-      <c r="E18" t="n">
-        <v>-0.1275</v>
-      </c>
-      <c r="F18" t="n">
-        <v>0.8577</v>
-      </c>
       <c r="G18" t="n">
-        <v>0.2698</v>
+        <v>0.7251</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>0.2184</v>
+        <v>0.1559</v>
       </c>
       <c r="B19" t="n">
-        <v>0.206</v>
+        <v>0.1423</v>
       </c>
       <c r="C19" t="n">
-        <v>0.1547</v>
+        <v>0.7796</v>
       </c>
       <c r="D19" t="n">
-        <v>0.8417</v>
+        <v>0.1154</v>
       </c>
       <c r="E19" t="n">
-        <v>-0.1251</v>
+        <v>0.0992</v>
       </c>
       <c r="F19" t="n">
-        <v>0.8567</v>
+        <v>0.2134</v>
       </c>
       <c r="G19" t="n">
-        <v>0.2684</v>
+        <v>0.6874</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>0.2189</v>
+        <v>0.1579</v>
       </c>
       <c r="B20" t="n">
-        <v>0.206</v>
+        <v>0.1446</v>
       </c>
       <c r="C20" t="n">
-        <v>0.1553</v>
+        <v>0.7808</v>
       </c>
       <c r="D20" t="n">
-        <v>0.8443000000000001</v>
+        <v>0.1161</v>
       </c>
       <c r="E20" t="n">
-        <v>-0.124</v>
+        <v>0.1453</v>
       </c>
       <c r="F20" t="n">
-        <v>0.8563</v>
+        <v>0.2091</v>
       </c>
       <c r="G20" t="n">
-        <v>0.2677</v>
+        <v>0.6456</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>0.2202</v>
+        <v>0.16</v>
       </c>
       <c r="B21" t="n">
-        <v>0.2059</v>
+        <v>0.1484</v>
       </c>
       <c r="C21" t="n">
-        <v>0.1566</v>
+        <v>0.7753</v>
       </c>
       <c r="D21" t="n">
-        <v>0.8509</v>
+        <v>0.116</v>
       </c>
       <c r="E21" t="n">
-        <v>-0.1213</v>
+        <v>0.1961</v>
       </c>
       <c r="F21" t="n">
-        <v>0.8552</v>
+        <v>0.2044</v>
       </c>
       <c r="G21" t="n">
-        <v>0.2661</v>
+        <v>0.5995</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>0.2208</v>
+        <v>0.1624</v>
       </c>
       <c r="B22" t="n">
-        <v>0.2059</v>
+        <v>0.154</v>
       </c>
       <c r="C22" t="n">
-        <v>0.1572</v>
+        <v>0.7625</v>
       </c>
       <c r="D22" t="n">
-        <v>0.8537</v>
+        <v>0.115</v>
       </c>
       <c r="E22" t="n">
-        <v>-0.1202</v>
+        <v>0.2516</v>
       </c>
       <c r="F22" t="n">
-        <v>0.8547</v>
+        <v>0.1993</v>
       </c>
       <c r="G22" t="n">
-        <v>0.2654</v>
+        <v>0.5491</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>0.2223</v>
+        <v>0.165</v>
       </c>
       <c r="B23" t="n">
-        <v>0.2059</v>
+        <v>0.1615</v>
       </c>
       <c r="C23" t="n">
-        <v>0.1587</v>
+        <v>0.7427</v>
       </c>
       <c r="D23" t="n">
-        <v>0.861</v>
+        <v>0.1128</v>
       </c>
       <c r="E23" t="n">
-        <v>-0.1172</v>
+        <v>0.3118</v>
       </c>
       <c r="F23" t="n">
-        <v>0.8535</v>
+        <v>0.1937</v>
       </c>
       <c r="G23" t="n">
-        <v>0.2637</v>
+        <v>0.4945</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>0.2229</v>
+        <v>0.1678</v>
       </c>
       <c r="B24" t="n">
-        <v>0.2059</v>
+        <v>0.1712</v>
       </c>
       <c r="C24" t="n">
-        <v>0.1593</v>
+        <v>0.717</v>
       </c>
       <c r="D24" t="n">
-        <v>0.8641</v>
+        <v>0.1091</v>
       </c>
       <c r="E24" t="n">
-        <v>-0.1159</v>
+        <v>0.3766</v>
       </c>
       <c r="F24" t="n">
-        <v>0.853</v>
+        <v>0.1877</v>
       </c>
       <c r="G24" t="n">
-        <v>0.2629</v>
+        <v>0.4356</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>0.2246</v>
+        <v>0.1707</v>
       </c>
       <c r="B25" t="n">
-        <v>0.2059</v>
+        <v>0.183</v>
       </c>
       <c r="C25" t="n">
-        <v>0.161</v>
+        <v>0.6869</v>
       </c>
       <c r="D25" t="n">
-        <v>0.872</v>
+        <v>0.1037</v>
       </c>
       <c r="E25" t="n">
-        <v>-0.1127</v>
+        <v>0.4462</v>
       </c>
       <c r="F25" t="n">
-        <v>0.8517</v>
+        <v>0.1813</v>
       </c>
       <c r="G25" t="n">
-        <v>0.261</v>
+        <v>0.3725</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>0.227</v>
+        <v>0.1739</v>
       </c>
       <c r="B26" t="n">
-        <v>0.206</v>
+        <v>0.197</v>
       </c>
       <c r="C26" t="n">
-        <v>0.1634</v>
+        <v>0.6542</v>
       </c>
       <c r="D26" t="n">
-        <v>0.8839</v>
+        <v>0.0963</v>
       </c>
       <c r="E26" t="n">
-        <v>-0.1077</v>
+        <v>0.5204</v>
       </c>
       <c r="F26" t="n">
-        <v>0.8497</v>
+        <v>0.1744</v>
       </c>
       <c r="G26" t="n">
-        <v>0.2581</v>
+        <v>0.3052</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>0.2297</v>
+        <v>0.1773</v>
       </c>
       <c r="B27" t="n">
-        <v>0.206</v>
+        <v>0.2131</v>
       </c>
       <c r="C27" t="n">
-        <v>0.1661</v>
+        <v>0.6206</v>
       </c>
       <c r="D27" t="n">
-        <v>0.8967000000000001</v>
+        <v>0.0864</v>
       </c>
       <c r="E27" t="n">
-        <v>-0.1024</v>
+        <v>0.5993000000000001</v>
       </c>
       <c r="F27" t="n">
-        <v>0.8475</v>
+        <v>0.1671</v>
       </c>
       <c r="G27" t="n">
-        <v>0.2549</v>
+        <v>0.2336</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>0.2326</v>
+        <v>0.1808</v>
       </c>
       <c r="B28" t="n">
-        <v>0.2061</v>
+        <v>0.2313</v>
       </c>
       <c r="C28" t="n">
-        <v>0.1689</v>
+        <v>0.5873</v>
       </c>
       <c r="D28" t="n">
-        <v>0.9103</v>
+        <v>0.0738</v>
       </c>
       <c r="E28" t="n">
-        <v>-0.09660000000000001</v>
+        <v>0.6829</v>
       </c>
       <c r="F28" t="n">
-        <v>0.8451</v>
+        <v>0.1594</v>
       </c>
       <c r="G28" t="n">
-        <v>0.2515</v>
+        <v>0.1577</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>0.2357</v>
+        <v>0.1846</v>
       </c>
       <c r="B29" t="n">
-        <v>0.2061</v>
+        <v>0.2515</v>
       </c>
       <c r="C29" t="n">
-        <v>0.1719</v>
+        <v>0.5552</v>
       </c>
       <c r="D29" t="n">
-        <v>0.9248</v>
+        <v>0.0581</v>
       </c>
       <c r="E29" t="n">
-        <v>-0.0905</v>
+        <v>0.7712</v>
       </c>
       <c r="F29" t="n">
-        <v>0.8426</v>
+        <v>0.1512</v>
       </c>
       <c r="G29" t="n">
-        <v>0.2478</v>
+        <v>0.0776</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>0.2389</v>
+        <v>0.1886</v>
       </c>
       <c r="B30" t="n">
-        <v>0.2063</v>
+        <v>0.2735</v>
       </c>
       <c r="C30" t="n">
-        <v>0.1751</v>
+        <v>0.5249</v>
       </c>
       <c r="D30" t="n">
-        <v>0.9401</v>
+        <v>0.0389</v>
       </c>
       <c r="E30" t="n">
-        <v>-0.0839</v>
+        <v>0.8641</v>
       </c>
       <c r="F30" t="n">
-        <v>0.84</v>
+        <v>0.1427</v>
       </c>
       <c r="G30" t="n">
-        <v>0.244</v>
+        <v>-0.0068</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>0.2424</v>
+        <v>0.1927</v>
       </c>
       <c r="B31" t="n">
-        <v>0.2064</v>
+        <v>0.2974</v>
       </c>
       <c r="C31" t="n">
-        <v>0.1785</v>
+        <v>0.4968</v>
       </c>
       <c r="D31" t="n">
-        <v>0.9562</v>
+        <v>0.0158</v>
       </c>
       <c r="E31" t="n">
-        <v>-0.077</v>
+        <v>0.9618</v>
       </c>
       <c r="F31" t="n">
-        <v>0.8371</v>
+        <v>0.1336</v>
       </c>
       <c r="G31" t="n">
-        <v>0.2398</v>
+        <v>-0.0954</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>0.2461</v>
+        <v>0.1971</v>
       </c>
       <c r="B32" t="n">
-        <v>0.2067</v>
+        <v>0.3231</v>
       </c>
       <c r="C32" t="n">
-        <v>0.182</v>
+        <v>0.4708</v>
       </c>
       <c r="D32" t="n">
-        <v>0.973</v>
+        <v>-0.0116</v>
       </c>
       <c r="E32" t="n">
-        <v>-0.0696</v>
+        <v>1.0641</v>
       </c>
       <c r="F32" t="n">
-        <v>0.8341</v>
+        <v>0.1242</v>
       </c>
       <c r="G32" t="n">
-        <v>0.2355</v>
+        <v>-0.1883</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>0.2499</v>
+        <v>0.2017</v>
       </c>
       <c r="B33" t="n">
-        <v>0.2069</v>
+        <v>0.3504</v>
       </c>
       <c r="C33" t="n">
-        <v>0.1857</v>
+        <v>0.4471</v>
       </c>
       <c r="D33" t="n">
-        <v>0.9903999999999999</v>
+        <v>-0.0439</v>
       </c>
       <c r="E33" t="n">
-        <v>-0.0619</v>
+        <v>1.1711</v>
       </c>
       <c r="F33" t="n">
-        <v>0.831</v>
+        <v>0.1143</v>
       </c>
       <c r="G33" t="n">
-        <v>0.2309</v>
+        <v>-0.2854</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>0.254</v>
+        <v>0.2065</v>
       </c>
       <c r="B34" t="n">
-        <v>0.2072</v>
+        <v>0.3794</v>
       </c>
       <c r="C34" t="n">
-        <v>0.1896</v>
+        <v>0.4255</v>
       </c>
       <c r="D34" t="n">
-        <v>1.0086</v>
+        <v>-0.0815</v>
       </c>
       <c r="E34" t="n">
-        <v>-0.0537</v>
+        <v>1.2828</v>
       </c>
       <c r="F34" t="n">
-        <v>0.8277</v>
+        <v>0.104</v>
       </c>
       <c r="G34" t="n">
-        <v>0.2261</v>
+        <v>-0.3867</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>0.2583</v>
+        <v>0.2114</v>
       </c>
       <c r="B35" t="n">
-        <v>0.2076</v>
+        <v>0.41</v>
       </c>
       <c r="C35" t="n">
-        <v>0.1936</v>
+        <v>0.4059</v>
       </c>
       <c r="D35" t="n">
-        <v>1.0273</v>
+        <v>-0.1248</v>
       </c>
       <c r="E35" t="n">
-        <v>-0.0452</v>
+        <v>1.3992</v>
       </c>
       <c r="F35" t="n">
-        <v>0.8242</v>
+        <v>0.09320000000000001</v>
       </c>
       <c r="G35" t="n">
-        <v>0.221</v>
+        <v>-0.4923</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>0.2627</v>
+        <v>0.2166</v>
       </c>
       <c r="B36" t="n">
-        <v>0.2081</v>
+        <v>0.4422</v>
       </c>
       <c r="C36" t="n">
-        <v>0.1978</v>
+        <v>0.3881</v>
       </c>
       <c r="D36" t="n">
-        <v>1.0466</v>
+        <v>-0.1745</v>
       </c>
       <c r="E36" t="n">
-        <v>-0.0362</v>
+        <v>1.5202</v>
       </c>
       <c r="F36" t="n">
-        <v>0.8205</v>
+        <v>0.082</v>
       </c>
       <c r="G36" t="n">
-        <v>0.2157</v>
+        <v>-0.6022</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>0.2674</v>
+        <v>0.222</v>
       </c>
       <c r="B37" t="n">
-        <v>0.2086</v>
+        <v>0.4759</v>
       </c>
       <c r="C37" t="n">
-        <v>0.2022</v>
+        <v>0.3719</v>
       </c>
       <c r="D37" t="n">
-        <v>1.0663</v>
+        <v>-0.2309</v>
       </c>
       <c r="E37" t="n">
-        <v>-0.0269</v>
+        <v>1.6459</v>
       </c>
       <c r="F37" t="n">
-        <v>0.8167</v>
+        <v>0.0704</v>
       </c>
       <c r="G37" t="n">
-        <v>0.2102</v>
+        <v>-0.7163</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>0.2723</v>
+        <v>0.2275</v>
       </c>
       <c r="B38" t="n">
-        <v>0.2092</v>
+        <v>0.5111</v>
       </c>
       <c r="C38" t="n">
-        <v>0.2066</v>
+        <v>0.3572</v>
       </c>
       <c r="D38" t="n">
-        <v>1.0865</v>
+        <v>-0.2948</v>
       </c>
       <c r="E38" t="n">
-        <v>-0.0171</v>
+        <v>1.7764</v>
       </c>
       <c r="F38" t="n">
-        <v>0.8127</v>
+        <v>0.0583</v>
       </c>
       <c r="G38" t="n">
-        <v>0.2044</v>
+        <v>-0.8347</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>0.2774</v>
+        <v>0.2333</v>
       </c>
       <c r="B39" t="n">
-        <v>0.2099</v>
+        <v>0.5477</v>
       </c>
       <c r="C39" t="n">
-        <v>0.2113</v>
+        <v>0.3438</v>
       </c>
       <c r="D39" t="n">
-        <v>1.107</v>
+        <v>-0.3667</v>
       </c>
       <c r="E39" t="n">
-        <v>-0.007</v>
+        <v>1.9115</v>
       </c>
       <c r="F39" t="n">
-        <v>0.8086</v>
+        <v>0.0458</v>
       </c>
       <c r="G39" t="n">
-        <v>0.1984</v>
+        <v>-0.9573</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>0.2826</v>
+        <v>0.2393</v>
       </c>
       <c r="B40" t="n">
-        <v>0.2107</v>
+        <v>0.5858</v>
       </c>
       <c r="C40" t="n">
-        <v>0.216</v>
+        <v>0.3316</v>
       </c>
       <c r="D40" t="n">
-        <v>1.1279</v>
+        <v>-0.4471</v>
       </c>
       <c r="E40" t="n">
-        <v>0.0036</v>
+        <v>2.0513</v>
       </c>
       <c r="F40" t="n">
-        <v>0.8043</v>
+        <v>0.0329</v>
       </c>
       <c r="G40" t="n">
-        <v>0.1921</v>
+        <v>-1.0842</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>0.2881</v>
+        <v>0.2454</v>
       </c>
       <c r="B41" t="n">
-        <v>0.2116</v>
+        <v>0.6254</v>
       </c>
       <c r="C41" t="n">
-        <v>0.2209</v>
+        <v>0.3205</v>
       </c>
       <c r="D41" t="n">
-        <v>1.1489</v>
+        <v>-0.5368000000000001</v>
       </c>
       <c r="E41" t="n">
-        <v>0.0145</v>
+        <v>2.1957</v>
       </c>
       <c r="F41" t="n">
-        <v>0.7998</v>
+        <v>0.0196</v>
       </c>
       <c r="G41" t="n">
-        <v>0.1856</v>
+        <v>-1.2153</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>0.2938</v>
+        <v>0.2518</v>
       </c>
       <c r="B42" t="n">
-        <v>0.2126</v>
+        <v>0.6664</v>
       </c>
       <c r="C42" t="n">
-        <v>0.226</v>
+        <v>0.3104</v>
       </c>
       <c r="D42" t="n">
-        <v>1.1702</v>
+        <v>-0.6363</v>
       </c>
       <c r="E42" t="n">
-        <v>0.0259</v>
+        <v>2.3449</v>
       </c>
       <c r="F42" t="n">
-        <v>0.7952</v>
+        <v>0.0058</v>
       </c>
       <c r="G42" t="n">
-        <v>0.1789</v>
+        <v>-1.3507</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>0.2996</v>
+        <v>0.2584</v>
       </c>
       <c r="B43" t="n">
-        <v>0.2137</v>
+        <v>0.7088</v>
       </c>
       <c r="C43" t="n">
-        <v>0.2311</v>
+        <v>0.3011</v>
       </c>
       <c r="D43" t="n">
-        <v>1.1914</v>
+        <v>-0.7463</v>
       </c>
       <c r="E43" t="n">
-        <v>0.0376</v>
+        <v>2.4987</v>
       </c>
       <c r="F43" t="n">
-        <v>0.7904</v>
+        <v>-0.008399999999999999</v>
       </c>
       <c r="G43" t="n">
-        <v>0.1719</v>
+        <v>-1.4903</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>0.3057</v>
+        <v>0.2652</v>
       </c>
       <c r="B44" t="n">
-        <v>0.215</v>
+        <v>0.7524999999999999</v>
       </c>
       <c r="C44" t="n">
-        <v>0.2364</v>
+        <v>0.2925</v>
       </c>
       <c r="D44" t="n">
-        <v>1.2127</v>
+        <v>-0.8675</v>
       </c>
       <c r="E44" t="n">
-        <v>0.0498</v>
+        <v>2.6572</v>
       </c>
       <c r="F44" t="n">
-        <v>0.7855</v>
+        <v>-0.0231</v>
       </c>
       <c r="G44" t="n">
-        <v>0.1647</v>
+        <v>-1.6341</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>0.312</v>
+        <v>0.2721</v>
       </c>
       <c r="B45" t="n">
-        <v>0.2164</v>
+        <v>0.7977</v>
       </c>
       <c r="C45" t="n">
-        <v>0.2418</v>
+        <v>0.2847</v>
       </c>
       <c r="D45" t="n">
-        <v>1.2339</v>
+        <v>-1.0006</v>
       </c>
       <c r="E45" t="n">
-        <v>0.0623</v>
+        <v>2.8204</v>
       </c>
       <c r="F45" t="n">
-        <v>0.7804</v>
+        <v>-0.0382</v>
       </c>
       <c r="G45" t="n">
-        <v>0.1573</v>
+        <v>-1.7822</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>0.3185</v>
+        <v>0.2793</v>
       </c>
       <c r="B46" t="n">
-        <v>0.2179</v>
+        <v>0.8443000000000001</v>
       </c>
       <c r="C46" t="n">
-        <v>0.2472</v>
+        <v>0.2775</v>
       </c>
       <c r="D46" t="n">
-        <v>1.255</v>
+        <v>-1.1464</v>
       </c>
       <c r="E46" t="n">
-        <v>0.07530000000000001</v>
+        <v>2.9883</v>
       </c>
       <c r="F46" t="n">
-        <v>0.7751</v>
+        <v>-0.0537</v>
       </c>
       <c r="G46" t="n">
-        <v>0.1496</v>
+        <v>-1.9346</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>0.3251</v>
+        <v>0.2867</v>
       </c>
       <c r="B47" t="n">
-        <v>0.2196</v>
+        <v>0.8922</v>
       </c>
       <c r="C47" t="n">
-        <v>0.2528</v>
+        <v>0.2708</v>
       </c>
       <c r="D47" t="n">
-        <v>1.2758</v>
+        <v>-1.3055</v>
       </c>
       <c r="E47" t="n">
-        <v>0.0886</v>
+        <v>3.1609</v>
       </c>
       <c r="F47" t="n">
-        <v>0.7696</v>
+        <v>-0.0697</v>
       </c>
       <c r="G47" t="n">
-        <v>0.1417</v>
+        <v>-2.0912</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>0.332</v>
+        <v>0.2942</v>
       </c>
       <c r="B48" t="n">
-        <v>0.2214</v>
+        <v>0.9415</v>
       </c>
       <c r="C48" t="n">
-        <v>0.2585</v>
+        <v>0.2647</v>
       </c>
       <c r="D48" t="n">
-        <v>1.2962</v>
+        <v>-1.4788</v>
       </c>
       <c r="E48" t="n">
-        <v>0.1024</v>
+        <v>3.3381</v>
       </c>
       <c r="F48" t="n">
-        <v>0.764</v>
+        <v>-0.08599999999999999</v>
       </c>
       <c r="G48" t="n">
-        <v>0.1336</v>
+        <v>-2.2521</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>0.3391</v>
+        <v>0.302</v>
       </c>
       <c r="B49" t="n">
-        <v>0.2234</v>
+        <v>0.9922</v>
       </c>
       <c r="C49" t="n">
-        <v>0.2642</v>
+        <v>0.259</v>
       </c>
       <c r="D49" t="n">
-        <v>1.3163</v>
+        <v>-1.667</v>
       </c>
       <c r="E49" t="n">
-        <v>0.1166</v>
+        <v>3.5201</v>
       </c>
       <c r="F49" t="n">
-        <v>0.7583</v>
+        <v>-0.1029</v>
       </c>
       <c r="G49" t="n">
-        <v>0.1252</v>
+        <v>-2.4172</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>0.3463</v>
+        <v>0.31</v>
       </c>
       <c r="B50" t="n">
-        <v>0.2256</v>
+        <v>1.0442</v>
       </c>
       <c r="C50" t="n">
-        <v>0.27</v>
+        <v>0.2537</v>
       </c>
       <c r="D50" t="n">
-        <v>1.336</v>
+        <v>-1.8709</v>
       </c>
       <c r="E50" t="n">
-        <v>0.1311</v>
+        <v>3.7067</v>
       </c>
       <c r="F50" t="n">
-        <v>0.7523</v>
+        <v>-0.1201</v>
       </c>
       <c r="G50" t="n">
-        <v>0.1166</v>
+        <v>-2.5866</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>0.3538</v>
+        <v>0.3181</v>
       </c>
       <c r="B51" t="n">
-        <v>0.2279</v>
+        <v>1.0976</v>
       </c>
       <c r="C51" t="n">
-        <v>0.2759</v>
+        <v>0.2488</v>
       </c>
       <c r="D51" t="n">
-        <v>1.3551</v>
+        <v>-2.0915</v>
       </c>
       <c r="E51" t="n">
-        <v>0.1461</v>
+        <v>3.898</v>
       </c>
       <c r="F51" t="n">
-        <v>0.7462</v>
+        <v>-0.1378</v>
       </c>
       <c r="G51" t="n">
-        <v>0.1077</v>
+        <v>-2.7602</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>0.3615</v>
+        <v>0.3265</v>
       </c>
       <c r="B52" t="n">
-        <v>0.2304</v>
+        <v>1.1524</v>
       </c>
       <c r="C52" t="n">
-        <v>0.2819</v>
+        <v>0.2443</v>
       </c>
       <c r="D52" t="n">
-        <v>1.3737</v>
+        <v>-2.3294</v>
       </c>
       <c r="E52" t="n">
-        <v>0.1614</v>
+        <v>4.094</v>
       </c>
       <c r="F52" t="n">
-        <v>0.74</v>
+        <v>-0.1559</v>
       </c>
       <c r="G52" t="n">
-        <v>0.09859999999999999</v>
+        <v>-2.9381</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>0.3693</v>
+        <v>0.3351</v>
       </c>
       <c r="B53" t="n">
-        <v>0.2331</v>
+        <v>1.2085</v>
       </c>
       <c r="C53" t="n">
-        <v>0.2879</v>
+        <v>0.24</v>
       </c>
       <c r="D53" t="n">
-        <v>1.3916</v>
+        <v>-2.5857</v>
       </c>
       <c r="E53" t="n">
-        <v>0.1772</v>
+        <v>4.2946</v>
       </c>
       <c r="F53" t="n">
-        <v>0.7336</v>
+        <v>-0.1745</v>
       </c>
       <c r="G53" t="n">
-        <v>0.0893</v>
+        <v>-3.1202</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>0.3774</v>
+        <v>0.3438</v>
       </c>
       <c r="B54" t="n">
-        <v>0.236</v>
+        <v>1.2659</v>
       </c>
       <c r="C54" t="n">
-        <v>0.2939</v>
+        <v>0.2361</v>
       </c>
       <c r="D54" t="n">
-        <v>1.4088</v>
+        <v>-2.8612</v>
       </c>
       <c r="E54" t="n">
-        <v>0.1933</v>
+        <v>4.5</v>
       </c>
       <c r="F54" t="n">
-        <v>0.727</v>
+        <v>-0.1934</v>
       </c>
       <c r="G54" t="n">
-        <v>0.07969999999999999</v>
+        <v>-3.3065</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>0.3857</v>
+        <v>0.3528</v>
       </c>
       <c r="B55" t="n">
-        <v>0.239</v>
+        <v>1.3247</v>
       </c>
       <c r="C55" t="n">
-        <v>0.3</v>
+        <v>0.2324</v>
       </c>
       <c r="D55" t="n">
-        <v>1.4253</v>
+        <v>-3.1568</v>
       </c>
       <c r="E55" t="n">
-        <v>0.2099</v>
+        <v>4.71</v>
       </c>
       <c r="F55" t="n">
-        <v>0.7202</v>
+        <v>-0.2129</v>
       </c>
       <c r="G55" t="n">
-        <v>0.0699</v>
+        <v>-3.4972</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>0.3942</v>
+        <v>0.362</v>
       </c>
       <c r="B56" t="n">
-        <v>0.2423</v>
+        <v>1.3848</v>
       </c>
       <c r="C56" t="n">
-        <v>0.3061</v>
+        <v>0.2289</v>
       </c>
       <c r="D56" t="n">
-        <v>1.441</v>
+        <v>-3.4734</v>
       </c>
       <c r="E56" t="n">
-        <v>0.2268</v>
+        <v>4.9247</v>
       </c>
       <c r="F56" t="n">
-        <v>0.7133</v>
+        <v>-0.2327</v>
       </c>
       <c r="G56" t="n">
-        <v>0.0598</v>
+        <v>-3.692</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>0.4028</v>
+        <v>0.3714</v>
       </c>
       <c r="B57" t="n">
-        <v>0.2458</v>
+        <v>1.4463</v>
       </c>
       <c r="C57" t="n">
-        <v>0.3122</v>
+        <v>0.2257</v>
       </c>
       <c r="D57" t="n">
-        <v>1.456</v>
+        <v>-3.812</v>
       </c>
       <c r="E57" t="n">
-        <v>0.2442</v>
+        <v>5.1441</v>
       </c>
       <c r="F57" t="n">
-        <v>0.7063</v>
+        <v>-0.253</v>
       </c>
       <c r="G57" t="n">
-        <v>0.0495</v>
+        <v>-3.8912</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>0.4117</v>
+        <v>0.3809</v>
       </c>
       <c r="B58" t="n">
-        <v>0.2494</v>
+        <v>1.5091</v>
       </c>
       <c r="C58" t="n">
-        <v>0.3184</v>
+        <v>0.2226</v>
       </c>
       <c r="D58" t="n">
-        <v>1.4701</v>
+        <v>-4.1737</v>
       </c>
       <c r="E58" t="n">
-        <v>0.262</v>
+        <v>5.3682</v>
       </c>
       <c r="F58" t="n">
-        <v>0.699</v>
+        <v>-0.2737</v>
       </c>
       <c r="G58" t="n">
-        <v>0.039</v>
+        <v>-4.0945</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>0.4208</v>
+        <v>0.3907</v>
       </c>
       <c r="B59" t="n">
-        <v>0.2533</v>
+        <v>1.5732</v>
       </c>
       <c r="C59" t="n">
-        <v>0.3245</v>
+        <v>0.2197</v>
       </c>
       <c r="D59" t="n">
-        <v>1.4834</v>
+        <v>-4.5593</v>
       </c>
       <c r="E59" t="n">
-        <v>0.2801</v>
+        <v>5.597</v>
       </c>
       <c r="F59" t="n">
-        <v>0.6916</v>
+        <v>-0.2948</v>
       </c>
       <c r="G59" t="n">
-        <v>0.0283</v>
+        <v>-4.3021</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>0.43</v>
+        <v>0.4007</v>
       </c>
       <c r="B60" t="n">
-        <v>0.2574</v>
+        <v>1.6387</v>
       </c>
       <c r="C60" t="n">
-        <v>0.3307</v>
+        <v>0.217</v>
       </c>
       <c r="D60" t="n">
-        <v>1.4959</v>
+        <v>-4.9699</v>
       </c>
       <c r="E60" t="n">
-        <v>0.2987</v>
+        <v>5.8304</v>
       </c>
       <c r="F60" t="n">
-        <v>0.6841</v>
+        <v>-0.3164</v>
       </c>
       <c r="G60" t="n">
-        <v>0.0173</v>
+        <v>-4.514</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>0.4395</v>
+        <v>0.4108</v>
       </c>
       <c r="B61" t="n">
-        <v>0.2617</v>
+        <v>1.7055</v>
       </c>
       <c r="C61" t="n">
-        <v>0.3368</v>
+        <v>0.2145</v>
       </c>
       <c r="D61" t="n">
-        <v>1.5075</v>
+        <v>-5.4065</v>
       </c>
       <c r="E61" t="n">
-        <v>0.3176</v>
+        <v>6.0686</v>
       </c>
       <c r="F61" t="n">
-        <v>0.6763</v>
+        <v>-0.3384</v>
       </c>
       <c r="G61" t="n">
-        <v>0.006</v>
+        <v>-4.7301</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>0.4492</v>
+        <v>0.4212</v>
       </c>
       <c r="B62" t="n">
-        <v>0.2662</v>
+        <v>1.7736</v>
       </c>
       <c r="C62" t="n">
-        <v>0.3429</v>
+        <v>0.2121</v>
       </c>
       <c r="D62" t="n">
-        <v>1.5183</v>
+        <v>-5.8703</v>
       </c>
       <c r="E62" t="n">
-        <v>0.337</v>
+        <v>6.3114</v>
       </c>
       <c r="F62" t="n">
-        <v>0.6684</v>
+        <v>-0.3609</v>
       </c>
       <c r="G62" t="n">
-        <v>-0.0054</v>
+        <v>-4.9505</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>0.459</v>
+        <v>0.4318</v>
       </c>
       <c r="B63" t="n">
-        <v>0.2709</v>
+        <v>1.8431</v>
       </c>
       <c r="C63" t="n">
-        <v>0.3489</v>
+        <v>0.2099</v>
       </c>
       <c r="D63" t="n">
-        <v>1.5282</v>
+        <v>-6.3622</v>
       </c>
       <c r="E63" t="n">
-        <v>0.3568</v>
+        <v>6.5589</v>
       </c>
       <c r="F63" t="n">
-        <v>0.6604</v>
+        <v>-0.3838</v>
       </c>
       <c r="G63" t="n">
-        <v>-0.0171</v>
+        <v>-5.1751</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>0.4691</v>
+        <v>0.4425</v>
       </c>
       <c r="B64" t="n">
-        <v>0.2759</v>
+        <v>1.9139</v>
       </c>
       <c r="C64" t="n">
-        <v>0.355</v>
+        <v>0.2077</v>
       </c>
       <c r="D64" t="n">
-        <v>1.5374</v>
+        <v>-6.8834</v>
       </c>
       <c r="E64" t="n">
-        <v>0.3769</v>
+        <v>6.8111</v>
       </c>
       <c r="F64" t="n">
-        <v>0.6522</v>
+        <v>-0.4071</v>
       </c>
       <c r="G64" t="n">
-        <v>-0.0291</v>
+        <v>-5.404</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>0.4794</v>
+        <v>0.4535</v>
       </c>
       <c r="B65" t="n">
-        <v>0.281</v>
+        <v>1.986</v>
       </c>
       <c r="C65" t="n">
-        <v>0.3609</v>
+        <v>0.2057</v>
       </c>
       <c r="D65" t="n">
-        <v>1.5457</v>
+        <v>-7.435</v>
       </c>
       <c r="E65" t="n">
-        <v>0.3975</v>
+        <v>7.0679</v>
       </c>
       <c r="F65" t="n">
-        <v>0.6438</v>
+        <v>-0.4308</v>
       </c>
       <c r="G65" t="n">
-        <v>-0.0413</v>
+        <v>-5.6371</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>0.4899</v>
+        <v>0.4647</v>
       </c>
       <c r="B66" t="n">
-        <v>0.2864</v>
+        <v>2.0595</v>
       </c>
       <c r="C66" t="n">
-        <v>0.3668</v>
+        <v>0.2038</v>
       </c>
       <c r="D66" t="n">
-        <v>1.5533</v>
+        <v>-8.0182</v>
       </c>
       <c r="E66" t="n">
-        <v>0.4184</v>
+        <v>7.3295</v>
       </c>
       <c r="F66" t="n">
-        <v>0.6352</v>
+        <v>-0.455</v>
       </c>
       <c r="G66" t="n">
-        <v>-0.0537</v>
+        <v>-5.8745</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>0.5004999999999999</v>
+        <v>0.4761</v>
       </c>
       <c r="B67" t="n">
-        <v>0.292</v>
+        <v>2.1343</v>
       </c>
       <c r="C67" t="n">
-        <v>0.3726</v>
+        <v>0.202</v>
       </c>
       <c r="D67" t="n">
-        <v>1.5601</v>
+        <v>-8.6341</v>
       </c>
       <c r="E67" t="n">
-        <v>0.4398</v>
+        <v>7.5957</v>
       </c>
       <c r="F67" t="n">
-        <v>0.6264999999999999</v>
+        <v>-0.4796</v>
       </c>
       <c r="G67" t="n">
-        <v>-0.0664</v>
+        <v>-6.1161</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>0.5114</v>
+        <v>0.4876</v>
       </c>
       <c r="B68" t="n">
-        <v>0.2978</v>
+        <v>2.2104</v>
       </c>
       <c r="C68" t="n">
-        <v>0.3784</v>
+        <v>0.2002</v>
       </c>
       <c r="D68" t="n">
-        <v>1.5662</v>
+        <v>-9.283899999999999</v>
       </c>
       <c r="E68" t="n">
-        <v>0.4616</v>
+        <v>7.8666</v>
       </c>
       <c r="F68" t="n">
-        <v>0.6177</v>
+        <v>-0.5046</v>
       </c>
       <c r="G68" t="n">
-        <v>-0.07920000000000001</v>
+        <v>-6.362</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>0.5225</v>
+        <v>0.4994</v>
       </c>
       <c r="B69" t="n">
-        <v>0.3038</v>
+        <v>2.2878</v>
       </c>
       <c r="C69" t="n">
-        <v>0.384</v>
+        <v>0.1986</v>
       </c>
       <c r="D69" t="n">
-        <v>1.5717</v>
+        <v>-9.9687</v>
       </c>
       <c r="E69" t="n">
-        <v>0.4837</v>
+        <v>8.142200000000001</v>
       </c>
       <c r="F69" t="n">
-        <v>0.6086</v>
+        <v>-0.5301</v>
       </c>
       <c r="G69" t="n">
-        <v>-0.0924</v>
+        <v>-6.6121</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>0.5337</v>
+        <v>0.5114</v>
       </c>
       <c r="B70" t="n">
-        <v>0.31</v>
+        <v>2.3666</v>
       </c>
       <c r="C70" t="n">
-        <v>0.3896</v>
+        <v>0.1971</v>
       </c>
       <c r="D70" t="n">
-        <v>1.5764</v>
+        <v>-10.69</v>
       </c>
       <c r="E70" t="n">
-        <v>0.5063</v>
+        <v>8.422499999999999</v>
       </c>
       <c r="F70" t="n">
-        <v>0.5995</v>
+        <v>-0.556</v>
       </c>
       <c r="G70" t="n">
-        <v>-0.1057</v>
+        <v>-6.8665</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>0.5452</v>
+        <v>0.5235</v>
       </c>
       <c r="B71" t="n">
-        <v>0.3165</v>
+        <v>2.4467</v>
       </c>
       <c r="C71" t="n">
-        <v>0.395</v>
+        <v>0.1956</v>
       </c>
       <c r="D71" t="n">
-        <v>1.5806</v>
+        <v>-11.4488</v>
       </c>
       <c r="E71" t="n">
-        <v>0.5293</v>
+        <v>8.7075</v>
       </c>
       <c r="F71" t="n">
-        <v>0.5901</v>
+        <v>-0.5824</v>
       </c>
       <c r="G71" t="n">
-        <v>-0.1194</v>
+        <v>-7.1251</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>0.5569</v>
+        <v>0.5359</v>
       </c>
       <c r="B72" t="n">
-        <v>0.3231</v>
+        <v>2.5281</v>
       </c>
       <c r="C72" t="n">
-        <v>0.4003</v>
+        <v>0.1942</v>
       </c>
       <c r="D72" t="n">
-        <v>1.5841</v>
+        <v>-12.2465</v>
       </c>
       <c r="E72" t="n">
-        <v>0.5526</v>
+        <v>8.9971</v>
       </c>
       <c r="F72" t="n">
-        <v>0.5806</v>
+        <v>-0.6091</v>
       </c>
       <c r="G72" t="n">
-        <v>-0.1332</v>
+        <v>-7.3879</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>0.5688</v>
+        <v>0.5485</v>
       </c>
       <c r="B73" t="n">
-        <v>0.33</v>
+        <v>2.6108</v>
       </c>
       <c r="C73" t="n">
-        <v>0.4054</v>
+        <v>0.1928</v>
       </c>
       <c r="D73" t="n">
-        <v>1.5871</v>
+        <v>-13.0843</v>
       </c>
       <c r="E73" t="n">
-        <v>0.5764</v>
+        <v>9.291399999999999</v>
       </c>
       <c r="F73" t="n">
-        <v>0.5709</v>
+        <v>-0.6364</v>
       </c>
       <c r="G73" t="n">
-        <v>-0.1473</v>
+        <v>-7.6551</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>0.5808</v>
+        <v>0.5612</v>
       </c>
       <c r="B74" t="n">
-        <v>0.3371</v>
+        <v>2.6949</v>
       </c>
       <c r="C74" t="n">
-        <v>0.4104</v>
+        <v>0.1916</v>
       </c>
       <c r="D74" t="n">
-        <v>1.5896</v>
+        <v>-13.9636</v>
       </c>
       <c r="E74" t="n">
-        <v>0.6006</v>
+        <v>9.590400000000001</v>
       </c>
       <c r="F74" t="n">
-        <v>0.5610000000000001</v>
+        <v>-0.664</v>
       </c>
       <c r="G74" t="n">
-        <v>-0.1616</v>
+        <v>-7.9264</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>0.5931</v>
+        <v>0.5742</v>
       </c>
       <c r="B75" t="n">
-        <v>0.3444</v>
+        <v>2.7803</v>
       </c>
       <c r="C75" t="n">
-        <v>0.4152</v>
+        <v>0.1903</v>
       </c>
       <c r="D75" t="n">
-        <v>1.5916</v>
+        <v>-14.8856</v>
       </c>
       <c r="E75" t="n">
-        <v>0.6251</v>
+        <v>9.8941</v>
       </c>
       <c r="F75" t="n">
-        <v>0.551</v>
+        <v>-0.6921</v>
       </c>
       <c r="G75" t="n">
-        <v>-0.1762</v>
+        <v>-8.2021</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>0.6056</v>
+        <v>0.5874</v>
       </c>
       <c r="B76" t="n">
-        <v>0.3519</v>
+        <v>2.867</v>
       </c>
       <c r="C76" t="n">
-        <v>0.4198</v>
+        <v>0.1892</v>
       </c>
       <c r="D76" t="n">
-        <v>1.5931</v>
+        <v>-15.8518</v>
       </c>
       <c r="E76" t="n">
-        <v>0.6501</v>
+        <v>10.2025</v>
       </c>
       <c r="F76" t="n">
-        <v>0.5409</v>
+        <v>-0.7206</v>
       </c>
       <c r="G76" t="n">
-        <v>-0.1909</v>
+        <v>-8.4819</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>0.6182</v>
+        <v>0.6008</v>
       </c>
       <c r="B77" t="n">
-        <v>0.3596</v>
+        <v>2.955</v>
       </c>
       <c r="C77" t="n">
-        <v>0.4243</v>
+        <v>0.1881</v>
       </c>
       <c r="D77" t="n">
-        <v>1.5942</v>
+        <v>-16.8636</v>
       </c>
       <c r="E77" t="n">
-        <v>0.6755</v>
+        <v>10.5156</v>
       </c>
       <c r="F77" t="n">
-        <v>0.5305</v>
+        <v>-0.7495000000000001</v>
       </c>
       <c r="G77" t="n">
-        <v>-0.206</v>
+        <v>-8.7661</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>0.6311</v>
+        <v>0.6143</v>
       </c>
       <c r="B78" t="n">
-        <v>0.3675</v>
+        <v>3.0444</v>
       </c>
       <c r="C78" t="n">
-        <v>0.4285</v>
+        <v>0.187</v>
       </c>
       <c r="D78" t="n">
-        <v>1.5949</v>
+        <v>-17.9222</v>
       </c>
       <c r="E78" t="n">
-        <v>0.7012</v>
+        <v>10.8333</v>
       </c>
       <c r="F78" t="n">
-        <v>0.52</v>
+        <v>-0.7789</v>
       </c>
       <c r="G78" t="n">
-        <v>-0.2212</v>
+        <v>-9.054399999999999</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>0.6442</v>
+        <v>0.6281</v>
       </c>
       <c r="B79" t="n">
-        <v>0.3756</v>
+        <v>3.1351</v>
       </c>
       <c r="C79" t="n">
-        <v>0.4326</v>
+        <v>0.186</v>
       </c>
       <c r="D79" t="n">
-        <v>1.5953</v>
+        <v>-19.0291</v>
       </c>
       <c r="E79" t="n">
-        <v>0.7274</v>
+        <v>11.1557</v>
       </c>
       <c r="F79" t="n">
-        <v>0.5094</v>
+        <v>-0.8087</v>
       </c>
       <c r="G79" t="n">
-        <v>-0.2367</v>
+        <v>-9.347099999999999</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>0.6574</v>
+        <v>0.6421</v>
       </c>
       <c r="B80" t="n">
-        <v>0.3839</v>
+        <v>3.2271</v>
       </c>
       <c r="C80" t="n">
-        <v>0.4364</v>
+        <v>0.185</v>
       </c>
       <c r="D80" t="n">
-        <v>1.5953</v>
+        <v>-20.1859</v>
       </c>
       <c r="E80" t="n">
-        <v>0.754</v>
+        <v>11.4829</v>
       </c>
       <c r="F80" t="n">
-        <v>0.4985</v>
+        <v>-0.8389</v>
       </c>
       <c r="G80" t="n">
-        <v>-0.2525</v>
+        <v>-9.6439</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>0.6709000000000001</v>
+        <v>0.6562</v>
       </c>
       <c r="B81" t="n">
-        <v>0.3924</v>
+        <v>3.3204</v>
       </c>
       <c r="C81" t="n">
-        <v>0.4399</v>
+        <v>0.1841</v>
       </c>
       <c r="D81" t="n">
-        <v>1.595</v>
+        <v>-21.3938</v>
       </c>
       <c r="E81" t="n">
-        <v>0.7809</v>
+        <v>11.8146</v>
       </c>
       <c r="F81" t="n">
-        <v>0.4875</v>
+        <v>-0.8696</v>
       </c>
       <c r="G81" t="n">
-        <v>-0.2685</v>
+        <v>-9.945</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>0.6846</v>
+        <v>0.6706</v>
       </c>
       <c r="B82" t="n">
-        <v>0.4011</v>
+        <v>3.415</v>
       </c>
       <c r="C82" t="n">
-        <v>0.4432</v>
+        <v>0.1832</v>
       </c>
       <c r="D82" t="n">
-        <v>1.5944</v>
+        <v>-22.6544</v>
       </c>
       <c r="E82" t="n">
-        <v>0.8083</v>
+        <v>12.1511</v>
       </c>
       <c r="F82" t="n">
-        <v>0.4764</v>
+        <v>-0.9006999999999999</v>
       </c>
       <c r="G82" t="n">
-        <v>-0.2847</v>
+        <v>-10.2504</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>0.6985</v>
+        <v>0.6852</v>
       </c>
       <c r="B83" t="n">
-        <v>0.4101</v>
+        <v>3.511</v>
       </c>
       <c r="C83" t="n">
-        <v>0.4462</v>
+        <v>0.1823</v>
       </c>
       <c r="D83" t="n">
-        <v>1.5936</v>
+        <v>-23.9692</v>
       </c>
       <c r="E83" t="n">
-        <v>0.8361</v>
+        <v>12.4923</v>
       </c>
       <c r="F83" t="n">
-        <v>0.4651</v>
+        <v>-0.9322</v>
       </c>
       <c r="G83" t="n">
-        <v>-0.3011</v>
+        <v>-10.56</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>0.7125</v>
+        <v>0.6999</v>
       </c>
       <c r="B84" t="n">
-        <v>0.4192</v>
+        <v>3.6083</v>
       </c>
       <c r="C84" t="n">
-        <v>0.449</v>
+        <v>0.1815</v>
       </c>
       <c r="D84" t="n">
-        <v>1.5925</v>
+        <v>-25.3398</v>
       </c>
       <c r="E84" t="n">
-        <v>0.8642</v>
+        <v>12.8381</v>
       </c>
       <c r="F84" t="n">
-        <v>0.4536</v>
+        <v>-0.9641999999999999</v>
       </c>
       <c r="G84" t="n">
-        <v>-0.3178</v>
+        <v>-10.8739</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>0.7268</v>
+        <v>0.7149</v>
       </c>
       <c r="B85" t="n">
-        <v>0.4285</v>
+        <v>3.7069</v>
       </c>
       <c r="C85" t="n">
-        <v>0.4514</v>
+        <v>0.1807</v>
       </c>
       <c r="D85" t="n">
-        <v>1.5913</v>
+        <v>-26.7676</v>
       </c>
       <c r="E85" t="n">
-        <v>0.8928</v>
+        <v>13.1887</v>
       </c>
       <c r="F85" t="n">
-        <v>0.442</v>
+        <v>-0.9966</v>
       </c>
       <c r="G85" t="n">
-        <v>-0.3348</v>
+        <v>-11.192</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>0.7413</v>
+        <v>0.7301</v>
       </c>
       <c r="B86" t="n">
-        <v>0.438</v>
+        <v>3.8069</v>
       </c>
       <c r="C86" t="n">
-        <v>0.4536</v>
+        <v>0.18</v>
       </c>
       <c r="D86" t="n">
-        <v>1.5898</v>
+        <v>-28.2542</v>
       </c>
       <c r="E86" t="n">
-        <v>0.9218</v>
+        <v>13.5439</v>
       </c>
       <c r="F86" t="n">
-        <v>0.4302</v>
+        <v>-1.0294</v>
       </c>
       <c r="G86" t="n">
-        <v>-0.3519</v>
+        <v>-11.5144</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>0.7559</v>
+        <v>0.7455000000000001</v>
       </c>
       <c r="B87" t="n">
-        <v>0.4476</v>
+        <v>3.9081</v>
       </c>
       <c r="C87" t="n">
-        <v>0.4554</v>
+        <v>0.1792</v>
       </c>
       <c r="D87" t="n">
-        <v>1.5882</v>
+        <v>-29.8012</v>
       </c>
       <c r="E87" t="n">
-        <v>0.9510999999999999</v>
+        <v>13.9038</v>
       </c>
       <c r="F87" t="n">
-        <v>0.4182</v>
+        <v>-1.0627</v>
       </c>
       <c r="G87" t="n">
-        <v>-0.3693</v>
+        <v>-11.841</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>0.7708</v>
+        <v>0.761</v>
       </c>
       <c r="B88" t="n">
-        <v>0.4575</v>
+        <v>4.0107</v>
       </c>
       <c r="C88" t="n">
-        <v>0.4568</v>
+        <v>0.1785</v>
       </c>
       <c r="D88" t="n">
-        <v>1.5864</v>
+        <v>-31.4102</v>
       </c>
       <c r="E88" t="n">
-        <v>0.9809</v>
+        <v>14.2683</v>
       </c>
       <c r="F88" t="n">
-        <v>0.4061</v>
+        <v>-1.0964</v>
       </c>
       <c r="G88" t="n">
-        <v>-0.387</v>
+        <v>-12.1719</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>0.7859</v>
+        <v>0.7768</v>
       </c>
       <c r="B89" t="n">
-        <v>0.4676</v>
+        <v>4.1146</v>
       </c>
       <c r="C89" t="n">
-        <v>0.4579</v>
+        <v>0.1779</v>
       </c>
       <c r="D89" t="n">
-        <v>1.5845</v>
+        <v>-33.0828</v>
       </c>
       <c r="E89" t="n">
-        <v>1.0111</v>
+        <v>14.6376</v>
       </c>
       <c r="F89" t="n">
-        <v>0.3938</v>
+        <v>-1.1305</v>
       </c>
       <c r="G89" t="n">
-        <v>-0.4048</v>
+        <v>-12.507</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>0.8012</v>
+        <v>0.7927999999999999</v>
       </c>
       <c r="B90" t="n">
-        <v>0.4778</v>
+        <v>4.2198</v>
       </c>
       <c r="C90" t="n">
-        <v>0.4587</v>
+        <v>0.1772</v>
       </c>
       <c r="D90" t="n">
-        <v>1.5825</v>
+        <v>-34.8207</v>
       </c>
       <c r="E90" t="n">
-        <v>1.0416</v>
+        <v>15.0115</v>
       </c>
       <c r="F90" t="n">
-        <v>0.3813</v>
+        <v>-1.1651</v>
       </c>
       <c r="G90" t="n">
-        <v>-0.423</v>
+        <v>-12.8464</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>0.8166</v>
+        <v>0.8089</v>
       </c>
       <c r="B91" t="n">
-        <v>0.4883</v>
+        <v>4.3263</v>
       </c>
       <c r="C91" t="n">
-        <v>0.459</v>
+        <v>0.1766</v>
       </c>
       <c r="D91" t="n">
-        <v>1.5804</v>
+        <v>-36.6256</v>
       </c>
       <c r="E91" t="n">
-        <v>1.0726</v>
+        <v>15.3902</v>
       </c>
       <c r="F91" t="n">
-        <v>0.3687</v>
+        <v>-1.2001</v>
       </c>
       <c r="G91" t="n">
-        <v>-0.4413</v>
+        <v>-13.19</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>0.8323</v>
+        <v>0.8253</v>
       </c>
       <c r="B92" t="n">
-        <v>0.4989</v>
+        <v>4.4342</v>
       </c>
       <c r="C92" t="n">
-        <v>0.459</v>
+        <v>0.176</v>
       </c>
       <c r="D92" t="n">
-        <v>1.5781</v>
+        <v>-38.4991</v>
       </c>
       <c r="E92" t="n">
-        <v>1.104</v>
+        <v>15.7735</v>
       </c>
       <c r="F92" t="n">
-        <v>0.3559</v>
+        <v>-1.2355</v>
       </c>
       <c r="G92" t="n">
-        <v>-0.4599</v>
+        <v>-13.5379</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>0.8482</v>
+        <v>0.8419</v>
       </c>
       <c r="B93" t="n">
-        <v>0.5097</v>
+        <v>4.5434</v>
       </c>
       <c r="C93" t="n">
-        <v>0.4585</v>
+        <v>0.1754</v>
       </c>
       <c r="D93" t="n">
-        <v>1.5758</v>
+        <v>-40.4428</v>
       </c>
       <c r="E93" t="n">
-        <v>1.1358</v>
+        <v>16.1615</v>
       </c>
       <c r="F93" t="n">
-        <v>0.343</v>
+        <v>-1.2714</v>
       </c>
       <c r="G93" t="n">
-        <v>-0.4787</v>
+        <v>-13.89</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>0.8642</v>
+        <v>0.8586</v>
       </c>
       <c r="B94" t="n">
-        <v>0.5207000000000001</v>
+        <v>4.6539</v>
       </c>
       <c r="C94" t="n">
-        <v>0.4576</v>
+        <v>0.1748</v>
       </c>
       <c r="D94" t="n">
-        <v>1.5734</v>
+        <v>-42.4587</v>
       </c>
       <c r="E94" t="n">
-        <v>1.1679</v>
+        <v>16.5541</v>
       </c>
       <c r="F94" t="n">
-        <v>0.3298</v>
+        <v>-1.3077</v>
       </c>
       <c r="G94" t="n">
-        <v>-0.4978</v>
+        <v>-14.2464</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>0.8804999999999999</v>
+        <v>0.8756</v>
       </c>
       <c r="B95" t="n">
-        <v>0.5318000000000001</v>
+        <v>4.7657</v>
       </c>
       <c r="C95" t="n">
-        <v>0.4562</v>
+        <v>0.1743</v>
       </c>
       <c r="D95" t="n">
-        <v>1.571</v>
+        <v>-44.5484</v>
       </c>
       <c r="E95" t="n">
-        <v>1.2005</v>
+        <v>16.9515</v>
       </c>
       <c r="F95" t="n">
-        <v>0.3166</v>
+        <v>-1.3444</v>
       </c>
       <c r="G95" t="n">
-        <v>-0.5171</v>
+        <v>-14.607</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>0.897</v>
+        <v>0.8928</v>
       </c>
       <c r="B96" t="n">
-        <v>0.5432</v>
+        <v>4.8789</v>
       </c>
       <c r="C96" t="n">
-        <v>0.4544</v>
+        <v>0.1738</v>
       </c>
       <c r="D96" t="n">
-        <v>1.5685</v>
+        <v>-46.7136</v>
       </c>
       <c r="E96" t="n">
-        <v>1.2335</v>
+        <v>17.3535</v>
       </c>
       <c r="F96" t="n">
-        <v>0.3031</v>
+        <v>-1.3816</v>
       </c>
       <c r="G96" t="n">
-        <v>-0.5366</v>
+        <v>-14.9719</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>0.9136</v>
+        <v>0.9102</v>
       </c>
       <c r="B97" t="n">
-        <v>0.5547</v>
+        <v>4.9933</v>
       </c>
       <c r="C97" t="n">
-        <v>0.4521</v>
+        <v>0.1733</v>
       </c>
       <c r="D97" t="n">
-        <v>1.566</v>
+        <v>-48.9562</v>
       </c>
       <c r="E97" t="n">
-        <v>1.2669</v>
+        <v>17.7603</v>
       </c>
       <c r="F97" t="n">
-        <v>0.2895</v>
+        <v>-1.4192</v>
       </c>
       <c r="G97" t="n">
-        <v>-0.5564</v>
+        <v>-15.341</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>0.9305</v>
+        <v>0.9277</v>
       </c>
       <c r="B98" t="n">
-        <v>0.5664</v>
+        <v>5.1091</v>
       </c>
       <c r="C98" t="n">
-        <v>0.4493</v>
+        <v>0.1728</v>
       </c>
       <c r="D98" t="n">
-        <v>1.5634</v>
+        <v>-51.278</v>
       </c>
       <c r="E98" t="n">
-        <v>1.3006</v>
+        <v>18.1717</v>
       </c>
       <c r="F98" t="n">
-        <v>0.2758</v>
+        <v>-1.4572</v>
       </c>
       <c r="G98" t="n">
-        <v>-0.5764</v>
+        <v>-15.7144</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>0.9476</v>
+        <v>0.9455</v>
       </c>
       <c r="B99" t="n">
-        <v>0.5783</v>
+        <v>5.2262</v>
       </c>
       <c r="C99" t="n">
-        <v>0.446</v>
+        <v>0.1723</v>
       </c>
       <c r="D99" t="n">
-        <v>1.5608</v>
+        <v>-53.6808</v>
       </c>
       <c r="E99" t="n">
-        <v>1.3348</v>
+        <v>18.5877</v>
       </c>
       <c r="F99" t="n">
-        <v>0.2618</v>
+        <v>-1.4957</v>
       </c>
       <c r="G99" t="n">
-        <v>-0.5967</v>
+        <v>-16.0921</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>0.9649</v>
+        <v>0.9635</v>
       </c>
       <c r="B100" t="n">
-        <v>0.5903</v>
+        <v>5.3446</v>
       </c>
       <c r="C100" t="n">
-        <v>0.4421</v>
+        <v>0.1718</v>
       </c>
       <c r="D100" t="n">
-        <v>1.5582</v>
+        <v>-56.1665</v>
       </c>
       <c r="E100" t="n">
-        <v>1.3694</v>
+        <v>19.0085</v>
       </c>
       <c r="F100" t="n">
-        <v>0.2478</v>
+        <v>-1.5346</v>
       </c>
       <c r="G100" t="n">
-        <v>-0.6171</v>
+        <v>-16.4739</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="n">
-        <v>0.9823</v>
+        <v>0.9816</v>
       </c>
       <c r="B101" t="n">
-        <v>0.6026</v>
+        <v>5.4644</v>
       </c>
       <c r="C101" t="n">
-        <v>0.4377</v>
+        <v>0.1714</v>
       </c>
       <c r="D101" t="n">
-        <v>1.5556</v>
+        <v>-58.7369</v>
       </c>
       <c r="E101" t="n">
-        <v>1.4044</v>
+        <v>19.434</v>
       </c>
       <c r="F101" t="n">
-        <v>0.2335</v>
+        <v>-1.5739</v>
       </c>
       <c r="G101" t="n">
-        <v>-0.6379</v>
+        <v>-16.8601</v>
       </c>
     </row>
     <row r="102">
@@ -7871,22 +7871,22 @@
         <v>1</v>
       </c>
       <c r="B102" t="n">
-        <v>0.615</v>
+        <v>5.5854</v>
       </c>
       <c r="C102" t="n">
-        <v>0.4327</v>
+        <v>0.171</v>
       </c>
       <c r="D102" t="n">
-        <v>1.5529</v>
+        <v>-61.3939</v>
       </c>
       <c r="E102" t="n">
-        <v>1.4397</v>
+        <v>19.8641</v>
       </c>
       <c r="F102" t="n">
-        <v>0.2191</v>
+        <v>-1.6137</v>
       </c>
       <c r="G102" t="n">
-        <v>-0.6588000000000001</v>
+        <v>-17.2504</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added some smarter data structure
</commit_message>
<xml_diff>
--- a/pythonCW/230023476PortfolioProblem.xlsx
+++ b/pythonCW/230023476PortfolioProblem.xlsx
@@ -5568,2325 +5568,2325 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.1472</v>
+        <v>0.0969</v>
       </c>
       <c r="B2" t="n">
-        <v>0.1461</v>
+        <v>0.07290000000000001</v>
       </c>
       <c r="C2" t="n">
-        <v>0.6992</v>
+        <v>0.7113</v>
       </c>
       <c r="D2" t="n">
-        <v>0.1045</v>
+        <v>0.08890000000000001</v>
       </c>
       <c r="E2" t="n">
-        <v>-0.1052</v>
+        <v>0.3277</v>
       </c>
       <c r="F2" t="n">
-        <v>0.2323</v>
+        <v>0.3277</v>
       </c>
       <c r="G2" t="n">
-        <v>0.8729</v>
+        <v>0.3133</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0.1472</v>
+        <v>0.0969</v>
       </c>
       <c r="B3" t="n">
-        <v>0.1461</v>
+        <v>0.073</v>
       </c>
       <c r="C3" t="n">
-        <v>0.6996</v>
+        <v>0.7115</v>
       </c>
       <c r="D3" t="n">
-        <v>0.1045</v>
+        <v>0.08890000000000001</v>
       </c>
       <c r="E3" t="n">
-        <v>-0.1045</v>
+        <v>0.3296</v>
       </c>
       <c r="F3" t="n">
-        <v>0.2322</v>
+        <v>0.3296</v>
       </c>
       <c r="G3" t="n">
-        <v>0.8723</v>
+        <v>0.31</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0.1473</v>
+        <v>0.097</v>
       </c>
       <c r="B4" t="n">
-        <v>0.1459</v>
+        <v>0.073</v>
       </c>
       <c r="C4" t="n">
-        <v>0.7017</v>
+        <v>0.7121</v>
       </c>
       <c r="D4" t="n">
-        <v>0.1048</v>
+        <v>0.089</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.1012</v>
+        <v>0.3267</v>
       </c>
       <c r="F4" t="n">
-        <v>0.2319</v>
+        <v>0.3267</v>
       </c>
       <c r="G4" t="n">
-        <v>0.8693</v>
+        <v>0.3167</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0.1474</v>
+        <v>0.09710000000000001</v>
       </c>
       <c r="B5" t="n">
-        <v>0.1457</v>
+        <v>0.0731</v>
       </c>
       <c r="C5" t="n">
-        <v>0.7030999999999999</v>
+        <v>0.7127</v>
       </c>
       <c r="D5" t="n">
-        <v>0.105</v>
+        <v>0.0891</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.09909999999999999</v>
+        <v>0.3323</v>
       </c>
       <c r="F5" t="n">
-        <v>0.2317</v>
+        <v>0.3323</v>
       </c>
       <c r="G5" t="n">
-        <v>0.8673999999999999</v>
+        <v>0.3067</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0.1477</v>
+        <v>0.0973</v>
       </c>
       <c r="B6" t="n">
-        <v>0.1452</v>
+        <v>0.0732</v>
       </c>
       <c r="C6" t="n">
-        <v>0.7072000000000001</v>
+        <v>0.7139</v>
       </c>
       <c r="D6" t="n">
-        <v>0.1055</v>
+        <v>0.0892</v>
       </c>
       <c r="E6" t="n">
-        <v>-0.0926</v>
+        <v>0.3264</v>
       </c>
       <c r="F6" t="n">
-        <v>0.2311</v>
+        <v>0.3264</v>
       </c>
       <c r="G6" t="n">
-        <v>0.8615</v>
+        <v>0.32</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0.1479</v>
+        <v>0.0975</v>
       </c>
       <c r="B7" t="n">
-        <v>0.145</v>
+        <v>0.07340000000000001</v>
       </c>
       <c r="C7" t="n">
-        <v>0.7094</v>
+        <v>0.7149</v>
       </c>
       <c r="D7" t="n">
-        <v>0.1058</v>
+        <v>0.08939999999999999</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.089</v>
+        <v>0.3357</v>
       </c>
       <c r="F7" t="n">
-        <v>0.2308</v>
+        <v>0.3357</v>
       </c>
       <c r="G7" t="n">
-        <v>0.8583</v>
+        <v>0.3033</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>0.1483</v>
+        <v>0.0977</v>
       </c>
       <c r="B8" t="n">
-        <v>0.1444</v>
+        <v>0.0736</v>
       </c>
       <c r="C8" t="n">
-        <v>0.7153</v>
+        <v>0.7167</v>
       </c>
       <c r="D8" t="n">
-        <v>0.1066</v>
+        <v>0.0896</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.07920000000000001</v>
+        <v>0.3269</v>
       </c>
       <c r="F8" t="n">
-        <v>0.2299</v>
+        <v>0.3269</v>
       </c>
       <c r="G8" t="n">
-        <v>0.8494</v>
+        <v>0.3233</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0.1485</v>
+        <v>0.098</v>
       </c>
       <c r="B9" t="n">
-        <v>0.1441</v>
+        <v>0.0738</v>
       </c>
       <c r="C9" t="n">
-        <v>0.7183</v>
+        <v>0.718</v>
       </c>
       <c r="D9" t="n">
-        <v>0.107</v>
+        <v>0.0898</v>
       </c>
       <c r="E9" t="n">
-        <v>-0.0743</v>
+        <v>0.34</v>
       </c>
       <c r="F9" t="n">
-        <v>0.2294</v>
+        <v>0.34</v>
       </c>
       <c r="G9" t="n">
-        <v>0.8449</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>0.1491</v>
+        <v>0.0983</v>
       </c>
       <c r="B10" t="n">
-        <v>0.1434</v>
+        <v>0.074</v>
       </c>
       <c r="C10" t="n">
-        <v>0.7258</v>
+        <v>0.7204</v>
       </c>
       <c r="D10" t="n">
-        <v>0.1079</v>
+        <v>0.0901</v>
       </c>
       <c r="E10" t="n">
-        <v>-0.0612</v>
+        <v>0.3283</v>
       </c>
       <c r="F10" t="n">
-        <v>0.2282</v>
+        <v>0.3283</v>
       </c>
       <c r="G10" t="n">
-        <v>0.833</v>
+        <v>0.3267</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>0.1493</v>
+        <v>0.0987</v>
       </c>
       <c r="B11" t="n">
-        <v>0.1431</v>
+        <v>0.07439999999999999</v>
       </c>
       <c r="C11" t="n">
-        <v>0.7292999999999999</v>
+        <v>0.722</v>
       </c>
       <c r="D11" t="n">
-        <v>0.1084</v>
+        <v>0.09039999999999999</v>
       </c>
       <c r="E11" t="n">
-        <v>-0.0548</v>
+        <v>0.3451</v>
       </c>
       <c r="F11" t="n">
-        <v>0.2276</v>
+        <v>0.3451</v>
       </c>
       <c r="G11" t="n">
-        <v>0.8272</v>
+        <v>0.2967</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>0.15</v>
+        <v>0.09909999999999999</v>
       </c>
       <c r="B12" t="n">
-        <v>0.1424</v>
+        <v>0.0746</v>
       </c>
       <c r="C12" t="n">
-        <v>0.7378</v>
+        <v>0.7251</v>
       </c>
       <c r="D12" t="n">
-        <v>0.1095</v>
+        <v>0.0907</v>
       </c>
       <c r="E12" t="n">
-        <v>-0.0385</v>
+        <v>0.3304</v>
       </c>
       <c r="F12" t="n">
-        <v>0.2261</v>
+        <v>0.3304</v>
       </c>
       <c r="G12" t="n">
-        <v>0.8124</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>0.1504</v>
+        <v>0.09950000000000001</v>
       </c>
       <c r="B13" t="n">
-        <v>0.1421</v>
+        <v>0.075</v>
       </c>
       <c r="C13" t="n">
-        <v>0.7416</v>
+        <v>0.7268</v>
       </c>
       <c r="D13" t="n">
-        <v>0.11</v>
+        <v>0.0911</v>
       </c>
       <c r="E13" t="n">
-        <v>-0.0307</v>
+        <v>0.3509</v>
       </c>
       <c r="F13" t="n">
-        <v>0.2254</v>
+        <v>0.3509</v>
       </c>
       <c r="G13" t="n">
-        <v>0.8053</v>
+        <v>0.2933</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>0.1512</v>
+        <v>0.1</v>
       </c>
       <c r="B14" t="n">
-        <v>0.1415</v>
+        <v>0.07530000000000001</v>
       </c>
       <c r="C14" t="n">
-        <v>0.7506</v>
+        <v>0.7306</v>
       </c>
       <c r="D14" t="n">
-        <v>0.1112</v>
+        <v>0.0915</v>
       </c>
       <c r="E14" t="n">
-        <v>-0.0111</v>
+        <v>0.3333</v>
       </c>
       <c r="F14" t="n">
-        <v>0.2236</v>
+        <v>0.3333</v>
       </c>
       <c r="G14" t="n">
-        <v>0.7875</v>
+        <v>0.3333</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>0.1516</v>
+        <v>0.1005</v>
       </c>
       <c r="B15" t="n">
-        <v>0.1413</v>
+        <v>0.07580000000000001</v>
       </c>
       <c r="C15" t="n">
-        <v>0.7544</v>
+        <v>0.7325</v>
       </c>
       <c r="D15" t="n">
-        <v>0.1117</v>
+        <v>0.0919</v>
       </c>
       <c r="E15" t="n">
-        <v>-0.0019</v>
+        <v>0.3576</v>
       </c>
       <c r="F15" t="n">
-        <v>0.2227</v>
+        <v>0.3576</v>
       </c>
       <c r="G15" t="n">
-        <v>0.7792</v>
+        <v>0.29</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>0.1526</v>
+        <v>0.1017</v>
       </c>
       <c r="B16" t="n">
-        <v>0.141</v>
+        <v>0.0767</v>
       </c>
       <c r="C16" t="n">
-        <v>0.7628</v>
+        <v>0.7388</v>
       </c>
       <c r="D16" t="n">
-        <v>0.1128</v>
+        <v>0.0929</v>
       </c>
       <c r="E16" t="n">
-        <v>0.021</v>
+        <v>0.3651</v>
       </c>
       <c r="F16" t="n">
-        <v>0.2206</v>
+        <v>0.3651</v>
       </c>
       <c r="G16" t="n">
-        <v>0.7584</v>
+        <v>0.2867</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>0.153</v>
+        <v>0.103</v>
       </c>
       <c r="B17" t="n">
-        <v>0.141</v>
+        <v>0.07779999999999999</v>
       </c>
       <c r="C17" t="n">
-        <v>0.7662</v>
+        <v>0.7459</v>
       </c>
       <c r="D17" t="n">
-        <v>0.1133</v>
+        <v>0.0939</v>
       </c>
       <c r="E17" t="n">
-        <v>0.0316</v>
+        <v>0.3733</v>
       </c>
       <c r="F17" t="n">
-        <v>0.2196</v>
+        <v>0.3733</v>
       </c>
       <c r="G17" t="n">
-        <v>0.7488</v>
+        <v>0.2833</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>0.1541</v>
+        <v>0.1045</v>
       </c>
       <c r="B18" t="n">
-        <v>0.1412</v>
+        <v>0.0789</v>
       </c>
       <c r="C18" t="n">
-        <v>0.7731</v>
+        <v>0.7534999999999999</v>
       </c>
       <c r="D18" t="n">
-        <v>0.1143</v>
+        <v>0.0951</v>
       </c>
       <c r="E18" t="n">
-        <v>0.0577</v>
+        <v>0.3824</v>
       </c>
       <c r="F18" t="n">
-        <v>0.2172</v>
+        <v>0.3824</v>
       </c>
       <c r="G18" t="n">
-        <v>0.7251</v>
+        <v>0.28</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>0.1559</v>
+        <v>0.1061</v>
       </c>
       <c r="B19" t="n">
-        <v>0.1423</v>
+        <v>0.08019999999999999</v>
       </c>
       <c r="C19" t="n">
-        <v>0.7796</v>
+        <v>0.7617</v>
       </c>
       <c r="D19" t="n">
-        <v>0.1154</v>
+        <v>0.0965</v>
       </c>
       <c r="E19" t="n">
-        <v>0.0992</v>
+        <v>0.3923</v>
       </c>
       <c r="F19" t="n">
-        <v>0.2134</v>
+        <v>0.3923</v>
       </c>
       <c r="G19" t="n">
-        <v>0.6874</v>
+        <v>0.2767</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>0.1579</v>
+        <v>0.1079</v>
       </c>
       <c r="B20" t="n">
-        <v>0.1446</v>
+        <v>0.08169999999999999</v>
       </c>
       <c r="C20" t="n">
-        <v>0.7808</v>
+        <v>0.7703</v>
       </c>
       <c r="D20" t="n">
-        <v>0.1161</v>
+        <v>0.0979</v>
       </c>
       <c r="E20" t="n">
-        <v>0.1453</v>
+        <v>0.4029</v>
       </c>
       <c r="F20" t="n">
-        <v>0.2091</v>
+        <v>0.4029</v>
       </c>
       <c r="G20" t="n">
-        <v>0.6456</v>
+        <v>0.2733</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>0.16</v>
+        <v>0.1099</v>
       </c>
       <c r="B21" t="n">
-        <v>0.1484</v>
+        <v>0.0833</v>
       </c>
       <c r="C21" t="n">
-        <v>0.7753</v>
+        <v>0.7793</v>
       </c>
       <c r="D21" t="n">
-        <v>0.116</v>
+        <v>0.09950000000000001</v>
       </c>
       <c r="E21" t="n">
-        <v>0.1961</v>
+        <v>0.4144</v>
       </c>
       <c r="F21" t="n">
-        <v>0.2044</v>
+        <v>0.4144</v>
       </c>
       <c r="G21" t="n">
-        <v>0.5995</v>
+        <v>0.27</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>0.1624</v>
+        <v>0.112</v>
       </c>
       <c r="B22" t="n">
-        <v>0.154</v>
+        <v>0.08500000000000001</v>
       </c>
       <c r="C22" t="n">
-        <v>0.7625</v>
+        <v>0.7886</v>
       </c>
       <c r="D22" t="n">
-        <v>0.115</v>
+        <v>0.1012</v>
       </c>
       <c r="E22" t="n">
-        <v>0.2516</v>
+        <v>0.4267</v>
       </c>
       <c r="F22" t="n">
-        <v>0.1993</v>
+        <v>0.4267</v>
       </c>
       <c r="G22" t="n">
-        <v>0.5491</v>
+        <v>0.2667</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>0.165</v>
+        <v>0.1143</v>
       </c>
       <c r="B23" t="n">
-        <v>0.1615</v>
+        <v>0.0868</v>
       </c>
       <c r="C23" t="n">
-        <v>0.7427</v>
+        <v>0.7981</v>
       </c>
       <c r="D23" t="n">
-        <v>0.1128</v>
+        <v>0.103</v>
       </c>
       <c r="E23" t="n">
-        <v>0.3118</v>
+        <v>0.4397</v>
       </c>
       <c r="F23" t="n">
-        <v>0.1937</v>
+        <v>0.4397</v>
       </c>
       <c r="G23" t="n">
-        <v>0.4945</v>
+        <v>0.2633</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>0.1678</v>
+        <v>0.1167</v>
       </c>
       <c r="B24" t="n">
-        <v>0.1712</v>
+        <v>0.0888</v>
       </c>
       <c r="C24" t="n">
-        <v>0.717</v>
+        <v>0.8078</v>
       </c>
       <c r="D24" t="n">
-        <v>0.1091</v>
+        <v>0.1049</v>
       </c>
       <c r="E24" t="n">
-        <v>0.3766</v>
+        <v>0.4536</v>
       </c>
       <c r="F24" t="n">
-        <v>0.1877</v>
+        <v>0.4536</v>
       </c>
       <c r="G24" t="n">
-        <v>0.4356</v>
+        <v>0.26</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>0.1707</v>
+        <v>0.1193</v>
       </c>
       <c r="B25" t="n">
-        <v>0.183</v>
+        <v>0.09089999999999999</v>
       </c>
       <c r="C25" t="n">
-        <v>0.6869</v>
+        <v>0.8177</v>
       </c>
       <c r="D25" t="n">
-        <v>0.1037</v>
+        <v>0.1069</v>
       </c>
       <c r="E25" t="n">
-        <v>0.4462</v>
+        <v>0.4683</v>
       </c>
       <c r="F25" t="n">
-        <v>0.1813</v>
+        <v>0.4683</v>
       </c>
       <c r="G25" t="n">
-        <v>0.3725</v>
+        <v>0.2567</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>0.1739</v>
+        <v>0.1221</v>
       </c>
       <c r="B26" t="n">
-        <v>0.197</v>
+        <v>0.0931</v>
       </c>
       <c r="C26" t="n">
-        <v>0.6542</v>
+        <v>0.8276</v>
       </c>
       <c r="D26" t="n">
-        <v>0.0963</v>
+        <v>0.1091</v>
       </c>
       <c r="E26" t="n">
-        <v>0.5204</v>
+        <v>0.4837</v>
       </c>
       <c r="F26" t="n">
-        <v>0.1744</v>
+        <v>0.4837</v>
       </c>
       <c r="G26" t="n">
-        <v>0.3052</v>
+        <v>0.2533</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>0.1773</v>
+        <v>0.125</v>
       </c>
       <c r="B27" t="n">
-        <v>0.2131</v>
+        <v>0.0955</v>
       </c>
       <c r="C27" t="n">
-        <v>0.6206</v>
+        <v>0.8375</v>
       </c>
       <c r="D27" t="n">
-        <v>0.0864</v>
+        <v>0.1113</v>
       </c>
       <c r="E27" t="n">
-        <v>0.5993000000000001</v>
+        <v>0.5</v>
       </c>
       <c r="F27" t="n">
-        <v>0.1671</v>
+        <v>0.5</v>
       </c>
       <c r="G27" t="n">
-        <v>0.2336</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>0.1808</v>
+        <v>0.1281</v>
       </c>
       <c r="B28" t="n">
-        <v>0.2313</v>
+        <v>0.098</v>
       </c>
       <c r="C28" t="n">
-        <v>0.5873</v>
+        <v>0.8474</v>
       </c>
       <c r="D28" t="n">
-        <v>0.0738</v>
+        <v>0.1137</v>
       </c>
       <c r="E28" t="n">
-        <v>0.6829</v>
+        <v>0.5171</v>
       </c>
       <c r="F28" t="n">
-        <v>0.1594</v>
+        <v>0.5171</v>
       </c>
       <c r="G28" t="n">
-        <v>0.1577</v>
+        <v>0.2467</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>0.1846</v>
+        <v>0.1313</v>
       </c>
       <c r="B29" t="n">
-        <v>0.2515</v>
+        <v>0.1007</v>
       </c>
       <c r="C29" t="n">
-        <v>0.5552</v>
+        <v>0.8572</v>
       </c>
       <c r="D29" t="n">
-        <v>0.0581</v>
+        <v>0.1161</v>
       </c>
       <c r="E29" t="n">
-        <v>0.7712</v>
+        <v>0.5349</v>
       </c>
       <c r="F29" t="n">
-        <v>0.1512</v>
+        <v>0.5349</v>
       </c>
       <c r="G29" t="n">
-        <v>0.0776</v>
+        <v>0.2433</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>0.1886</v>
+        <v>0.1347</v>
       </c>
       <c r="B30" t="n">
-        <v>0.2735</v>
+        <v>0.1035</v>
       </c>
       <c r="C30" t="n">
-        <v>0.5249</v>
+        <v>0.8669</v>
       </c>
       <c r="D30" t="n">
-        <v>0.0389</v>
+        <v>0.1187</v>
       </c>
       <c r="E30" t="n">
-        <v>0.8641</v>
+        <v>0.5536</v>
       </c>
       <c r="F30" t="n">
-        <v>0.1427</v>
+        <v>0.5536</v>
       </c>
       <c r="G30" t="n">
-        <v>-0.0068</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>0.1927</v>
+        <v>0.1383</v>
       </c>
       <c r="B31" t="n">
-        <v>0.2974</v>
+        <v>0.1064</v>
       </c>
       <c r="C31" t="n">
-        <v>0.4968</v>
+        <v>0.8764999999999999</v>
       </c>
       <c r="D31" t="n">
-        <v>0.0158</v>
+        <v>0.1213</v>
       </c>
       <c r="E31" t="n">
-        <v>0.9618</v>
+        <v>0.5731000000000001</v>
       </c>
       <c r="F31" t="n">
-        <v>0.1336</v>
+        <v>0.5731000000000001</v>
       </c>
       <c r="G31" t="n">
-        <v>-0.0954</v>
+        <v>0.2367</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>0.1971</v>
+        <v>0.142</v>
       </c>
       <c r="B32" t="n">
-        <v>0.3231</v>
+        <v>0.1095</v>
       </c>
       <c r="C32" t="n">
-        <v>0.4708</v>
+        <v>0.8859</v>
       </c>
       <c r="D32" t="n">
-        <v>-0.0116</v>
+        <v>0.124</v>
       </c>
       <c r="E32" t="n">
-        <v>1.0641</v>
+        <v>0.5933</v>
       </c>
       <c r="F32" t="n">
-        <v>0.1242</v>
+        <v>0.5933</v>
       </c>
       <c r="G32" t="n">
-        <v>-0.1883</v>
+        <v>0.2333</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>0.2017</v>
+        <v>0.1459</v>
       </c>
       <c r="B33" t="n">
-        <v>0.3504</v>
+        <v>0.1127</v>
       </c>
       <c r="C33" t="n">
-        <v>0.4471</v>
+        <v>0.8952</v>
       </c>
       <c r="D33" t="n">
-        <v>-0.0439</v>
+        <v>0.1268</v>
       </c>
       <c r="E33" t="n">
-        <v>1.1711</v>
+        <v>0.6143999999999999</v>
       </c>
       <c r="F33" t="n">
-        <v>0.1143</v>
+        <v>0.6143999999999999</v>
       </c>
       <c r="G33" t="n">
-        <v>-0.2854</v>
+        <v>0.23</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>0.2065</v>
+        <v>0.1499</v>
       </c>
       <c r="B34" t="n">
-        <v>0.3794</v>
+        <v>0.116</v>
       </c>
       <c r="C34" t="n">
-        <v>0.4255</v>
+        <v>0.9042</v>
       </c>
       <c r="D34" t="n">
-        <v>-0.0815</v>
+        <v>0.1297</v>
       </c>
       <c r="E34" t="n">
-        <v>1.2828</v>
+        <v>0.6363</v>
       </c>
       <c r="F34" t="n">
-        <v>0.104</v>
+        <v>0.6363</v>
       </c>
       <c r="G34" t="n">
-        <v>-0.3867</v>
+        <v>0.2267</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>0.2114</v>
+        <v>0.1541</v>
       </c>
       <c r="B35" t="n">
-        <v>0.41</v>
+        <v>0.1195</v>
       </c>
       <c r="C35" t="n">
-        <v>0.4059</v>
+        <v>0.9131</v>
       </c>
       <c r="D35" t="n">
-        <v>-0.1248</v>
+        <v>0.1327</v>
       </c>
       <c r="E35" t="n">
-        <v>1.3992</v>
+        <v>0.6589</v>
       </c>
       <c r="F35" t="n">
-        <v>0.09320000000000001</v>
+        <v>0.6589</v>
       </c>
       <c r="G35" t="n">
-        <v>-0.4923</v>
+        <v>0.2233</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>0.2166</v>
+        <v>0.1585</v>
       </c>
       <c r="B36" t="n">
-        <v>0.4422</v>
+        <v>0.1231</v>
       </c>
       <c r="C36" t="n">
-        <v>0.3881</v>
+        <v>0.9217</v>
       </c>
       <c r="D36" t="n">
-        <v>-0.1745</v>
+        <v>0.1357</v>
       </c>
       <c r="E36" t="n">
-        <v>1.5202</v>
+        <v>0.6824</v>
       </c>
       <c r="F36" t="n">
-        <v>0.082</v>
+        <v>0.6824</v>
       </c>
       <c r="G36" t="n">
-        <v>-0.6022</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>0.222</v>
+        <v>0.163</v>
       </c>
       <c r="B37" t="n">
-        <v>0.4759</v>
+        <v>0.1269</v>
       </c>
       <c r="C37" t="n">
-        <v>0.3719</v>
+        <v>0.9301</v>
       </c>
       <c r="D37" t="n">
-        <v>-0.2309</v>
+        <v>0.1389</v>
       </c>
       <c r="E37" t="n">
-        <v>1.6459</v>
+        <v>0.7067</v>
       </c>
       <c r="F37" t="n">
-        <v>0.0704</v>
+        <v>0.7067</v>
       </c>
       <c r="G37" t="n">
-        <v>-0.7163</v>
+        <v>0.2167</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>0.2275</v>
+        <v>0.1677</v>
       </c>
       <c r="B38" t="n">
-        <v>0.5111</v>
+        <v>0.1308</v>
       </c>
       <c r="C38" t="n">
-        <v>0.3572</v>
+        <v>0.9382</v>
       </c>
       <c r="D38" t="n">
-        <v>-0.2948</v>
+        <v>0.142</v>
       </c>
       <c r="E38" t="n">
-        <v>1.7764</v>
+        <v>0.7317</v>
       </c>
       <c r="F38" t="n">
-        <v>0.0583</v>
+        <v>0.7317</v>
       </c>
       <c r="G38" t="n">
-        <v>-0.8347</v>
+        <v>0.2133</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>0.2333</v>
+        <v>0.1725</v>
       </c>
       <c r="B39" t="n">
-        <v>0.5477</v>
+        <v>0.1348</v>
       </c>
       <c r="C39" t="n">
-        <v>0.3438</v>
+        <v>0.9461000000000001</v>
       </c>
       <c r="D39" t="n">
-        <v>-0.3667</v>
+        <v>0.1453</v>
       </c>
       <c r="E39" t="n">
-        <v>1.9115</v>
+        <v>0.7576000000000001</v>
       </c>
       <c r="F39" t="n">
-        <v>0.0458</v>
+        <v>0.7576000000000001</v>
       </c>
       <c r="G39" t="n">
-        <v>-0.9573</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>0.2393</v>
+        <v>0.1775</v>
       </c>
       <c r="B40" t="n">
-        <v>0.5858</v>
+        <v>0.1389</v>
       </c>
       <c r="C40" t="n">
-        <v>0.3316</v>
+        <v>0.9538</v>
       </c>
       <c r="D40" t="n">
-        <v>-0.4471</v>
+        <v>0.1486</v>
       </c>
       <c r="E40" t="n">
-        <v>2.0513</v>
+        <v>0.7843</v>
       </c>
       <c r="F40" t="n">
-        <v>0.0329</v>
+        <v>0.7843</v>
       </c>
       <c r="G40" t="n">
-        <v>-1.0842</v>
+        <v>0.2067</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>0.2454</v>
+        <v>0.1827</v>
       </c>
       <c r="B41" t="n">
-        <v>0.6254</v>
+        <v>0.1432</v>
       </c>
       <c r="C41" t="n">
-        <v>0.3205</v>
+        <v>0.9613</v>
       </c>
       <c r="D41" t="n">
-        <v>-0.5368000000000001</v>
+        <v>0.1519</v>
       </c>
       <c r="E41" t="n">
-        <v>2.1957</v>
+        <v>0.8117</v>
       </c>
       <c r="F41" t="n">
-        <v>0.0196</v>
+        <v>0.8117</v>
       </c>
       <c r="G41" t="n">
-        <v>-1.2153</v>
+        <v>0.2033</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>0.2518</v>
+        <v>0.188</v>
       </c>
       <c r="B42" t="n">
-        <v>0.6664</v>
+        <v>0.1477</v>
       </c>
       <c r="C42" t="n">
-        <v>0.3104</v>
+        <v>0.9684</v>
       </c>
       <c r="D42" t="n">
-        <v>-0.6363</v>
+        <v>0.1553</v>
       </c>
       <c r="E42" t="n">
-        <v>2.3449</v>
+        <v>0.84</v>
       </c>
       <c r="F42" t="n">
-        <v>0.0058</v>
+        <v>0.84</v>
       </c>
       <c r="G42" t="n">
-        <v>-1.3507</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>0.2584</v>
+        <v>0.1935</v>
       </c>
       <c r="B43" t="n">
-        <v>0.7088</v>
+        <v>0.1522</v>
       </c>
       <c r="C43" t="n">
-        <v>0.3011</v>
+        <v>0.9754</v>
       </c>
       <c r="D43" t="n">
-        <v>-0.7463</v>
+        <v>0.1587</v>
       </c>
       <c r="E43" t="n">
-        <v>2.4987</v>
+        <v>0.8691</v>
       </c>
       <c r="F43" t="n">
-        <v>-0.008399999999999999</v>
+        <v>0.8691</v>
       </c>
       <c r="G43" t="n">
-        <v>-1.4903</v>
+        <v>0.1967</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>0.2652</v>
+        <v>0.1991</v>
       </c>
       <c r="B44" t="n">
-        <v>0.7524999999999999</v>
+        <v>0.1569</v>
       </c>
       <c r="C44" t="n">
-        <v>0.2925</v>
+        <v>0.9821</v>
       </c>
       <c r="D44" t="n">
-        <v>-0.8675</v>
+        <v>0.1622</v>
       </c>
       <c r="E44" t="n">
-        <v>2.6572</v>
+        <v>0.8989</v>
       </c>
       <c r="F44" t="n">
-        <v>-0.0231</v>
+        <v>0.8989</v>
       </c>
       <c r="G44" t="n">
-        <v>-1.6341</v>
+        <v>0.1933</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>0.2721</v>
+        <v>0.2049</v>
       </c>
       <c r="B45" t="n">
-        <v>0.7977</v>
+        <v>0.1618</v>
       </c>
       <c r="C45" t="n">
-        <v>0.2847</v>
+        <v>0.9886</v>
       </c>
       <c r="D45" t="n">
-        <v>-1.0006</v>
+        <v>0.1657</v>
       </c>
       <c r="E45" t="n">
-        <v>2.8204</v>
+        <v>0.9296</v>
       </c>
       <c r="F45" t="n">
-        <v>-0.0382</v>
+        <v>0.9296</v>
       </c>
       <c r="G45" t="n">
-        <v>-1.7822</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>0.2793</v>
+        <v>0.2109</v>
       </c>
       <c r="B46" t="n">
-        <v>0.8443000000000001</v>
+        <v>0.1667</v>
       </c>
       <c r="C46" t="n">
-        <v>0.2775</v>
+        <v>0.9949</v>
       </c>
       <c r="D46" t="n">
-        <v>-1.1464</v>
+        <v>0.1692</v>
       </c>
       <c r="E46" t="n">
-        <v>2.9883</v>
+        <v>0.9611</v>
       </c>
       <c r="F46" t="n">
-        <v>-0.0537</v>
+        <v>0.9611</v>
       </c>
       <c r="G46" t="n">
-        <v>-1.9346</v>
+        <v>0.1867</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>0.2867</v>
+        <v>0.217</v>
       </c>
       <c r="B47" t="n">
-        <v>0.8922</v>
+        <v>0.1718</v>
       </c>
       <c r="C47" t="n">
-        <v>0.2708</v>
+        <v>1.001</v>
       </c>
       <c r="D47" t="n">
-        <v>-1.3055</v>
+        <v>0.1727</v>
       </c>
       <c r="E47" t="n">
-        <v>3.1609</v>
+        <v>0.9933</v>
       </c>
       <c r="F47" t="n">
-        <v>-0.0697</v>
+        <v>0.9933</v>
       </c>
       <c r="G47" t="n">
-        <v>-2.0912</v>
+        <v>0.1833</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>0.2942</v>
+        <v>0.2233</v>
       </c>
       <c r="B48" t="n">
-        <v>0.9415</v>
+        <v>0.1771</v>
       </c>
       <c r="C48" t="n">
-        <v>0.2647</v>
+        <v>1.0068</v>
       </c>
       <c r="D48" t="n">
-        <v>-1.4788</v>
+        <v>0.1762</v>
       </c>
       <c r="E48" t="n">
-        <v>3.3381</v>
+        <v>1.0264</v>
       </c>
       <c r="F48" t="n">
-        <v>-0.08599999999999999</v>
+        <v>1.0264</v>
       </c>
       <c r="G48" t="n">
-        <v>-2.2521</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>0.302</v>
+        <v>0.2297</v>
       </c>
       <c r="B49" t="n">
-        <v>0.9922</v>
+        <v>0.1824</v>
       </c>
       <c r="C49" t="n">
-        <v>0.259</v>
+        <v>1.0125</v>
       </c>
       <c r="D49" t="n">
-        <v>-1.667</v>
+        <v>0.1798</v>
       </c>
       <c r="E49" t="n">
-        <v>3.5201</v>
+        <v>1.0603</v>
       </c>
       <c r="F49" t="n">
-        <v>-0.1029</v>
+        <v>1.0603</v>
       </c>
       <c r="G49" t="n">
-        <v>-2.4172</v>
+        <v>0.1767</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>0.31</v>
+        <v>0.2363</v>
       </c>
       <c r="B50" t="n">
-        <v>1.0442</v>
+        <v>0.188</v>
       </c>
       <c r="C50" t="n">
-        <v>0.2537</v>
+        <v>1.0179</v>
       </c>
       <c r="D50" t="n">
-        <v>-1.8709</v>
+        <v>0.1833</v>
       </c>
       <c r="E50" t="n">
-        <v>3.7067</v>
+        <v>1.0949</v>
       </c>
       <c r="F50" t="n">
-        <v>-0.1201</v>
+        <v>1.0949</v>
       </c>
       <c r="G50" t="n">
-        <v>-2.5866</v>
+        <v>0.1733</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>0.3181</v>
+        <v>0.2431</v>
       </c>
       <c r="B51" t="n">
-        <v>1.0976</v>
+        <v>0.1936</v>
       </c>
       <c r="C51" t="n">
-        <v>0.2488</v>
+        <v>1.0232</v>
       </c>
       <c r="D51" t="n">
-        <v>-2.0915</v>
+        <v>0.1869</v>
       </c>
       <c r="E51" t="n">
-        <v>3.898</v>
+        <v>1.1304</v>
       </c>
       <c r="F51" t="n">
-        <v>-0.1378</v>
+        <v>1.1304</v>
       </c>
       <c r="G51" t="n">
-        <v>-2.7602</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>0.3265</v>
+        <v>0.25</v>
       </c>
       <c r="B52" t="n">
-        <v>1.1524</v>
+        <v>0.1994</v>
       </c>
       <c r="C52" t="n">
-        <v>0.2443</v>
+        <v>1.0282</v>
       </c>
       <c r="D52" t="n">
-        <v>-2.3294</v>
+        <v>0.1904</v>
       </c>
       <c r="E52" t="n">
-        <v>4.094</v>
+        <v>1.1667</v>
       </c>
       <c r="F52" t="n">
-        <v>-0.1559</v>
+        <v>1.1667</v>
       </c>
       <c r="G52" t="n">
-        <v>-2.9381</v>
+        <v>0.1667</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>0.3351</v>
+        <v>0.2571</v>
       </c>
       <c r="B53" t="n">
-        <v>1.2085</v>
+        <v>0.2053</v>
       </c>
       <c r="C53" t="n">
-        <v>0.24</v>
+        <v>1.0331</v>
       </c>
       <c r="D53" t="n">
-        <v>-2.5857</v>
+        <v>0.1939</v>
       </c>
       <c r="E53" t="n">
-        <v>4.2946</v>
+        <v>1.2037</v>
       </c>
       <c r="F53" t="n">
-        <v>-0.1745</v>
+        <v>1.2037</v>
       </c>
       <c r="G53" t="n">
-        <v>-3.1202</v>
+        <v>0.1633</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>0.3438</v>
+        <v>0.2643</v>
       </c>
       <c r="B54" t="n">
-        <v>1.2659</v>
+        <v>0.2113</v>
       </c>
       <c r="C54" t="n">
-        <v>0.2361</v>
+        <v>1.0378</v>
       </c>
       <c r="D54" t="n">
-        <v>-2.8612</v>
+        <v>0.1973</v>
       </c>
       <c r="E54" t="n">
-        <v>4.5</v>
+        <v>1.2416</v>
       </c>
       <c r="F54" t="n">
-        <v>-0.1934</v>
+        <v>1.2416</v>
       </c>
       <c r="G54" t="n">
-        <v>-3.3065</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>0.3528</v>
+        <v>0.2717</v>
       </c>
       <c r="B55" t="n">
-        <v>1.3247</v>
+        <v>0.2175</v>
       </c>
       <c r="C55" t="n">
-        <v>0.2324</v>
+        <v>1.0424</v>
       </c>
       <c r="D55" t="n">
-        <v>-3.1568</v>
+        <v>0.2008</v>
       </c>
       <c r="E55" t="n">
-        <v>4.71</v>
+        <v>1.2803</v>
       </c>
       <c r="F55" t="n">
-        <v>-0.2129</v>
+        <v>1.2803</v>
       </c>
       <c r="G55" t="n">
-        <v>-3.4972</v>
+        <v>0.1567</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>0.362</v>
+        <v>0.2793</v>
       </c>
       <c r="B56" t="n">
-        <v>1.3848</v>
+        <v>0.2238</v>
       </c>
       <c r="C56" t="n">
-        <v>0.2289</v>
+        <v>1.0467</v>
       </c>
       <c r="D56" t="n">
-        <v>-3.4734</v>
+        <v>0.2041</v>
       </c>
       <c r="E56" t="n">
-        <v>4.9247</v>
+        <v>1.3197</v>
       </c>
       <c r="F56" t="n">
-        <v>-0.2327</v>
+        <v>1.3197</v>
       </c>
       <c r="G56" t="n">
-        <v>-3.692</v>
+        <v>0.1533</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>0.3714</v>
+        <v>0.287</v>
       </c>
       <c r="B57" t="n">
-        <v>1.4463</v>
+        <v>0.2303</v>
       </c>
       <c r="C57" t="n">
-        <v>0.2257</v>
+        <v>1.051</v>
       </c>
       <c r="D57" t="n">
-        <v>-3.812</v>
+        <v>0.2075</v>
       </c>
       <c r="E57" t="n">
-        <v>5.1441</v>
+        <v>1.36</v>
       </c>
       <c r="F57" t="n">
-        <v>-0.253</v>
+        <v>1.36</v>
       </c>
       <c r="G57" t="n">
-        <v>-3.8912</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>0.3809</v>
+        <v>0.2949</v>
       </c>
       <c r="B58" t="n">
-        <v>1.5091</v>
+        <v>0.2368</v>
       </c>
       <c r="C58" t="n">
-        <v>0.2226</v>
+        <v>1.0551</v>
       </c>
       <c r="D58" t="n">
-        <v>-4.1737</v>
+        <v>0.2107</v>
       </c>
       <c r="E58" t="n">
-        <v>5.3682</v>
+        <v>1.4011</v>
       </c>
       <c r="F58" t="n">
-        <v>-0.2737</v>
+        <v>1.4011</v>
       </c>
       <c r="G58" t="n">
-        <v>-4.0945</v>
+        <v>0.1467</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>0.3907</v>
+        <v>0.3029</v>
       </c>
       <c r="B59" t="n">
-        <v>1.5732</v>
+        <v>0.2435</v>
       </c>
       <c r="C59" t="n">
-        <v>0.2197</v>
+        <v>1.059</v>
       </c>
       <c r="D59" t="n">
-        <v>-4.5593</v>
+        <v>0.2139</v>
       </c>
       <c r="E59" t="n">
-        <v>5.597</v>
+        <v>1.4429</v>
       </c>
       <c r="F59" t="n">
-        <v>-0.2948</v>
+        <v>1.4429</v>
       </c>
       <c r="G59" t="n">
-        <v>-4.3021</v>
+        <v>0.1433</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>0.4007</v>
+        <v>0.3111</v>
       </c>
       <c r="B60" t="n">
-        <v>1.6387</v>
+        <v>0.2504</v>
       </c>
       <c r="C60" t="n">
-        <v>0.217</v>
+        <v>1.0628</v>
       </c>
       <c r="D60" t="n">
-        <v>-4.9699</v>
+        <v>0.2171</v>
       </c>
       <c r="E60" t="n">
-        <v>5.8304</v>
+        <v>1.4856</v>
       </c>
       <c r="F60" t="n">
-        <v>-0.3164</v>
+        <v>1.4856</v>
       </c>
       <c r="G60" t="n">
-        <v>-4.514</v>
+        <v>0.14</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>0.4108</v>
+        <v>0.3195</v>
       </c>
       <c r="B61" t="n">
-        <v>1.7055</v>
+        <v>0.2574</v>
       </c>
       <c r="C61" t="n">
-        <v>0.2145</v>
+        <v>1.0665</v>
       </c>
       <c r="D61" t="n">
-        <v>-5.4065</v>
+        <v>0.2201</v>
       </c>
       <c r="E61" t="n">
-        <v>6.0686</v>
+        <v>1.5291</v>
       </c>
       <c r="F61" t="n">
-        <v>-0.3384</v>
+        <v>1.5291</v>
       </c>
       <c r="G61" t="n">
-        <v>-4.7301</v>
+        <v>0.1367</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>0.4212</v>
+        <v>0.328</v>
       </c>
       <c r="B62" t="n">
-        <v>1.7736</v>
+        <v>0.2645</v>
       </c>
       <c r="C62" t="n">
-        <v>0.2121</v>
+        <v>1.07</v>
       </c>
       <c r="D62" t="n">
-        <v>-5.8703</v>
+        <v>0.2231</v>
       </c>
       <c r="E62" t="n">
-        <v>6.3114</v>
+        <v>1.5733</v>
       </c>
       <c r="F62" t="n">
-        <v>-0.3609</v>
+        <v>1.5733</v>
       </c>
       <c r="G62" t="n">
-        <v>-4.9505</v>
+        <v>0.1333</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>0.4318</v>
+        <v>0.3367</v>
       </c>
       <c r="B63" t="n">
-        <v>1.8431</v>
+        <v>0.2717</v>
       </c>
       <c r="C63" t="n">
-        <v>0.2099</v>
+        <v>1.0734</v>
       </c>
       <c r="D63" t="n">
-        <v>-6.3622</v>
+        <v>0.2259</v>
       </c>
       <c r="E63" t="n">
-        <v>6.5589</v>
+        <v>1.6184</v>
       </c>
       <c r="F63" t="n">
-        <v>-0.3838</v>
+        <v>1.6184</v>
       </c>
       <c r="G63" t="n">
-        <v>-5.1751</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>0.4425</v>
+        <v>0.3455</v>
       </c>
       <c r="B64" t="n">
-        <v>1.9139</v>
+        <v>0.2791</v>
       </c>
       <c r="C64" t="n">
-        <v>0.2077</v>
+        <v>1.0768</v>
       </c>
       <c r="D64" t="n">
-        <v>-6.8834</v>
+        <v>0.2287</v>
       </c>
       <c r="E64" t="n">
-        <v>6.8111</v>
+        <v>1.6643</v>
       </c>
       <c r="F64" t="n">
-        <v>-0.4071</v>
+        <v>1.6643</v>
       </c>
       <c r="G64" t="n">
-        <v>-5.404</v>
+        <v>0.1267</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>0.4535</v>
+        <v>0.3545</v>
       </c>
       <c r="B65" t="n">
-        <v>1.986</v>
+        <v>0.2866</v>
       </c>
       <c r="C65" t="n">
-        <v>0.2057</v>
+        <v>1.0799</v>
       </c>
       <c r="D65" t="n">
-        <v>-7.435</v>
+        <v>0.2313</v>
       </c>
       <c r="E65" t="n">
-        <v>7.0679</v>
+        <v>1.7109</v>
       </c>
       <c r="F65" t="n">
-        <v>-0.4308</v>
+        <v>1.7109</v>
       </c>
       <c r="G65" t="n">
-        <v>-5.6371</v>
+        <v>0.1233</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>0.4647</v>
+        <v>0.3637</v>
       </c>
       <c r="B66" t="n">
-        <v>2.0595</v>
+        <v>0.2942</v>
       </c>
       <c r="C66" t="n">
-        <v>0.2038</v>
+        <v>1.083</v>
       </c>
       <c r="D66" t="n">
-        <v>-8.0182</v>
+        <v>0.2338</v>
       </c>
       <c r="E66" t="n">
-        <v>7.3295</v>
+        <v>1.7584</v>
       </c>
       <c r="F66" t="n">
-        <v>-0.455</v>
+        <v>1.7584</v>
       </c>
       <c r="G66" t="n">
-        <v>-5.8745</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>0.4761</v>
+        <v>0.373</v>
       </c>
       <c r="B67" t="n">
-        <v>2.1343</v>
+        <v>0.302</v>
       </c>
       <c r="C67" t="n">
-        <v>0.202</v>
+        <v>1.086</v>
       </c>
       <c r="D67" t="n">
-        <v>-8.6341</v>
+        <v>0.2362</v>
       </c>
       <c r="E67" t="n">
-        <v>7.5957</v>
+        <v>1.8067</v>
       </c>
       <c r="F67" t="n">
-        <v>-0.4796</v>
+        <v>1.8067</v>
       </c>
       <c r="G67" t="n">
-        <v>-6.1161</v>
+        <v>0.1167</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>0.4876</v>
+        <v>0.3825</v>
       </c>
       <c r="B68" t="n">
-        <v>2.2104</v>
+        <v>0.3099</v>
       </c>
       <c r="C68" t="n">
-        <v>0.2002</v>
+        <v>1.0889</v>
       </c>
       <c r="D68" t="n">
-        <v>-9.283899999999999</v>
+        <v>0.2384</v>
       </c>
       <c r="E68" t="n">
-        <v>7.8666</v>
+        <v>1.8557</v>
       </c>
       <c r="F68" t="n">
-        <v>-0.5046</v>
+        <v>1.8557</v>
       </c>
       <c r="G68" t="n">
-        <v>-6.362</v>
+        <v>0.1133</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>0.4994</v>
+        <v>0.3921</v>
       </c>
       <c r="B69" t="n">
-        <v>2.2878</v>
+        <v>0.318</v>
       </c>
       <c r="C69" t="n">
-        <v>0.1986</v>
+        <v>1.0917</v>
       </c>
       <c r="D69" t="n">
-        <v>-9.9687</v>
+        <v>0.2405</v>
       </c>
       <c r="E69" t="n">
-        <v>8.142200000000001</v>
+        <v>1.9056</v>
       </c>
       <c r="F69" t="n">
-        <v>-0.5301</v>
+        <v>1.9056</v>
       </c>
       <c r="G69" t="n">
-        <v>-6.6121</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>0.5114</v>
+        <v>0.4019</v>
       </c>
       <c r="B70" t="n">
-        <v>2.3666</v>
+        <v>0.3261</v>
       </c>
       <c r="C70" t="n">
-        <v>0.1971</v>
+        <v>1.0944</v>
       </c>
       <c r="D70" t="n">
-        <v>-10.69</v>
+        <v>0.2424</v>
       </c>
       <c r="E70" t="n">
-        <v>8.422499999999999</v>
+        <v>1.9563</v>
       </c>
       <c r="F70" t="n">
-        <v>-0.556</v>
+        <v>1.9563</v>
       </c>
       <c r="G70" t="n">
-        <v>-6.8665</v>
+        <v>0.1067</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>0.5235</v>
+        <v>0.4119</v>
       </c>
       <c r="B71" t="n">
-        <v>2.4467</v>
+        <v>0.3344</v>
       </c>
       <c r="C71" t="n">
-        <v>0.1956</v>
+        <v>1.097</v>
       </c>
       <c r="D71" t="n">
-        <v>-11.4488</v>
+        <v>0.2441</v>
       </c>
       <c r="E71" t="n">
-        <v>8.7075</v>
+        <v>2.0077</v>
       </c>
       <c r="F71" t="n">
-        <v>-0.5824</v>
+        <v>2.0077</v>
       </c>
       <c r="G71" t="n">
-        <v>-7.1251</v>
+        <v>0.1033</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>0.5359</v>
+        <v>0.422</v>
       </c>
       <c r="B72" t="n">
-        <v>2.5281</v>
+        <v>0.3429</v>
       </c>
       <c r="C72" t="n">
-        <v>0.1942</v>
+        <v>1.0995</v>
       </c>
       <c r="D72" t="n">
-        <v>-12.2465</v>
+        <v>0.2457</v>
       </c>
       <c r="E72" t="n">
-        <v>8.9971</v>
+        <v>2.06</v>
       </c>
       <c r="F72" t="n">
-        <v>-0.6091</v>
+        <v>2.06</v>
       </c>
       <c r="G72" t="n">
-        <v>-7.3879</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>0.5485</v>
+        <v>0.4323</v>
       </c>
       <c r="B73" t="n">
-        <v>2.6108</v>
+        <v>0.3514</v>
       </c>
       <c r="C73" t="n">
-        <v>0.1928</v>
+        <v>1.102</v>
       </c>
       <c r="D73" t="n">
-        <v>-13.0843</v>
+        <v>0.247</v>
       </c>
       <c r="E73" t="n">
-        <v>9.291399999999999</v>
+        <v>2.1131</v>
       </c>
       <c r="F73" t="n">
-        <v>-0.6364</v>
+        <v>2.1131</v>
       </c>
       <c r="G73" t="n">
-        <v>-7.6551</v>
+        <v>0.09669999999999999</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>0.5612</v>
+        <v>0.4427</v>
       </c>
       <c r="B74" t="n">
-        <v>2.6949</v>
+        <v>0.3601</v>
       </c>
       <c r="C74" t="n">
-        <v>0.1916</v>
+        <v>1.1044</v>
       </c>
       <c r="D74" t="n">
-        <v>-13.9636</v>
+        <v>0.2482</v>
       </c>
       <c r="E74" t="n">
-        <v>9.590400000000001</v>
+        <v>2.1669</v>
       </c>
       <c r="F74" t="n">
-        <v>-0.664</v>
+        <v>2.1669</v>
       </c>
       <c r="G74" t="n">
-        <v>-7.9264</v>
+        <v>0.09329999999999999</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>0.5742</v>
+        <v>0.4533</v>
       </c>
       <c r="B75" t="n">
-        <v>2.7803</v>
+        <v>0.369</v>
       </c>
       <c r="C75" t="n">
-        <v>0.1903</v>
+        <v>1.1066</v>
       </c>
       <c r="D75" t="n">
-        <v>-14.8856</v>
+        <v>0.2491</v>
       </c>
       <c r="E75" t="n">
-        <v>9.8941</v>
+        <v>2.2216</v>
       </c>
       <c r="F75" t="n">
-        <v>-0.6921</v>
+        <v>2.2216</v>
       </c>
       <c r="G75" t="n">
-        <v>-8.2021</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>0.5874</v>
+        <v>0.4641</v>
       </c>
       <c r="B76" t="n">
-        <v>2.867</v>
+        <v>0.3779</v>
       </c>
       <c r="C76" t="n">
-        <v>0.1892</v>
+        <v>1.1089</v>
       </c>
       <c r="D76" t="n">
-        <v>-15.8518</v>
+        <v>0.2498</v>
       </c>
       <c r="E76" t="n">
-        <v>10.2025</v>
+        <v>2.2771</v>
       </c>
       <c r="F76" t="n">
-        <v>-0.7206</v>
+        <v>2.2771</v>
       </c>
       <c r="G76" t="n">
-        <v>-8.4819</v>
+        <v>0.0867</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>0.6008</v>
+        <v>0.475</v>
       </c>
       <c r="B77" t="n">
-        <v>2.955</v>
+        <v>0.387</v>
       </c>
       <c r="C77" t="n">
-        <v>0.1881</v>
+        <v>1.111</v>
       </c>
       <c r="D77" t="n">
-        <v>-16.8636</v>
+        <v>0.2503</v>
       </c>
       <c r="E77" t="n">
-        <v>10.5156</v>
+        <v>2.3333</v>
       </c>
       <c r="F77" t="n">
-        <v>-0.7495000000000001</v>
+        <v>2.3333</v>
       </c>
       <c r="G77" t="n">
-        <v>-8.7661</v>
+        <v>0.0833</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>0.6143</v>
+        <v>0.4861</v>
       </c>
       <c r="B78" t="n">
-        <v>3.0444</v>
+        <v>0.3963</v>
       </c>
       <c r="C78" t="n">
-        <v>0.187</v>
+        <v>1.1131</v>
       </c>
       <c r="D78" t="n">
-        <v>-17.9222</v>
+        <v>0.2506</v>
       </c>
       <c r="E78" t="n">
-        <v>10.8333</v>
+        <v>2.3904</v>
       </c>
       <c r="F78" t="n">
-        <v>-0.7789</v>
+        <v>2.3904</v>
       </c>
       <c r="G78" t="n">
-        <v>-9.054399999999999</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>0.6281</v>
+        <v>0.4973</v>
       </c>
       <c r="B79" t="n">
-        <v>3.1351</v>
+        <v>0.4056</v>
       </c>
       <c r="C79" t="n">
-        <v>0.186</v>
+        <v>1.1151</v>
       </c>
       <c r="D79" t="n">
-        <v>-19.0291</v>
+        <v>0.2505</v>
       </c>
       <c r="E79" t="n">
-        <v>11.1557</v>
+        <v>2.4483</v>
       </c>
       <c r="F79" t="n">
-        <v>-0.8087</v>
+        <v>2.4483</v>
       </c>
       <c r="G79" t="n">
-        <v>-9.347099999999999</v>
+        <v>0.0767</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>0.6421</v>
+        <v>0.5087</v>
       </c>
       <c r="B80" t="n">
-        <v>3.2271</v>
+        <v>0.4151</v>
       </c>
       <c r="C80" t="n">
-        <v>0.185</v>
+        <v>1.1171</v>
       </c>
       <c r="D80" t="n">
-        <v>-20.1859</v>
+        <v>0.2502</v>
       </c>
       <c r="E80" t="n">
-        <v>11.4829</v>
+        <v>2.5069</v>
       </c>
       <c r="F80" t="n">
-        <v>-0.8389</v>
+        <v>2.5069</v>
       </c>
       <c r="G80" t="n">
-        <v>-9.6439</v>
+        <v>0.0733</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>0.6562</v>
+        <v>0.5203</v>
       </c>
       <c r="B81" t="n">
-        <v>3.3204</v>
+        <v>0.4247</v>
       </c>
       <c r="C81" t="n">
-        <v>0.1841</v>
+        <v>1.119</v>
       </c>
       <c r="D81" t="n">
-        <v>-21.3938</v>
+        <v>0.2497</v>
       </c>
       <c r="E81" t="n">
-        <v>11.8146</v>
+        <v>2.5664</v>
       </c>
       <c r="F81" t="n">
-        <v>-0.8696</v>
+        <v>2.5664</v>
       </c>
       <c r="G81" t="n">
-        <v>-9.945</v>
+        <v>0.07000000000000001</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>0.6706</v>
+        <v>0.532</v>
       </c>
       <c r="B82" t="n">
-        <v>3.415</v>
+        <v>0.4345</v>
       </c>
       <c r="C82" t="n">
-        <v>0.1832</v>
+        <v>1.1209</v>
       </c>
       <c r="D82" t="n">
-        <v>-22.6544</v>
+        <v>0.2488</v>
       </c>
       <c r="E82" t="n">
-        <v>12.1511</v>
+        <v>2.6267</v>
       </c>
       <c r="F82" t="n">
-        <v>-0.9006999999999999</v>
+        <v>2.6267</v>
       </c>
       <c r="G82" t="n">
-        <v>-10.2504</v>
+        <v>0.0667</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>0.6852</v>
+        <v>0.5439000000000001</v>
       </c>
       <c r="B83" t="n">
-        <v>3.511</v>
+        <v>0.4444</v>
       </c>
       <c r="C83" t="n">
-        <v>0.1823</v>
+        <v>1.1227</v>
       </c>
       <c r="D83" t="n">
-        <v>-23.9692</v>
+        <v>0.2477</v>
       </c>
       <c r="E83" t="n">
-        <v>12.4923</v>
+        <v>2.6877</v>
       </c>
       <c r="F83" t="n">
-        <v>-0.9322</v>
+        <v>2.6877</v>
       </c>
       <c r="G83" t="n">
-        <v>-10.56</v>
+        <v>0.0633</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>0.6999</v>
+        <v>0.5558999999999999</v>
       </c>
       <c r="B84" t="n">
-        <v>3.6083</v>
+        <v>0.4544</v>
       </c>
       <c r="C84" t="n">
-        <v>0.1815</v>
+        <v>1.1244</v>
       </c>
       <c r="D84" t="n">
-        <v>-25.3398</v>
+        <v>0.2462</v>
       </c>
       <c r="E84" t="n">
-        <v>12.8381</v>
+        <v>2.7496</v>
       </c>
       <c r="F84" t="n">
-        <v>-0.9641999999999999</v>
+        <v>2.7496</v>
       </c>
       <c r="G84" t="n">
-        <v>-10.8739</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>0.7149</v>
+        <v>0.5681</v>
       </c>
       <c r="B85" t="n">
-        <v>3.7069</v>
+        <v>0.4645</v>
       </c>
       <c r="C85" t="n">
-        <v>0.1807</v>
+        <v>1.1261</v>
       </c>
       <c r="D85" t="n">
-        <v>-26.7676</v>
+        <v>0.2444</v>
       </c>
       <c r="E85" t="n">
-        <v>13.1887</v>
+        <v>2.8123</v>
       </c>
       <c r="F85" t="n">
-        <v>-0.9966</v>
+        <v>2.8123</v>
       </c>
       <c r="G85" t="n">
-        <v>-11.192</v>
+        <v>0.0567</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>0.7301</v>
+        <v>0.5805</v>
       </c>
       <c r="B86" t="n">
-        <v>3.8069</v>
+        <v>0.4748</v>
       </c>
       <c r="C86" t="n">
-        <v>0.18</v>
+        <v>1.1277</v>
       </c>
       <c r="D86" t="n">
-        <v>-28.2542</v>
+        <v>0.2423</v>
       </c>
       <c r="E86" t="n">
-        <v>13.5439</v>
+        <v>2.8757</v>
       </c>
       <c r="F86" t="n">
-        <v>-1.0294</v>
+        <v>2.8757</v>
       </c>
       <c r="G86" t="n">
-        <v>-11.5144</v>
+        <v>0.0533</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>0.7455000000000001</v>
+        <v>0.593</v>
       </c>
       <c r="B87" t="n">
-        <v>3.9081</v>
+        <v>0.4852</v>
       </c>
       <c r="C87" t="n">
-        <v>0.1792</v>
+        <v>1.1293</v>
       </c>
       <c r="D87" t="n">
-        <v>-29.8012</v>
+        <v>0.2398</v>
       </c>
       <c r="E87" t="n">
-        <v>13.9038</v>
+        <v>2.94</v>
       </c>
       <c r="F87" t="n">
-        <v>-1.0627</v>
+        <v>2.94</v>
       </c>
       <c r="G87" t="n">
-        <v>-11.841</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>0.761</v>
+        <v>0.6057</v>
       </c>
       <c r="B88" t="n">
-        <v>4.0107</v>
+        <v>0.4958</v>
       </c>
       <c r="C88" t="n">
-        <v>0.1785</v>
+        <v>1.1309</v>
       </c>
       <c r="D88" t="n">
-        <v>-31.4102</v>
+        <v>0.237</v>
       </c>
       <c r="E88" t="n">
-        <v>14.2683</v>
+        <v>3.0051</v>
       </c>
       <c r="F88" t="n">
-        <v>-1.0964</v>
+        <v>3.0051</v>
       </c>
       <c r="G88" t="n">
-        <v>-12.1719</v>
+        <v>0.0467</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>0.7768</v>
+        <v>0.6185</v>
       </c>
       <c r="B89" t="n">
-        <v>4.1146</v>
+        <v>0.5065</v>
       </c>
       <c r="C89" t="n">
-        <v>0.1779</v>
+        <v>1.1324</v>
       </c>
       <c r="D89" t="n">
-        <v>-33.0828</v>
+        <v>0.2338</v>
       </c>
       <c r="E89" t="n">
-        <v>14.6376</v>
+        <v>3.0709</v>
       </c>
       <c r="F89" t="n">
-        <v>-1.1305</v>
+        <v>3.0709</v>
       </c>
       <c r="G89" t="n">
-        <v>-12.507</v>
+        <v>0.0433</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>0.7927999999999999</v>
+        <v>0.6315</v>
       </c>
       <c r="B90" t="n">
-        <v>4.2198</v>
+        <v>0.5173</v>
       </c>
       <c r="C90" t="n">
-        <v>0.1772</v>
+        <v>1.1339</v>
       </c>
       <c r="D90" t="n">
-        <v>-34.8207</v>
+        <v>0.2302</v>
       </c>
       <c r="E90" t="n">
-        <v>15.0115</v>
+        <v>3.1376</v>
       </c>
       <c r="F90" t="n">
-        <v>-1.1651</v>
+        <v>3.1376</v>
       </c>
       <c r="G90" t="n">
-        <v>-12.8464</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>0.8089</v>
+        <v>0.6447000000000001</v>
       </c>
       <c r="B91" t="n">
-        <v>4.3263</v>
+        <v>0.5282</v>
       </c>
       <c r="C91" t="n">
-        <v>0.1766</v>
+        <v>1.1353</v>
       </c>
       <c r="D91" t="n">
-        <v>-36.6256</v>
+        <v>0.2262</v>
       </c>
       <c r="E91" t="n">
-        <v>15.3902</v>
+        <v>3.2051</v>
       </c>
       <c r="F91" t="n">
-        <v>-1.2001</v>
+        <v>3.2051</v>
       </c>
       <c r="G91" t="n">
-        <v>-13.19</v>
+        <v>0.0367</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>0.8253</v>
+        <v>0.658</v>
       </c>
       <c r="B92" t="n">
-        <v>4.4342</v>
+        <v>0.5393</v>
       </c>
       <c r="C92" t="n">
-        <v>0.176</v>
+        <v>1.1367</v>
       </c>
       <c r="D92" t="n">
-        <v>-38.4991</v>
+        <v>0.2217</v>
       </c>
       <c r="E92" t="n">
-        <v>15.7735</v>
+        <v>3.2733</v>
       </c>
       <c r="F92" t="n">
-        <v>-1.2355</v>
+        <v>3.2733</v>
       </c>
       <c r="G92" t="n">
-        <v>-13.5379</v>
+        <v>0.0333</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>0.8419</v>
+        <v>0.6715</v>
       </c>
       <c r="B93" t="n">
-        <v>4.5434</v>
+        <v>0.5505</v>
       </c>
       <c r="C93" t="n">
-        <v>0.1754</v>
+        <v>1.138</v>
       </c>
       <c r="D93" t="n">
-        <v>-40.4428</v>
+        <v>0.2169</v>
       </c>
       <c r="E93" t="n">
-        <v>16.1615</v>
+        <v>3.3424</v>
       </c>
       <c r="F93" t="n">
-        <v>-1.2714</v>
+        <v>3.3424</v>
       </c>
       <c r="G93" t="n">
-        <v>-13.89</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>0.8586</v>
+        <v>0.6851</v>
       </c>
       <c r="B94" t="n">
-        <v>4.6539</v>
+        <v>0.5618</v>
       </c>
       <c r="C94" t="n">
-        <v>0.1748</v>
+        <v>1.1393</v>
       </c>
       <c r="D94" t="n">
-        <v>-42.4587</v>
+        <v>0.2116</v>
       </c>
       <c r="E94" t="n">
-        <v>16.5541</v>
+        <v>3.4123</v>
       </c>
       <c r="F94" t="n">
-        <v>-1.3077</v>
+        <v>3.4123</v>
       </c>
       <c r="G94" t="n">
-        <v>-14.2464</v>
+        <v>0.0267</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>0.8756</v>
+        <v>0.6989</v>
       </c>
       <c r="B95" t="n">
-        <v>4.7657</v>
+        <v>0.5733</v>
       </c>
       <c r="C95" t="n">
-        <v>0.1743</v>
+        <v>1.1406</v>
       </c>
       <c r="D95" t="n">
-        <v>-44.5484</v>
+        <v>0.2059</v>
       </c>
       <c r="E95" t="n">
-        <v>16.9515</v>
+        <v>3.4829</v>
       </c>
       <c r="F95" t="n">
-        <v>-1.3444</v>
+        <v>3.4829</v>
       </c>
       <c r="G95" t="n">
-        <v>-14.607</v>
+        <v>0.0233</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>0.8928</v>
+        <v>0.7129</v>
       </c>
       <c r="B96" t="n">
-        <v>4.8789</v>
+        <v>0.5849</v>
       </c>
       <c r="C96" t="n">
-        <v>0.1738</v>
+        <v>1.1419</v>
       </c>
       <c r="D96" t="n">
-        <v>-46.7136</v>
+        <v>0.1997</v>
       </c>
       <c r="E96" t="n">
-        <v>17.3535</v>
+        <v>3.5544</v>
       </c>
       <c r="F96" t="n">
-        <v>-1.3816</v>
+        <v>3.5544</v>
       </c>
       <c r="G96" t="n">
-        <v>-14.9719</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>0.9102</v>
+        <v>0.727</v>
       </c>
       <c r="B97" t="n">
-        <v>4.9933</v>
+        <v>0.5966</v>
       </c>
       <c r="C97" t="n">
-        <v>0.1733</v>
+        <v>1.1431</v>
       </c>
       <c r="D97" t="n">
-        <v>-48.9562</v>
+        <v>0.193</v>
       </c>
       <c r="E97" t="n">
-        <v>17.7603</v>
+        <v>3.6267</v>
       </c>
       <c r="F97" t="n">
-        <v>-1.4192</v>
+        <v>3.6267</v>
       </c>
       <c r="G97" t="n">
-        <v>-15.341</v>
+        <v>0.0167</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>0.9277</v>
+        <v>0.7413</v>
       </c>
       <c r="B98" t="n">
-        <v>5.1091</v>
+        <v>0.6085</v>
       </c>
       <c r="C98" t="n">
-        <v>0.1728</v>
+        <v>1.1443</v>
       </c>
       <c r="D98" t="n">
-        <v>-51.278</v>
+        <v>0.1859</v>
       </c>
       <c r="E98" t="n">
-        <v>18.1717</v>
+        <v>3.6997</v>
       </c>
       <c r="F98" t="n">
-        <v>-1.4572</v>
+        <v>3.6997</v>
       </c>
       <c r="G98" t="n">
-        <v>-15.7144</v>
+        <v>0.0133</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>0.9455</v>
+        <v>0.7557</v>
       </c>
       <c r="B99" t="n">
-        <v>5.2262</v>
+        <v>0.6205000000000001</v>
       </c>
       <c r="C99" t="n">
-        <v>0.1723</v>
+        <v>1.1454</v>
       </c>
       <c r="D99" t="n">
-        <v>-53.6808</v>
+        <v>0.1782</v>
       </c>
       <c r="E99" t="n">
-        <v>18.5877</v>
+        <v>3.7736</v>
       </c>
       <c r="F99" t="n">
-        <v>-1.4957</v>
+        <v>3.7736</v>
       </c>
       <c r="G99" t="n">
-        <v>-16.0921</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>0.9635</v>
+        <v>0.7703</v>
       </c>
       <c r="B100" t="n">
-        <v>5.3446</v>
+        <v>0.6326000000000001</v>
       </c>
       <c r="C100" t="n">
-        <v>0.1718</v>
+        <v>1.1465</v>
       </c>
       <c r="D100" t="n">
-        <v>-56.1665</v>
+        <v>0.17</v>
       </c>
       <c r="E100" t="n">
-        <v>19.0085</v>
+        <v>3.8483</v>
       </c>
       <c r="F100" t="n">
-        <v>-1.5346</v>
+        <v>3.8483</v>
       </c>
       <c r="G100" t="n">
-        <v>-16.4739</v>
+        <v>0.0067</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="n">
-        <v>0.9816</v>
+        <v>0.7851</v>
       </c>
       <c r="B101" t="n">
-        <v>5.4644</v>
+        <v>0.6449</v>
       </c>
       <c r="C101" t="n">
-        <v>0.1714</v>
+        <v>1.1476</v>
       </c>
       <c r="D101" t="n">
-        <v>-58.7369</v>
+        <v>0.1613</v>
       </c>
       <c r="E101" t="n">
-        <v>19.434</v>
+        <v>3.9237</v>
       </c>
       <c r="F101" t="n">
-        <v>-1.5739</v>
+        <v>3.9237</v>
       </c>
       <c r="G101" t="n">
-        <v>-16.8601</v>
+        <v>0.0033</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="n">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="B102" t="n">
-        <v>5.5854</v>
+        <v>0.6573</v>
       </c>
       <c r="C102" t="n">
-        <v>0.171</v>
+        <v>1.1487</v>
       </c>
       <c r="D102" t="n">
-        <v>-61.3939</v>
+        <v>0.152</v>
       </c>
       <c r="E102" t="n">
-        <v>19.8641</v>
+        <v>4</v>
       </c>
       <c r="F102" t="n">
-        <v>-1.6137</v>
+        <v>4</v>
       </c>
       <c r="G102" t="n">
-        <v>-17.2504</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>